<commit_message>
1. Add new page - Design Collection 2. Update Media page 3. Add animation for navbar toogle
</commit_message>
<xml_diff>
--- a/data/media.xlsx
+++ b/data/media.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="710">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2159,6 +2159,17 @@
   </si>
   <si>
     <t>tt0137523</t>
+  </si>
+  <si>
+    <t>/images/poster/Arrow Season 02.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/images/poster/12 Years A Slave.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/images/poster/</t>
   </si>
 </sst>
 </file>
@@ -2523,8 +2534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A336" workbookViewId="0">
-      <selection activeCell="C349" sqref="C349:C354"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E350" sqref="E350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2532,7 +2543,7 @@
     <col min="1" max="1" width="67.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
@@ -2559,6 +2570,9 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
@@ -2570,6 +2584,9 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
+      <c r="D3" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
@@ -2581,6 +2598,9 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
@@ -2592,6 +2612,9 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
@@ -2603,6 +2626,9 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
@@ -2614,6 +2640,9 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
@@ -2625,6 +2654,9 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
+      <c r="D8" s="1" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
@@ -2636,6 +2668,9 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
@@ -2647,6 +2682,9 @@
       <c r="C10" t="s">
         <v>5</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
@@ -2658,6 +2696,9 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
+      <c r="D11" s="1" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -2669,6 +2710,9 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
+      <c r="D12" s="1" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
@@ -2680,6 +2724,9 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
@@ -2691,6 +2738,9 @@
       <c r="C14" t="s">
         <v>5</v>
       </c>
+      <c r="D14" s="1" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
@@ -2702,6 +2752,9 @@
       <c r="C15" t="s">
         <v>5</v>
       </c>
+      <c r="D15" s="1" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
@@ -2713,8 +2766,11 @@
       <c r="C16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D16" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2724,8 +2780,11 @@
       <c r="C17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D17" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -2735,8 +2794,11 @@
       <c r="C18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D18" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -2746,8 +2808,11 @@
       <c r="C19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D19" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -2757,8 +2822,11 @@
       <c r="C20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D20" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -2768,8 +2836,11 @@
       <c r="C21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D21" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -2779,8 +2850,11 @@
       <c r="C22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D22" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2790,8 +2864,11 @@
       <c r="C23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D23" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -2801,8 +2878,11 @@
       <c r="C24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D24" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -2812,8 +2892,11 @@
       <c r="C25" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D25" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -2823,8 +2906,11 @@
       <c r="C26" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D26" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -2834,8 +2920,11 @@
       <c r="C27" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D27" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -2845,8 +2934,11 @@
       <c r="C28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D28" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2856,8 +2948,11 @@
       <c r="C29" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D29" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -2867,8 +2962,11 @@
       <c r="C30" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D30" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -2878,8 +2976,11 @@
       <c r="C31" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D31" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -2889,8 +2990,11 @@
       <c r="C32" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D32" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -2900,8 +3004,11 @@
       <c r="C33" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D33" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -2911,8 +3018,11 @@
       <c r="C34" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D34" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -2922,8 +3032,11 @@
       <c r="C35" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D35" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -2933,8 +3046,11 @@
       <c r="C36" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D36" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>76</v>
       </c>
@@ -2944,8 +3060,11 @@
       <c r="C37" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D37" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -2955,8 +3074,11 @@
       <c r="C38" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D38" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>80</v>
       </c>
@@ -2966,8 +3088,11 @@
       <c r="C39" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D39" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>82</v>
       </c>
@@ -2977,8 +3102,11 @@
       <c r="C40" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D40" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -2988,8 +3116,11 @@
       <c r="C41" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D41" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -2999,8 +3130,11 @@
       <c r="C42" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D42" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -3010,8 +3144,11 @@
       <c r="C43" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D43" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -3021,8 +3158,11 @@
       <c r="C44" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D44" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>92</v>
       </c>
@@ -3032,8 +3172,11 @@
       <c r="C45" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D45" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>94</v>
       </c>
@@ -3043,8 +3186,11 @@
       <c r="C46" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D46" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -3054,8 +3200,11 @@
       <c r="C47" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D47" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -3065,8 +3214,11 @@
       <c r="C48" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D48" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -3076,8 +3228,11 @@
       <c r="C49" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D49" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -3087,8 +3242,11 @@
       <c r="C50" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D50" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -3098,8 +3256,11 @@
       <c r="C51" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D51" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>104</v>
       </c>
@@ -3109,8 +3270,11 @@
       <c r="C52" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D52" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>105</v>
       </c>
@@ -3120,8 +3284,11 @@
       <c r="C53" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D53" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -3131,8 +3298,11 @@
       <c r="C54" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D54" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>107</v>
       </c>
@@ -3142,8 +3312,11 @@
       <c r="C55" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D55" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>108</v>
       </c>
@@ -3153,8 +3326,11 @@
       <c r="C56" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D56" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>109</v>
       </c>
@@ -3164,8 +3340,11 @@
       <c r="C57" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D57" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>110</v>
       </c>
@@ -3175,8 +3354,11 @@
       <c r="C58" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D58" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>111</v>
       </c>
@@ -3186,8 +3368,11 @@
       <c r="C59" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D59" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -3197,8 +3382,11 @@
       <c r="C60" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D60" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>113</v>
       </c>
@@ -3208,8 +3396,11 @@
       <c r="C61" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D61" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>114</v>
       </c>
@@ -3219,8 +3410,11 @@
       <c r="C62" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D62" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>115</v>
       </c>
@@ -3230,8 +3424,11 @@
       <c r="C63" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D63" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>116</v>
       </c>
@@ -3241,8 +3438,11 @@
       <c r="C64" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D64" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>117</v>
       </c>
@@ -3252,8 +3452,11 @@
       <c r="C65" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D65" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>118</v>
       </c>
@@ -3263,8 +3466,11 @@
       <c r="C66" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D66" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>119</v>
       </c>
@@ -3274,8 +3480,11 @@
       <c r="C67" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D67" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>120</v>
       </c>
@@ -3285,8 +3494,11 @@
       <c r="C68" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D68" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>121</v>
       </c>
@@ -3296,8 +3508,11 @@
       <c r="C69" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D69" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
         <v>150</v>
       </c>
@@ -3307,8 +3522,11 @@
       <c r="C70" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D70" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>151</v>
       </c>
@@ -3318,8 +3536,11 @@
       <c r="C71" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D71" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>152</v>
       </c>
@@ -3329,8 +3550,11 @@
       <c r="C72" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D72" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>153</v>
       </c>
@@ -3340,8 +3564,11 @@
       <c r="C73" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D73" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>154</v>
       </c>
@@ -3351,8 +3578,11 @@
       <c r="C74" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D74" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>155</v>
       </c>
@@ -3362,8 +3592,11 @@
       <c r="C75" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D75" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>156</v>
       </c>
@@ -3373,8 +3606,11 @@
       <c r="C76" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D76" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>157</v>
       </c>
@@ -3384,8 +3620,11 @@
       <c r="C77" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D77" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>158</v>
       </c>
@@ -3395,8 +3634,11 @@
       <c r="C78" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D78" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
         <v>159</v>
       </c>
@@ -3406,8 +3648,11 @@
       <c r="C79" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D79" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>160</v>
       </c>
@@ -3417,8 +3662,11 @@
       <c r="C80" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D80" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>161</v>
       </c>
@@ -3428,8 +3676,11 @@
       <c r="C81" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D81" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>162</v>
       </c>
@@ -3439,8 +3690,11 @@
       <c r="C82" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D82" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>163</v>
       </c>
@@ -3450,8 +3704,11 @@
       <c r="C83" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D83" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -3461,8 +3718,11 @@
       <c r="C84" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D84" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>165</v>
       </c>
@@ -3472,8 +3732,11 @@
       <c r="C85" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D85" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>166</v>
       </c>
@@ -3483,8 +3746,11 @@
       <c r="C86" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D86" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>167</v>
       </c>
@@ -3494,8 +3760,11 @@
       <c r="C87" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D87" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
         <v>168</v>
       </c>
@@ -3505,8 +3774,11 @@
       <c r="C88" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D88" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>169</v>
       </c>
@@ -3516,8 +3788,11 @@
       <c r="C89" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D89" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>170</v>
       </c>
@@ -3527,8 +3802,11 @@
       <c r="C90" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D90" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>171</v>
       </c>
@@ -3538,8 +3816,11 @@
       <c r="C91" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D91" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
         <v>172</v>
       </c>
@@ -3549,8 +3830,11 @@
       <c r="C92" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D92" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
         <v>173</v>
       </c>
@@ -3560,8 +3844,11 @@
       <c r="C93" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D93" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>174</v>
       </c>
@@ -3571,8 +3858,11 @@
       <c r="C94" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D94" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
         <v>175</v>
       </c>
@@ -3582,8 +3872,11 @@
       <c r="C95" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D95" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
         <v>176</v>
       </c>
@@ -3593,8 +3886,11 @@
       <c r="C96" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D96" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
         <v>177</v>
       </c>
@@ -3604,8 +3900,11 @@
       <c r="C97" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D97" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
         <v>178</v>
       </c>
@@ -3615,8 +3914,11 @@
       <c r="C98" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D98" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
         <v>179</v>
       </c>
@@ -3626,8 +3928,11 @@
       <c r="C99" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D99" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
         <v>180</v>
       </c>
@@ -3637,8 +3942,11 @@
       <c r="C100" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D100" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
         <v>181</v>
       </c>
@@ -3648,8 +3956,11 @@
       <c r="C101" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D101" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
         <v>182</v>
       </c>
@@ -3659,8 +3970,11 @@
       <c r="C102" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D102" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
         <v>183</v>
       </c>
@@ -3670,8 +3984,11 @@
       <c r="C103" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D103" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
         <v>184</v>
       </c>
@@ -3681,8 +3998,11 @@
       <c r="C104" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D104" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
         <v>185</v>
       </c>
@@ -3692,8 +4012,11 @@
       <c r="C105" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D105" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
         <v>186</v>
       </c>
@@ -3703,8 +4026,11 @@
       <c r="C106" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D106" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
         <v>187</v>
       </c>
@@ -3714,8 +4040,11 @@
       <c r="C107" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D107" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
         <v>188</v>
       </c>
@@ -3725,8 +4054,11 @@
       <c r="C108" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D108" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
         <v>189</v>
       </c>
@@ -3736,8 +4068,11 @@
       <c r="C109" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D109" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
         <v>190</v>
       </c>
@@ -3747,8 +4082,11 @@
       <c r="C110" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D110" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
         <v>191</v>
       </c>
@@ -3758,8 +4096,11 @@
       <c r="C111" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D111" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
         <v>192</v>
       </c>
@@ -3769,8 +4110,11 @@
       <c r="C112" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D112" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
         <v>193</v>
       </c>
@@ -3780,8 +4124,11 @@
       <c r="C113" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D113" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
         <v>194</v>
       </c>
@@ -3791,8 +4138,11 @@
       <c r="C114" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D114" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
         <v>195</v>
       </c>
@@ -3802,8 +4152,11 @@
       <c r="C115" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D115" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
         <v>196</v>
       </c>
@@ -3813,8 +4166,11 @@
       <c r="C116" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D116" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
         <v>197</v>
       </c>
@@ -3824,8 +4180,11 @@
       <c r="C117" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D117" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
         <v>198</v>
       </c>
@@ -3835,8 +4194,11 @@
       <c r="C118" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D118" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
         <v>199</v>
       </c>
@@ -3846,8 +4208,11 @@
       <c r="C119" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D119" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
         <v>200</v>
       </c>
@@ -3857,8 +4222,11 @@
       <c r="C120" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D120" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
         <v>201</v>
       </c>
@@ -3868,8 +4236,11 @@
       <c r="C121" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D121" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
         <v>202</v>
       </c>
@@ -3879,8 +4250,11 @@
       <c r="C122" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D122" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
         <v>203</v>
       </c>
@@ -3890,8 +4264,11 @@
       <c r="C123" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D123" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
         <v>204</v>
       </c>
@@ -3901,8 +4278,11 @@
       <c r="C124" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D124" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
         <v>205</v>
       </c>
@@ -3912,8 +4292,11 @@
       <c r="C125" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D125" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
         <v>206</v>
       </c>
@@ -3923,8 +4306,11 @@
       <c r="C126" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D126" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
         <v>207</v>
       </c>
@@ -3934,8 +4320,11 @@
       <c r="C127" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D127" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
         <v>208</v>
       </c>
@@ -3945,8 +4334,11 @@
       <c r="C128" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D128" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A129" t="s">
         <v>209</v>
       </c>
@@ -3956,8 +4348,11 @@
       <c r="C129" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D129" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A130" t="s">
         <v>210</v>
       </c>
@@ -3967,8 +4362,11 @@
       <c r="C130" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D130" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A131" t="s">
         <v>211</v>
       </c>
@@ -3978,8 +4376,11 @@
       <c r="C131" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D131" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A132" t="s">
         <v>212</v>
       </c>
@@ -3989,8 +4390,11 @@
       <c r="C132" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D132" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
         <v>213</v>
       </c>
@@ -4000,8 +4404,11 @@
       <c r="C133" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D133" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
         <v>214</v>
       </c>
@@ -4011,8 +4418,11 @@
       <c r="C134" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D134" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
         <v>215</v>
       </c>
@@ -4022,8 +4432,11 @@
       <c r="C135" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D135" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A136" t="s">
         <v>216</v>
       </c>
@@ -4033,8 +4446,11 @@
       <c r="C136" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D136" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A137" t="s">
         <v>217</v>
       </c>
@@ -4044,8 +4460,11 @@
       <c r="C137" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D137" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A138" t="s">
         <v>218</v>
       </c>
@@ -4055,8 +4474,11 @@
       <c r="C138" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D138" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A139" t="s">
         <v>213</v>
       </c>
@@ -4066,8 +4488,11 @@
       <c r="C139" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D139" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A140" t="s">
         <v>219</v>
       </c>
@@ -4077,8 +4502,11 @@
       <c r="C140" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D140" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A141" t="s">
         <v>220</v>
       </c>
@@ -4088,8 +4516,11 @@
       <c r="C141" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D141" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A142" t="s">
         <v>221</v>
       </c>
@@ -4099,8 +4530,11 @@
       <c r="C142" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D142" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A143" t="s">
         <v>222</v>
       </c>
@@ -4110,8 +4544,11 @@
       <c r="C143" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D143" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A144" t="s">
         <v>223</v>
       </c>
@@ -4121,8 +4558,11 @@
       <c r="C144" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D144" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A145" t="s">
         <v>224</v>
       </c>
@@ -4132,8 +4572,11 @@
       <c r="C145" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D145" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A146" t="s">
         <v>225</v>
       </c>
@@ -4143,8 +4586,11 @@
       <c r="C146" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D146" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A147" t="s">
         <v>226</v>
       </c>
@@ -4154,8 +4600,11 @@
       <c r="C147" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D147" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A148" t="s">
         <v>227</v>
       </c>
@@ -4165,8 +4614,11 @@
       <c r="C148" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D148" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A149" t="s">
         <v>228</v>
       </c>
@@ -4176,8 +4628,11 @@
       <c r="C149" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D149" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A150" t="s">
         <v>229</v>
       </c>
@@ -4187,8 +4642,11 @@
       <c r="C150" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D150" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A151" t="s">
         <v>230</v>
       </c>
@@ -4198,8 +4656,11 @@
       <c r="C151" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D151" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A152" t="s">
         <v>231</v>
       </c>
@@ -4209,8 +4670,11 @@
       <c r="C152" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D152" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A153" t="s">
         <v>232</v>
       </c>
@@ -4220,8 +4684,11 @@
       <c r="C153" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D153" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A154" t="s">
         <v>233</v>
       </c>
@@ -4231,8 +4698,11 @@
       <c r="C154" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D154" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A155" t="s">
         <v>234</v>
       </c>
@@ -4242,8 +4712,11 @@
       <c r="C155" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D155" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A156" t="s">
         <v>235</v>
       </c>
@@ -4253,8 +4726,11 @@
       <c r="C156" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D156" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A157" t="s">
         <v>236</v>
       </c>
@@ -4264,8 +4740,11 @@
       <c r="C157" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D157" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A158" t="s">
         <v>237</v>
       </c>
@@ -4275,8 +4754,11 @@
       <c r="C158" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D158" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A159" t="s">
         <v>238</v>
       </c>
@@ -4286,8 +4768,11 @@
       <c r="C159" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D159" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A160" t="s">
         <v>239</v>
       </c>
@@ -4297,8 +4782,11 @@
       <c r="C160" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D160" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A161" t="s">
         <v>240</v>
       </c>
@@ -4308,8 +4796,11 @@
       <c r="C161" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D161" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A162" t="s">
         <v>241</v>
       </c>
@@ -4319,8 +4810,11 @@
       <c r="C162" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D162" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A163" t="s">
         <v>242</v>
       </c>
@@ -4330,8 +4824,11 @@
       <c r="C163" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D163" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A164" t="s">
         <v>243</v>
       </c>
@@ -4341,16 +4838,22 @@
       <c r="C164" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D164" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A165" t="s">
         <v>244</v>
       </c>
       <c r="C165" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D165" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A166" t="s">
         <v>245</v>
       </c>
@@ -4360,8 +4863,11 @@
       <c r="C166" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D166" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A167" t="s">
         <v>246</v>
       </c>
@@ -4371,8 +4877,11 @@
       <c r="C167" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D167" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A168" t="s">
         <v>247</v>
       </c>
@@ -4382,8 +4891,11 @@
       <c r="C168" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D168" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A169" t="s">
         <v>248</v>
       </c>
@@ -4393,8 +4905,11 @@
       <c r="C169" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D169" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A170" t="s">
         <v>249</v>
       </c>
@@ -4404,8 +4919,11 @@
       <c r="C170" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D170" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A171" t="s">
         <v>250</v>
       </c>
@@ -4415,8 +4933,11 @@
       <c r="C171" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D171" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A172" t="s">
         <v>251</v>
       </c>
@@ -4426,8 +4947,11 @@
       <c r="C172" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D172" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A173" t="s">
         <v>252</v>
       </c>
@@ -4437,8 +4961,11 @@
       <c r="C173" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D173" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A174" t="s">
         <v>253</v>
       </c>
@@ -4448,8 +4975,11 @@
       <c r="C174" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D174" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A175" t="s">
         <v>254</v>
       </c>
@@ -4459,8 +4989,11 @@
       <c r="C175" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D175" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A176" t="s">
         <v>255</v>
       </c>
@@ -4470,8 +5003,11 @@
       <c r="C176" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D176" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A177" t="s">
         <v>256</v>
       </c>
@@ -4481,8 +5017,11 @@
       <c r="C177" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D177" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A178" t="s">
         <v>257</v>
       </c>
@@ -4492,8 +5031,11 @@
       <c r="C178" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D178" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A179" t="s">
         <v>258</v>
       </c>
@@ -4503,8 +5045,11 @@
       <c r="C179" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D179" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A180" t="s">
         <v>259</v>
       </c>
@@ -4514,8 +5059,11 @@
       <c r="C180" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D180" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A181" t="s">
         <v>260</v>
       </c>
@@ -4525,8 +5073,11 @@
       <c r="C181" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D181" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A182" t="s">
         <v>261</v>
       </c>
@@ -4536,8 +5087,11 @@
       <c r="C182" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D182" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A183" t="s">
         <v>262</v>
       </c>
@@ -4547,8 +5101,11 @@
       <c r="C183" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D183" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A184" t="s">
         <v>263</v>
       </c>
@@ -4558,8 +5115,11 @@
       <c r="C184" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D184" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A185" t="s">
         <v>264</v>
       </c>
@@ -4569,8 +5129,11 @@
       <c r="C185" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D185" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A186" t="s">
         <v>265</v>
       </c>
@@ -4580,8 +5143,11 @@
       <c r="C186" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D186" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A187" t="s">
         <v>266</v>
       </c>
@@ -4591,8 +5157,11 @@
       <c r="C187" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D187" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A188" t="s">
         <v>267</v>
       </c>
@@ -4602,8 +5171,11 @@
       <c r="C188" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D188" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A189" t="s">
         <v>268</v>
       </c>
@@ -4613,8 +5185,11 @@
       <c r="C189" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D189" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A190" t="s">
         <v>269</v>
       </c>
@@ -4624,8 +5199,11 @@
       <c r="C190" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D190" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A191" t="s">
         <v>270</v>
       </c>
@@ -4635,8 +5213,11 @@
       <c r="C191" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D191" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A192" t="s">
         <v>271</v>
       </c>
@@ -4646,8 +5227,11 @@
       <c r="C192" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D192" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A193" t="s">
         <v>272</v>
       </c>
@@ -4657,8 +5241,11 @@
       <c r="C193" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D193" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A194" t="s">
         <v>273</v>
       </c>
@@ -4668,8 +5255,11 @@
       <c r="C194" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D194" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A195" t="s">
         <v>274</v>
       </c>
@@ -4679,8 +5269,11 @@
       <c r="C195" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D195" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A196" t="s">
         <v>275</v>
       </c>
@@ -4690,8 +5283,11 @@
       <c r="C196" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D196" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A197" t="s">
         <v>276</v>
       </c>
@@ -4701,8 +5297,11 @@
       <c r="C197" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D197" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A198" t="s">
         <v>277</v>
       </c>
@@ -4712,8 +5311,11 @@
       <c r="C198" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D198" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A199" t="s">
         <v>278</v>
       </c>
@@ -4723,8 +5325,11 @@
       <c r="C199" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D199" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A200" t="s">
         <v>279</v>
       </c>
@@ -4734,8 +5339,11 @@
       <c r="C200" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D200" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A201" t="s">
         <v>280</v>
       </c>
@@ -4745,8 +5353,11 @@
       <c r="C201" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D201" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A202" t="s">
         <v>281</v>
       </c>
@@ -4756,8 +5367,11 @@
       <c r="C202" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D202" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A203" t="s">
         <v>282</v>
       </c>
@@ -4767,8 +5381,11 @@
       <c r="C203" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D203" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A204" t="s">
         <v>283</v>
       </c>
@@ -4778,8 +5395,11 @@
       <c r="C204" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D204" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A205" t="s">
         <v>284</v>
       </c>
@@ -4789,8 +5409,11 @@
       <c r="C205" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D205" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A206" t="s">
         <v>285</v>
       </c>
@@ -4800,8 +5423,11 @@
       <c r="C206" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D206" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A207" t="s">
         <v>286</v>
       </c>
@@ -4811,8 +5437,11 @@
       <c r="C207" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D207" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A208" t="s">
         <v>287</v>
       </c>
@@ -4822,8 +5451,11 @@
       <c r="C208" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D208" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A209" t="s">
         <v>288</v>
       </c>
@@ -4833,8 +5465,11 @@
       <c r="C209" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D209" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A210" t="s">
         <v>289</v>
       </c>
@@ -4844,8 +5479,11 @@
       <c r="C210" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D210" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A211" t="s">
         <v>290</v>
       </c>
@@ -4855,8 +5493,11 @@
       <c r="C211" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D211" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A212" t="s">
         <v>291</v>
       </c>
@@ -4866,8 +5507,11 @@
       <c r="C212" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D212" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A213" t="s">
         <v>292</v>
       </c>
@@ -4877,8 +5521,11 @@
       <c r="C213" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D213" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A214" t="s">
         <v>293</v>
       </c>
@@ -4888,8 +5535,11 @@
       <c r="C214" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D214" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A215" t="s">
         <v>294</v>
       </c>
@@ -4899,8 +5549,11 @@
       <c r="C215" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D215" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A216" t="s">
         <v>295</v>
       </c>
@@ -4910,8 +5563,11 @@
       <c r="C216" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D216" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A217" t="s">
         <v>296</v>
       </c>
@@ -4921,8 +5577,11 @@
       <c r="C217" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D217" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A218" t="s">
         <v>297</v>
       </c>
@@ -4932,8 +5591,11 @@
       <c r="C218" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D218" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A219" t="s">
         <v>298</v>
       </c>
@@ -4943,8 +5605,11 @@
       <c r="C219" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D219" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A220" t="s">
         <v>299</v>
       </c>
@@ -4954,8 +5619,11 @@
       <c r="C220" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D220" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A221" t="s">
         <v>300</v>
       </c>
@@ -4965,8 +5633,11 @@
       <c r="C221" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D221" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A222" t="s">
         <v>301</v>
       </c>
@@ -4976,16 +5647,22 @@
       <c r="C222" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D222" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A223" t="s">
         <v>302</v>
       </c>
       <c r="C223" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D223" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A224" t="s">
         <v>303</v>
       </c>
@@ -4995,8 +5672,11 @@
       <c r="C224" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D224" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A225" t="s">
         <v>304</v>
       </c>
@@ -5006,8 +5686,11 @@
       <c r="C225" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D225" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A226" t="s">
         <v>305</v>
       </c>
@@ -5017,8 +5700,11 @@
       <c r="C226" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D226" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A227" t="s">
         <v>306</v>
       </c>
@@ -5028,8 +5714,11 @@
       <c r="C227" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D227" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A228" t="s">
         <v>307</v>
       </c>
@@ -5039,8 +5728,11 @@
       <c r="C228" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D228" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A229" t="s">
         <v>308</v>
       </c>
@@ -5050,8 +5742,11 @@
       <c r="C229" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D229" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A230" t="s">
         <v>309</v>
       </c>
@@ -5061,8 +5756,11 @@
       <c r="C230" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D230" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A231" t="s">
         <v>310</v>
       </c>
@@ -5072,8 +5770,11 @@
       <c r="C231" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D231" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A232" t="s">
         <v>311</v>
       </c>
@@ -5083,8 +5784,11 @@
       <c r="C232" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D232" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A233" t="s">
         <v>312</v>
       </c>
@@ -5094,8 +5798,11 @@
       <c r="C233" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D233" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A234" t="s">
         <v>313</v>
       </c>
@@ -5105,8 +5812,11 @@
       <c r="C234" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D234" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A235" t="s">
         <v>314</v>
       </c>
@@ -5116,8 +5826,11 @@
       <c r="C235" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D235" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A236" t="s">
         <v>315</v>
       </c>
@@ -5127,8 +5840,11 @@
       <c r="C236" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D236" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A237" t="s">
         <v>316</v>
       </c>
@@ -5138,8 +5854,11 @@
       <c r="C237" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D237" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A238" t="s">
         <v>317</v>
       </c>
@@ -5149,8 +5868,11 @@
       <c r="C238" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D238" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A239" t="s">
         <v>318</v>
       </c>
@@ -5160,8 +5882,11 @@
       <c r="C239" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D239" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A240" t="s">
         <v>319</v>
       </c>
@@ -5171,8 +5896,11 @@
       <c r="C240" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D240" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A241" t="s">
         <v>320</v>
       </c>
@@ -5182,8 +5910,11 @@
       <c r="C241" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D241" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A242" t="s">
         <v>321</v>
       </c>
@@ -5193,8 +5924,11 @@
       <c r="C242" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D242" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A243" t="s">
         <v>322</v>
       </c>
@@ -5204,8 +5938,11 @@
       <c r="C243" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D243" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A244" t="s">
         <v>323</v>
       </c>
@@ -5215,8 +5952,11 @@
       <c r="C244" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D244" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A245" t="s">
         <v>324</v>
       </c>
@@ -5226,8 +5966,11 @@
       <c r="C245" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D245" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A246" t="s">
         <v>325</v>
       </c>
@@ -5237,8 +5980,11 @@
       <c r="C246" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D246" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A247" t="s">
         <v>326</v>
       </c>
@@ -5248,8 +5994,11 @@
       <c r="C247" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D247" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A248" t="s">
         <v>327</v>
       </c>
@@ -5259,8 +6008,11 @@
       <c r="C248" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D248" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A249" t="s">
         <v>328</v>
       </c>
@@ -5270,8 +6022,11 @@
       <c r="C249" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D249" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A250" t="s">
         <v>329</v>
       </c>
@@ -5281,8 +6036,11 @@
       <c r="C250" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D250" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A251" t="s">
         <v>330</v>
       </c>
@@ -5292,8 +6050,11 @@
       <c r="C251" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D251" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A252" t="s">
         <v>331</v>
       </c>
@@ -5303,8 +6064,11 @@
       <c r="C252" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D252" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A253" t="s">
         <v>332</v>
       </c>
@@ -5314,8 +6078,11 @@
       <c r="C253" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D253" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A254" t="s">
         <v>333</v>
       </c>
@@ -5325,8 +6092,11 @@
       <c r="C254" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D254" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A255" t="s">
         <v>334</v>
       </c>
@@ -5336,8 +6106,11 @@
       <c r="C255" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D255" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A256" t="s">
         <v>335</v>
       </c>
@@ -5347,8 +6120,11 @@
       <c r="C256" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D256" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A257" t="s">
         <v>336</v>
       </c>
@@ -5358,8 +6134,11 @@
       <c r="C257" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D257" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A258" t="s">
         <v>337</v>
       </c>
@@ -5369,8 +6148,11 @@
       <c r="C258" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D258" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A259" t="s">
         <v>338</v>
       </c>
@@ -5380,8 +6162,11 @@
       <c r="C259" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D259" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A260" t="s">
         <v>339</v>
       </c>
@@ -5391,8 +6176,11 @@
       <c r="C260" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D260" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A261" t="s">
         <v>340</v>
       </c>
@@ -5402,8 +6190,11 @@
       <c r="C261" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D261" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A262" t="s">
         <v>341</v>
       </c>
@@ -5413,8 +6204,11 @@
       <c r="C262" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D262" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A263" t="s">
         <v>342</v>
       </c>
@@ -5424,8 +6218,11 @@
       <c r="C263" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D263" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A264" t="s">
         <v>343</v>
       </c>
@@ -5435,8 +6232,11 @@
       <c r="C264" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D264" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A265" t="s">
         <v>344</v>
       </c>
@@ -5446,8 +6246,11 @@
       <c r="C265" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D265" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A266" t="s">
         <v>345</v>
       </c>
@@ -5457,8 +6260,11 @@
       <c r="C266" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D266" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A267" t="s">
         <v>346</v>
       </c>
@@ -5468,8 +6274,11 @@
       <c r="C267" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D267" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A268" t="s">
         <v>347</v>
       </c>
@@ -5479,8 +6288,11 @@
       <c r="C268" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D268" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A269" t="s">
         <v>348</v>
       </c>
@@ -5490,8 +6302,11 @@
       <c r="C269" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D269" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A270" t="s">
         <v>349</v>
       </c>
@@ -5501,8 +6316,11 @@
       <c r="C270" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D270" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A271" t="s">
         <v>350</v>
       </c>
@@ -5512,8 +6330,11 @@
       <c r="C271" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D271" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A272" t="s">
         <v>351</v>
       </c>
@@ -5523,8 +6344,11 @@
       <c r="C272" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D272" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A273" t="s">
         <v>352</v>
       </c>
@@ -5534,8 +6358,11 @@
       <c r="C273" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D273" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A274" t="s">
         <v>353</v>
       </c>
@@ -5545,8 +6372,11 @@
       <c r="C274" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D274" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A275" t="s">
         <v>354</v>
       </c>
@@ -5556,8 +6386,11 @@
       <c r="C275" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D275" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A276" t="s">
         <v>355</v>
       </c>
@@ -5567,8 +6400,11 @@
       <c r="C276" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D276" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A277" t="s">
         <v>356</v>
       </c>
@@ -5578,8 +6414,11 @@
       <c r="C277" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D277" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A278" t="s">
         <v>357</v>
       </c>
@@ -5589,8 +6428,11 @@
       <c r="C278" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D278" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A279" t="s">
         <v>358</v>
       </c>
@@ -5600,8 +6442,11 @@
       <c r="C279" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D279" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A280" t="s">
         <v>359</v>
       </c>
@@ -5611,8 +6456,11 @@
       <c r="C280" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D280" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A281" t="s">
         <v>360</v>
       </c>
@@ -5622,8 +6470,11 @@
       <c r="C281" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D281" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A282" t="s">
         <v>361</v>
       </c>
@@ -5633,8 +6484,11 @@
       <c r="C282" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D282" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A283" t="s">
         <v>362</v>
       </c>
@@ -5644,8 +6498,11 @@
       <c r="C283" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D283" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A284" t="s">
         <v>363</v>
       </c>
@@ -5655,8 +6512,11 @@
       <c r="C284" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D284" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A285" t="s">
         <v>364</v>
       </c>
@@ -5666,8 +6526,11 @@
       <c r="C285" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D285" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A286" t="s">
         <v>143</v>
       </c>
@@ -5677,8 +6540,11 @@
       <c r="C286" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D286" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A287" t="s">
         <v>365</v>
       </c>
@@ -5688,8 +6554,11 @@
       <c r="C287" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D287" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A288" t="s">
         <v>366</v>
       </c>
@@ -5699,8 +6568,11 @@
       <c r="C288" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D288" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A289" t="s">
         <v>367</v>
       </c>
@@ -5710,8 +6582,11 @@
       <c r="C289" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D289" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A290" t="s">
         <v>368</v>
       </c>
@@ -5721,8 +6596,11 @@
       <c r="C290" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D290" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A291" t="s">
         <v>369</v>
       </c>
@@ -5732,8 +6610,11 @@
       <c r="C291" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D291" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A292" t="s">
         <v>370</v>
       </c>
@@ -5743,8 +6624,11 @@
       <c r="C292" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D292" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A293" t="s">
         <v>371</v>
       </c>
@@ -5754,8 +6638,11 @@
       <c r="C293" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D293" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A294" t="s">
         <v>372</v>
       </c>
@@ -5765,8 +6652,11 @@
       <c r="C294" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D294" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A295" t="s">
         <v>373</v>
       </c>
@@ -5776,8 +6666,11 @@
       <c r="C295" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D295" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A296" t="s">
         <v>374</v>
       </c>
@@ -5787,8 +6680,11 @@
       <c r="C296" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D296" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A297" t="s">
         <v>375</v>
       </c>
@@ -5798,8 +6694,11 @@
       <c r="C297" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D297" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A298" t="s">
         <v>376</v>
       </c>
@@ -5809,8 +6708,11 @@
       <c r="C298" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D298" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A299" t="s">
         <v>145</v>
       </c>
@@ -5820,8 +6722,11 @@
       <c r="C299" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D299" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A300" t="s">
         <v>147</v>
       </c>
@@ -5831,16 +6736,22 @@
       <c r="C300" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D300" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A301" t="s">
         <v>149</v>
       </c>
       <c r="C301" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D301" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A302" t="s">
         <v>600</v>
       </c>
@@ -5850,8 +6761,11 @@
       <c r="C302" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D302" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A303" t="s">
         <v>602</v>
       </c>
@@ -5861,8 +6775,11 @@
       <c r="C303" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D303" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A304" t="s">
         <v>604</v>
       </c>
@@ -5872,8 +6789,11 @@
       <c r="C304" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D304" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A305" t="s">
         <v>606</v>
       </c>
@@ -5883,8 +6803,11 @@
       <c r="C305" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D305" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A306" t="s">
         <v>608</v>
       </c>
@@ -5894,8 +6817,11 @@
       <c r="C306" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D306" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A307" t="s">
         <v>611</v>
       </c>
@@ -5905,8 +6831,11 @@
       <c r="C307" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D307" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A308" t="s">
         <v>612</v>
       </c>
@@ -5916,8 +6845,11 @@
       <c r="C308" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D308" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A309" t="s">
         <v>614</v>
       </c>
@@ -5927,8 +6859,11 @@
       <c r="C309" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D309" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A310" t="s">
         <v>616</v>
       </c>
@@ -5938,8 +6873,11 @@
       <c r="C310" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D310" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A311" t="s">
         <v>621</v>
       </c>
@@ -5949,8 +6887,11 @@
       <c r="C311" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D311" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A312" t="s">
         <v>619</v>
       </c>
@@ -5960,8 +6901,11 @@
       <c r="C312" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D312" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A313" t="s">
         <v>622</v>
       </c>
@@ -5971,8 +6915,11 @@
       <c r="C313" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D313" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A314" t="s">
         <v>624</v>
       </c>
@@ -5982,8 +6929,11 @@
       <c r="C314" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D314" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A315" t="s">
         <v>626</v>
       </c>
@@ -5993,8 +6943,11 @@
       <c r="C315" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D315" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A316" t="s">
         <v>628</v>
       </c>
@@ -6004,8 +6957,11 @@
       <c r="C316" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D316" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A317" t="s">
         <v>630</v>
       </c>
@@ -6015,8 +6971,11 @@
       <c r="C317" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D317" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A318" t="s">
         <v>632</v>
       </c>
@@ -6026,8 +6985,11 @@
       <c r="C318" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D318" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A319" t="s">
         <v>634</v>
       </c>
@@ -6037,8 +6999,11 @@
       <c r="C319" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D319" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A320" t="s">
         <v>636</v>
       </c>
@@ -6048,8 +7013,11 @@
       <c r="C320" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D320" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A321" t="s">
         <v>638</v>
       </c>
@@ -6059,8 +7027,11 @@
       <c r="C321" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D321" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A322" t="s">
         <v>640</v>
       </c>
@@ -6070,8 +7041,11 @@
       <c r="C322" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D322" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A323" t="s">
         <v>642</v>
       </c>
@@ -6081,8 +7055,11 @@
       <c r="C323" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D323" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A324" t="s">
         <v>644</v>
       </c>
@@ -6092,8 +7069,11 @@
       <c r="C324" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D324" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A325" t="s">
         <v>646</v>
       </c>
@@ -6103,8 +7083,11 @@
       <c r="C325" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D325" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A326" t="s">
         <v>648</v>
       </c>
@@ -6114,8 +7097,11 @@
       <c r="C326" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D326" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A327" t="s">
         <v>651</v>
       </c>
@@ -6125,8 +7111,11 @@
       <c r="C327" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D327" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A328" t="s">
         <v>653</v>
       </c>
@@ -6136,8 +7125,11 @@
       <c r="C328" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D328" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A329" t="s">
         <v>655</v>
       </c>
@@ -6147,8 +7139,11 @@
       <c r="C329" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D329" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A330" t="s">
         <v>656</v>
       </c>
@@ -6158,8 +7153,11 @@
       <c r="C330" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D330" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A331" t="s">
         <v>657</v>
       </c>
@@ -6169,8 +7167,11 @@
       <c r="C331" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D331" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A332" t="s">
         <v>658</v>
       </c>
@@ -6180,8 +7181,11 @@
       <c r="C332" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D332" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A333" t="s">
         <v>659</v>
       </c>
@@ -6191,8 +7195,11 @@
       <c r="C333" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D333" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A334" t="s">
         <v>665</v>
       </c>
@@ -6202,8 +7209,11 @@
       <c r="C334" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D334" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A335" s="1" t="s">
         <v>667</v>
       </c>
@@ -6213,8 +7223,11 @@
       <c r="C335" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D335" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A336" t="s">
         <v>670</v>
       </c>
@@ -6224,8 +7237,11 @@
       <c r="C336" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D336" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A337" t="s">
         <v>671</v>
       </c>
@@ -6235,8 +7251,11 @@
       <c r="C337" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D337" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A338" t="s">
         <v>673</v>
       </c>
@@ -6246,8 +7265,11 @@
       <c r="C338" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D338" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A339" t="s">
         <v>675</v>
       </c>
@@ -6257,8 +7279,11 @@
       <c r="C339" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D339" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A340" t="s">
         <v>677</v>
       </c>
@@ -6268,8 +7293,11 @@
       <c r="C340" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D340" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A341" t="s">
         <v>679</v>
       </c>
@@ -6279,8 +7307,11 @@
       <c r="C341" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D341" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A342" t="s">
         <v>681</v>
       </c>
@@ -6290,8 +7321,11 @@
       <c r="C342" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D342" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A343" t="s">
         <v>683</v>
       </c>
@@ -6301,8 +7335,11 @@
       <c r="C343" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D343" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A344" t="s">
         <v>685</v>
       </c>
@@ -6312,8 +7349,11 @@
       <c r="C344" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D344" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A345" s="1" t="s">
         <v>687</v>
       </c>
@@ -6323,8 +7363,11 @@
       <c r="C345" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D345" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A346" s="1" t="s">
         <v>690</v>
       </c>
@@ -6334,8 +7377,11 @@
       <c r="C346" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D346" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A347" t="s">
         <v>691</v>
       </c>
@@ -6345,8 +7391,11 @@
       <c r="C347" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D347" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A348" t="s">
         <v>693</v>
       </c>
@@ -6356,8 +7405,11 @@
       <c r="C348" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D348" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A349" t="s">
         <v>695</v>
       </c>
@@ -6367,8 +7419,11 @@
       <c r="C349" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D349" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A350" t="s">
         <v>697</v>
       </c>
@@ -6378,8 +7433,11 @@
       <c r="C350" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D350" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A351" t="s">
         <v>699</v>
       </c>
@@ -6389,8 +7447,11 @@
       <c r="C351" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D351" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A352" t="s">
         <v>701</v>
       </c>
@@ -6400,8 +7461,11 @@
       <c r="C352" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D352" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A353" t="s">
         <v>703</v>
       </c>
@@ -6411,8 +7475,11 @@
       <c r="C353" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D353" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A354" t="s">
         <v>705</v>
       </c>
@@ -6421,6 +7488,9 @@
       </c>
       <c r="C354" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="D354" s="1" t="s">
+        <v>709</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Update media data 2. Restore bible black cover
</commit_message>
<xml_diff>
--- a/data/media.xlsx
+++ b/data/media.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="812">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2473,6 +2473,18 @@
   <si>
     <t>TV</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miracles from Heaven</t>
+  </si>
+  <si>
+    <t>tt4257926</t>
+  </si>
+  <si>
+    <t>The Huntsman Winters War</t>
+  </si>
+  <si>
+    <t>tt2381991</t>
   </si>
 </sst>
 </file>
@@ -2841,10 +2853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D402"/>
+  <dimension ref="A1:D404"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
-      <selection activeCell="C401" sqref="C401:C402"/>
+      <selection activeCell="C404" sqref="C404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7624,6 +7636,28 @@
         <v>807</v>
       </c>
     </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A403" t="s">
+        <v>808</v>
+      </c>
+      <c r="B403" t="s">
+        <v>809</v>
+      </c>
+      <c r="C403" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A404" t="s">
+        <v>810</v>
+      </c>
+      <c r="B404" t="s">
+        <v>811</v>
+      </c>
+      <c r="C404" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add new blog install node-sass on windows.
</commit_message>
<xml_diff>
--- a/data/media.xlsx
+++ b/data/media.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="820">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2497,6 +2497,18 @@
   </si>
   <si>
     <t>tt0435651</t>
+  </si>
+  <si>
+    <t>Batman v Superman: Dawn of Justice</t>
+  </si>
+  <si>
+    <t>tt2975590</t>
+  </si>
+  <si>
+    <t>The Angry Birds Movie</t>
+  </si>
+  <si>
+    <t>tt1985949</t>
   </si>
 </sst>
 </file>
@@ -2865,10 +2877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D406"/>
+  <dimension ref="A1:D408"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
-      <selection activeCell="C404" sqref="C404:C406"/>
+      <selection activeCell="C406" sqref="C406:C408"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7692,6 +7704,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A407" t="s">
+        <v>816</v>
+      </c>
+      <c r="B407" t="s">
+        <v>817</v>
+      </c>
+      <c r="C407" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A408" t="s">
+        <v>818</v>
+      </c>
+      <c r="B408" t="s">
+        <v>819</v>
+      </c>
+      <c r="C408" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update loading animation Add media data
</commit_message>
<xml_diff>
--- a/data/media.xlsx
+++ b/data/media.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="824">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2509,6 +2509,18 @@
   </si>
   <si>
     <t>tt1985949</t>
+  </si>
+  <si>
+    <t>Demolition</t>
+  </si>
+  <si>
+    <t>The Trip</t>
+  </si>
+  <si>
+    <t>tt1172049</t>
+  </si>
+  <si>
+    <t>tt0250067</t>
   </si>
 </sst>
 </file>
@@ -2551,13 +2563,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -2877,10 +2890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D408"/>
+  <dimension ref="A1:D410"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
-      <selection activeCell="C406" sqref="C406:C408"/>
+      <selection activeCell="C408" sqref="C408:C410"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7726,6 +7739,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="409" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A409" t="s">
+        <v>820</v>
+      </c>
+      <c r="B409" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="C409" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A410" t="s">
+        <v>821</v>
+      </c>
+      <c r="B410" t="s">
+        <v>823</v>
+      </c>
+      <c r="C410" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update resume Add media data
</commit_message>
<xml_diff>
--- a/data/media.xlsx
+++ b/data/media.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="830">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2521,6 +2521,24 @@
   </si>
   <si>
     <t>tt0250067</t>
+  </si>
+  <si>
+    <t>I Robot</t>
+  </si>
+  <si>
+    <t>tt0343818</t>
+  </si>
+  <si>
+    <t>Warcraft</t>
+  </si>
+  <si>
+    <t>tt0803096</t>
+  </si>
+  <si>
+    <t>The Jungle Book</t>
+  </si>
+  <si>
+    <t>tt3040964</t>
   </si>
 </sst>
 </file>
@@ -2890,10 +2908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D410"/>
+  <dimension ref="A1:D413"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
-      <selection activeCell="C408" sqref="C408:C410"/>
+      <selection activeCell="C412" sqref="C412:C413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7761,6 +7779,39 @@
         <v>5</v>
       </c>
     </row>
+    <row r="411" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A411" t="s">
+        <v>824</v>
+      </c>
+      <c r="B411" t="s">
+        <v>825</v>
+      </c>
+      <c r="C411" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A412" t="s">
+        <v>826</v>
+      </c>
+      <c r="B412" t="s">
+        <v>827</v>
+      </c>
+      <c r="C412" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A413" t="s">
+        <v>828</v>
+      </c>
+      <c r="B413" t="s">
+        <v>829</v>
+      </c>
+      <c r="C413" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update about me page.
</commit_message>
<xml_diff>
--- a/data/media.xlsx
+++ b/data/media.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="834">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2539,6 +2539,19 @@
   </si>
   <si>
     <t>tt3040964</t>
+  </si>
+  <si>
+    <t>Neighbors 2 Sorority Rising</t>
+  </si>
+  <si>
+    <t>tt4438848</t>
+  </si>
+  <si>
+    <t>X-Men Apocalypse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tt3385516</t>
   </si>
 </sst>
 </file>
@@ -2908,10 +2921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D413"/>
+  <dimension ref="A1:D415"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
-      <selection activeCell="C412" sqref="C412:C413"/>
+      <selection activeCell="C414" sqref="C414:C415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7812,6 +7825,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="414" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A414" t="s">
+        <v>830</v>
+      </c>
+      <c r="B414" t="s">
+        <v>831</v>
+      </c>
+      <c r="C414" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A415" t="s">
+        <v>832</v>
+      </c>
+      <c r="B415" t="s">
+        <v>833</v>
+      </c>
+      <c r="C415" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. Fix style issues. 2. Add media data.
</commit_message>
<xml_diff>
--- a/data/media.xlsx
+++ b/data/media.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7308"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="1073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="1077">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2095,7 +2095,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3287,22 +3287,34 @@
   <si>
     <t>tt4425200</t>
   </si>
+  <si>
+    <t>The Green Mile</t>
+  </si>
+  <si>
+    <t>tt0120689</t>
+  </si>
+  <si>
+    <t>Life </t>
+  </si>
+  <si>
+    <t>tt5442430</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3310,7 +3322,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3344,7 +3356,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -3375,7 +3387,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3450,23 +3462,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3502,23 +3497,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3695,13 +3673,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D534"/>
+  <dimension ref="A1:D536"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A514" workbookViewId="0">
-      <selection activeCell="C532" sqref="C532:C534"/>
+      <selection activeCell="C535" sqref="C535:C536"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="67.15625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.578125" style="1" bestFit="1" customWidth="1"/>
@@ -3710,7 +3688,7 @@
     <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3724,7 +3702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>780</v>
       </c>
@@ -3735,7 +3713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -3746,7 +3724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3757,7 +3735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3768,7 +3746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>694</v>
       </c>
@@ -3779,7 +3757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -3790,7 +3768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -3801,7 +3779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>631</v>
       </c>
@@ -3812,7 +3790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>925</v>
       </c>
@@ -3823,7 +3801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -3834,7 +3812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -3845,7 +3823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -3856,7 +3834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -3867,7 +3845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>941</v>
       </c>
@@ -3878,7 +3856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -3889,7 +3867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>947</v>
       </c>
@@ -3900,7 +3878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -3911,7 +3889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -3922,7 +3900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
         <v>768</v>
       </c>
@@ -3933,7 +3911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>863</v>
       </c>
@@ -3944,7 +3922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -3955,7 +3933,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -3966,7 +3944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
         <v>35</v>
       </c>
@@ -3977,7 +3955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
         <v>652</v>
       </c>
@@ -3988,7 +3966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
         <v>999</v>
       </c>
@@ -3999,7 +3977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
         <v>760</v>
       </c>
@@ -4010,7 +3988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
@@ -4021,7 +3999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
         <v>668</v>
       </c>
@@ -4032,7 +4010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
         <v>957</v>
       </c>
@@ -4043,7 +4021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
@@ -4054,7 +4032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
         <v>943</v>
       </c>
@@ -4065,7 +4043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -4076,7 +4054,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
         <v>619</v>
       </c>
@@ -4087,7 +4065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
         <v>799</v>
       </c>
@@ -4098,7 +4076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
         <v>997</v>
       </c>
@@ -4109,7 +4087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
         <v>1003</v>
       </c>
@@ -4120,7 +4098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -4131,7 +4109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
         <v>664</v>
       </c>
@@ -4142,7 +4120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -4153,7 +4131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
@@ -4164,7 +4142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
         <v>48</v>
       </c>
@@ -4175,7 +4153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
         <v>939</v>
       </c>
@@ -4186,7 +4164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
@@ -4197,7 +4175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
         <v>52</v>
       </c>
@@ -4208,7 +4186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
@@ -4219,7 +4197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
         <v>758</v>
       </c>
@@ -4230,7 +4208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
@@ -4241,7 +4219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
         <v>959</v>
       </c>
@@ -4252,7 +4230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
@@ -4263,7 +4241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
         <v>816</v>
       </c>
@@ -4274,7 +4252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
         <v>861</v>
       </c>
@@ -4285,7 +4263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
         <v>60</v>
       </c>
@@ -4296,7 +4274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
         <v>62</v>
       </c>
@@ -4307,7 +4285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
         <v>64</v>
       </c>
@@ -4318,7 +4296,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
         <v>66</v>
       </c>
@@ -4329,7 +4307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
         <v>68</v>
       </c>
@@ -4340,7 +4318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
         <v>762</v>
       </c>
@@ -4351,7 +4329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
         <v>627</v>
       </c>
@@ -4362,7 +4340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
         <v>70</v>
       </c>
@@ -4373,7 +4351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
         <v>72</v>
       </c>
@@ -4384,7 +4362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
         <v>633</v>
       </c>
@@ -4395,7 +4373,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:3">
       <c r="A63" s="1" t="s">
         <v>74</v>
       </c>
@@ -4406,7 +4384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
         <v>76</v>
       </c>
@@ -4417,7 +4395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
         <v>648</v>
       </c>
@@ -4428,7 +4406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
         <v>78</v>
       </c>
@@ -4439,7 +4417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
         <v>80</v>
       </c>
@@ -4450,7 +4428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
         <v>82</v>
       </c>
@@ -4461,7 +4439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
         <v>84</v>
       </c>
@@ -4472,7 +4450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:3">
       <c r="A70" s="1" t="s">
         <v>848</v>
       </c>
@@ -4483,7 +4461,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:3">
       <c r="A71" s="1" t="s">
         <v>887</v>
       </c>
@@ -4494,7 +4472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
         <v>86</v>
       </c>
@@ -4505,7 +4483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
         <v>88</v>
       </c>
@@ -4516,7 +4494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
         <v>90</v>
       </c>
@@ -4527,7 +4505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:3">
       <c r="A75" s="1" t="s">
         <v>654</v>
       </c>
@@ -4538,7 +4516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:3">
       <c r="A76" s="1" t="s">
         <v>92</v>
       </c>
@@ -4549,7 +4527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:3">
       <c r="A77" s="1" t="s">
         <v>94</v>
       </c>
@@ -4560,7 +4538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:3">
       <c r="A78" s="1" t="s">
         <v>96</v>
       </c>
@@ -4571,7 +4549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:3">
       <c r="A79" s="1" t="s">
         <v>97</v>
       </c>
@@ -4582,7 +4560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:3">
       <c r="A80" s="1" t="s">
         <v>99</v>
       </c>
@@ -4593,7 +4571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
         <v>748</v>
       </c>
@@ -4604,7 +4582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:3">
       <c r="A82" s="1" t="s">
         <v>101</v>
       </c>
@@ -4615,7 +4593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:3">
       <c r="A83" s="1" t="s">
         <v>621</v>
       </c>
@@ -4626,7 +4604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:3">
       <c r="A84" s="1" t="s">
         <v>995</v>
       </c>
@@ -4637,7 +4615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
         <v>934</v>
       </c>
@@ -4648,7 +4626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:3">
       <c r="A86" s="1" t="s">
         <v>103</v>
       </c>
@@ -4659,7 +4637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:3">
       <c r="A87" s="1" t="s">
         <v>104</v>
       </c>
@@ -4670,7 +4648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:3">
       <c r="A88" s="1" t="s">
         <v>105</v>
       </c>
@@ -4681,7 +4659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
         <v>106</v>
       </c>
@@ -4692,7 +4670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:3">
       <c r="A90" s="1" t="s">
         <v>107</v>
       </c>
@@ -4703,7 +4681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:3">
       <c r="A91" s="1" t="s">
         <v>108</v>
       </c>
@@ -4714,7 +4692,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:3">
       <c r="A92" s="1" t="s">
         <v>109</v>
       </c>
@@ -4725,7 +4703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:3">
       <c r="A93" s="1" t="s">
         <v>782</v>
       </c>
@@ -4736,7 +4714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:3">
       <c r="A94" s="1" t="s">
         <v>820</v>
       </c>
@@ -4747,7 +4725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:3">
       <c r="A95" s="1" t="s">
         <v>110</v>
       </c>
@@ -4758,7 +4736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:3">
       <c r="A96" s="1" t="s">
         <v>111</v>
       </c>
@@ -4769,7 +4747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:3">
       <c r="A97" s="1" t="s">
         <v>742</v>
       </c>
@@ -4780,7 +4758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:3">
       <c r="A98" s="1" t="s">
         <v>112</v>
       </c>
@@ -4791,7 +4769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:3">
       <c r="A99" s="1" t="s">
         <v>113</v>
       </c>
@@ -4802,7 +4780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:3">
       <c r="A100" s="1" t="s">
         <v>114</v>
       </c>
@@ -4813,7 +4791,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:3">
       <c r="A101" s="1" t="s">
         <v>115</v>
       </c>
@@ -4824,7 +4802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:3">
       <c r="A102" s="1" t="s">
         <v>116</v>
       </c>
@@ -4835,7 +4813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:3">
       <c r="A103" s="1" t="s">
         <v>117</v>
       </c>
@@ -4846,7 +4824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:3">
       <c r="A104" s="1" t="s">
         <v>118</v>
       </c>
@@ -4857,7 +4835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:3">
       <c r="A105" s="1" t="s">
         <v>119</v>
       </c>
@@ -4868,7 +4846,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:3">
       <c r="A106" s="1" t="s">
         <v>909</v>
       </c>
@@ -4879,7 +4857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:3">
       <c r="A107" s="1" t="s">
         <v>751</v>
       </c>
@@ -4890,7 +4868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:3">
       <c r="A108" s="1" t="s">
         <v>120</v>
       </c>
@@ -4901,7 +4879,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:3">
       <c r="A109" s="1" t="s">
         <v>121</v>
       </c>
@@ -4912,7 +4890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:3">
       <c r="A110" s="1" t="s">
         <v>655</v>
       </c>
@@ -4923,7 +4901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:3">
       <c r="A111" s="1" t="s">
         <v>149</v>
       </c>
@@ -4934,7 +4912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:3">
       <c r="A112" s="1" t="s">
         <v>150</v>
       </c>
@@ -4945,7 +4923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:3">
       <c r="A113" s="1" t="s">
         <v>151</v>
       </c>
@@ -4956,7 +4934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:3">
       <c r="A114" s="1" t="s">
         <v>979</v>
       </c>
@@ -4967,7 +4945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:3">
       <c r="A115" s="1" t="s">
         <v>152</v>
       </c>
@@ -4978,7 +4956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:3">
       <c r="A116" s="1" t="s">
         <v>794</v>
       </c>
@@ -4989,7 +4967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:3">
       <c r="A117" s="1" t="s">
         <v>153</v>
       </c>
@@ -5000,7 +4978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:3">
       <c r="A118" s="1" t="s">
         <v>154</v>
       </c>
@@ -5011,7 +4989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:3">
       <c r="A119" s="1" t="s">
         <v>155</v>
       </c>
@@ -5022,7 +5000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:3">
       <c r="A120" s="1" t="s">
         <v>156</v>
       </c>
@@ -5033,7 +5011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:3">
       <c r="A121" s="1" t="s">
         <v>981</v>
       </c>
@@ -5044,7 +5022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:3">
       <c r="A122" s="1" t="s">
         <v>157</v>
       </c>
@@ -5055,7 +5033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:3">
       <c r="A123" s="1" t="s">
         <v>158</v>
       </c>
@@ -5066,7 +5044,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:3">
       <c r="A124" s="1" t="s">
         <v>159</v>
       </c>
@@ -5077,7 +5055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:3">
       <c r="A125" s="1" t="s">
         <v>944</v>
       </c>
@@ -5088,7 +5066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:3">
       <c r="A126" s="1" t="s">
         <v>160</v>
       </c>
@@ -5099,7 +5077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:3">
       <c r="A127" s="1" t="s">
         <v>873</v>
       </c>
@@ -5110,7 +5088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:3">
       <c r="A128" s="1" t="s">
         <v>702</v>
       </c>
@@ -5121,7 +5099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:3">
       <c r="A129" s="1" t="s">
         <v>895</v>
       </c>
@@ -5132,7 +5110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:3">
       <c r="A130" s="1" t="s">
         <v>983</v>
       </c>
@@ -5143,7 +5121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:3">
       <c r="A131" s="1" t="s">
         <v>611</v>
       </c>
@@ -5154,7 +5132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:3">
       <c r="A132" s="1" t="s">
         <v>161</v>
       </c>
@@ -5165,7 +5143,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:3">
       <c r="A133" s="1" t="s">
         <v>162</v>
       </c>
@@ -5176,7 +5154,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:3">
       <c r="A134" s="1" t="s">
         <v>163</v>
       </c>
@@ -5187,7 +5165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:3">
       <c r="A135" s="1" t="s">
         <v>164</v>
       </c>
@@ -5198,7 +5176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:3">
       <c r="A136" s="1" t="s">
         <v>165</v>
       </c>
@@ -5209,7 +5187,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:3">
       <c r="A137" s="1" t="s">
         <v>166</v>
       </c>
@@ -5220,7 +5198,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:3">
       <c r="A138" s="1" t="s">
         <v>167</v>
       </c>
@@ -5231,7 +5209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:3">
       <c r="A139" s="1" t="s">
         <v>168</v>
       </c>
@@ -5242,7 +5220,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:3">
       <c r="A140" s="1" t="s">
         <v>985</v>
       </c>
@@ -5253,7 +5231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:3">
       <c r="A141" s="1" t="s">
         <v>169</v>
       </c>
@@ -5264,7 +5242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:3">
       <c r="A142" s="1" t="s">
         <v>865</v>
       </c>
@@ -5275,7 +5253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:3">
       <c r="A143" s="1" t="s">
         <v>883</v>
       </c>
@@ -5286,7 +5264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:3">
       <c r="A144" s="1" t="s">
         <v>790</v>
       </c>
@@ -5297,7 +5275,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:3">
       <c r="A145" s="1" t="s">
         <v>170</v>
       </c>
@@ -5308,7 +5286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:3">
       <c r="A146" s="1" t="s">
         <v>172</v>
       </c>
@@ -5319,7 +5297,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:3">
       <c r="A147" s="1" t="s">
         <v>603</v>
       </c>
@@ -5330,7 +5308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:3">
       <c r="A148" s="1" t="s">
         <v>171</v>
       </c>
@@ -5341,7 +5319,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:3">
       <c r="A149" s="1" t="s">
         <v>173</v>
       </c>
@@ -5352,7 +5330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:3">
       <c r="A150" s="1" t="s">
         <v>921</v>
       </c>
@@ -5363,7 +5341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:3">
       <c r="A151" s="1" t="s">
         <v>174</v>
       </c>
@@ -5374,7 +5352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:3">
       <c r="A152" s="1" t="s">
         <v>175</v>
       </c>
@@ -5385,7 +5363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:3">
       <c r="A153" s="1" t="s">
         <v>812</v>
       </c>
@@ -5396,7 +5374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:3">
       <c r="A154" s="1" t="s">
         <v>635</v>
       </c>
@@ -5407,7 +5385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:3">
       <c r="A155" s="1" t="s">
         <v>177</v>
       </c>
@@ -5418,7 +5396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:3">
       <c r="A156" s="1" t="s">
         <v>182</v>
       </c>
@@ -5429,7 +5407,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:3">
       <c r="A157" s="1" t="s">
         <v>183</v>
       </c>
@@ -5440,7 +5418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:3">
       <c r="A158" s="1" t="s">
         <v>179</v>
       </c>
@@ -5451,7 +5429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:3">
       <c r="A159" s="1" t="s">
         <v>181</v>
       </c>
@@ -5462,7 +5440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:3">
       <c r="A160" s="1" t="s">
         <v>180</v>
       </c>
@@ -5473,7 +5451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:3">
       <c r="A161" s="1" t="s">
         <v>178</v>
       </c>
@@ -5484,7 +5462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:3">
       <c r="A162" s="1" t="s">
         <v>176</v>
       </c>
@@ -5495,7 +5473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:3">
       <c r="A163" s="1" t="s">
         <v>977</v>
       </c>
@@ -5506,7 +5484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:3">
       <c r="A164" s="1" t="s">
         <v>184</v>
       </c>
@@ -5517,7 +5495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:3">
       <c r="A165" s="1" t="s">
         <v>185</v>
       </c>
@@ -5528,7 +5506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:3">
       <c r="A166" s="1" t="s">
         <v>186</v>
       </c>
@@ -5539,7 +5517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:3">
       <c r="A167" s="1" t="s">
         <v>935</v>
       </c>
@@ -5550,7 +5528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:3">
       <c r="A168" s="1" t="s">
         <v>931</v>
       </c>
@@ -5561,7 +5539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:3">
       <c r="A169" s="1" t="s">
         <v>187</v>
       </c>
@@ -5572,7 +5550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:3">
       <c r="A170" s="1" t="s">
         <v>764</v>
       </c>
@@ -5583,7 +5561,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:3">
       <c r="A171" s="1" t="s">
         <v>700</v>
       </c>
@@ -5594,7 +5572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:3">
       <c r="A172" s="1" t="s">
         <v>729</v>
       </c>
@@ -5605,7 +5583,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:3">
       <c r="A173" s="1" t="s">
         <v>188</v>
       </c>
@@ -5616,7 +5594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:3">
       <c r="A174" s="1" t="s">
         <v>189</v>
       </c>
@@ -5627,7 +5605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:3">
       <c r="A175" s="1" t="s">
         <v>190</v>
       </c>
@@ -5638,7 +5616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:3">
       <c r="A176" s="1" t="s">
         <v>191</v>
       </c>
@@ -5649,7 +5627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:3">
       <c r="A177" s="1" t="s">
         <v>776</v>
       </c>
@@ -5660,7 +5638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:3">
       <c r="A178" s="1" t="s">
         <v>192</v>
       </c>
@@ -5671,7 +5649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:3">
       <c r="A179" s="1" t="s">
         <v>193</v>
       </c>
@@ -5682,7 +5660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:3">
       <c r="A180" s="1" t="s">
         <v>879</v>
       </c>
@@ -5693,7 +5671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:3">
       <c r="A181" s="1" t="s">
         <v>871</v>
       </c>
@@ -5704,7 +5682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:3">
       <c r="A182" s="1" t="s">
         <v>194</v>
       </c>
@@ -5715,7 +5693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:3">
       <c r="A183" s="1" t="s">
         <v>824</v>
       </c>
@@ -5726,7 +5704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:3">
       <c r="A184" s="1" t="s">
         <v>195</v>
       </c>
@@ -5737,7 +5715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:3">
       <c r="A185" s="1" t="s">
         <v>955</v>
       </c>
@@ -5748,7 +5726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:3">
       <c r="A186" s="1" t="s">
         <v>875</v>
       </c>
@@ -5759,7 +5737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:3">
       <c r="A187" s="1" t="s">
         <v>196</v>
       </c>
@@ -5770,7 +5748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:3">
       <c r="A188" s="1" t="s">
         <v>605</v>
       </c>
@@ -5781,7 +5759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:3">
       <c r="A189" s="1" t="s">
         <v>597</v>
       </c>
@@ -5792,7 +5770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:3">
       <c r="A190" s="1" t="s">
         <v>197</v>
       </c>
@@ -5803,7 +5781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:3">
       <c r="A191" s="1" t="s">
         <v>867</v>
       </c>
@@ -5814,7 +5792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:3">
       <c r="A192" s="1" t="s">
         <v>927</v>
       </c>
@@ -5825,7 +5803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:3">
       <c r="A193" s="1" t="s">
         <v>198</v>
       </c>
@@ -5836,7 +5814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:3">
       <c r="A194" s="1" t="s">
         <v>199</v>
       </c>
@@ -5847,7 +5825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:3">
       <c r="A195" s="1" t="s">
         <v>200</v>
       </c>
@@ -5858,7 +5836,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:3">
       <c r="A196" s="1" t="s">
         <v>201</v>
       </c>
@@ -5869,7 +5847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:3">
       <c r="A197" s="1" t="s">
         <v>202</v>
       </c>
@@ -5880,7 +5858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:3">
       <c r="A198" s="1" t="s">
         <v>203</v>
       </c>
@@ -5891,7 +5869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:3">
       <c r="A199" s="1" t="s">
         <v>204</v>
       </c>
@@ -5902,7 +5880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:3">
       <c r="A200" s="1" t="s">
         <v>205</v>
       </c>
@@ -5913,7 +5891,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:3">
       <c r="A201" s="1" t="s">
         <v>662</v>
       </c>
@@ -5924,7 +5902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:3">
       <c r="A202" s="1" t="s">
         <v>207</v>
       </c>
@@ -5935,7 +5913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:3">
       <c r="A203" s="1" t="s">
         <v>206</v>
       </c>
@@ -5946,7 +5924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:3">
       <c r="A204" s="1" t="s">
         <v>208</v>
       </c>
@@ -5957,7 +5935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:3">
       <c r="A205" s="1" t="s">
         <v>209</v>
       </c>
@@ -5968,7 +5946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:3">
       <c r="A206" s="1" t="s">
         <v>210</v>
       </c>
@@ -5979,7 +5957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:3">
       <c r="A207" s="1" t="s">
         <v>211</v>
       </c>
@@ -5990,7 +5968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:3">
       <c r="A208" s="1" t="s">
         <v>212</v>
       </c>
@@ -6001,7 +5979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:3">
       <c r="A209" s="1" t="s">
         <v>212</v>
       </c>
@@ -6012,7 +5990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:3">
       <c r="A210" s="1" t="s">
         <v>213</v>
       </c>
@@ -6023,7 +6001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:3">
       <c r="A211" s="1" t="s">
         <v>214</v>
       </c>
@@ -6034,7 +6012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:3">
       <c r="A212" s="1" t="s">
         <v>216</v>
       </c>
@@ -6045,7 +6023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:3">
       <c r="A213" s="1" t="s">
         <v>217</v>
       </c>
@@ -6056,7 +6034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:3">
       <c r="A214" s="1" t="s">
         <v>855</v>
       </c>
@@ -6067,7 +6045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:3">
       <c r="A215" s="1" t="s">
         <v>893</v>
       </c>
@@ -6078,7 +6056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:3">
       <c r="A216" s="1" t="s">
         <v>215</v>
       </c>
@@ -6089,7 +6067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:3">
       <c r="A217" s="1" t="s">
         <v>852</v>
       </c>
@@ -6100,7 +6078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:3">
       <c r="A218" s="1" t="s">
         <v>650</v>
       </c>
@@ -6111,7 +6089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:3">
       <c r="A219" s="1" t="s">
         <v>772</v>
       </c>
@@ -6122,7 +6100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:3">
       <c r="A220" s="1" t="s">
         <v>901</v>
       </c>
@@ -6133,7 +6111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:3">
       <c r="A221" s="1" t="s">
         <v>682</v>
       </c>
@@ -6144,7 +6122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:3">
       <c r="A222" s="1" t="s">
         <v>938</v>
       </c>
@@ -6155,7 +6133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:3">
       <c r="A223" s="1" t="s">
         <v>1005</v>
       </c>
@@ -6166,7 +6144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:3">
       <c r="A224" s="1" t="s">
         <v>756</v>
       </c>
@@ -6177,7 +6155,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="225" spans="1:3">
       <c r="A225" s="1" t="s">
         <v>692</v>
       </c>
@@ -6188,7 +6166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:3">
       <c r="A226" s="1" t="s">
         <v>218</v>
       </c>
@@ -6199,7 +6177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="227" spans="1:3">
       <c r="A227" s="1" t="s">
         <v>623</v>
       </c>
@@ -6210,7 +6188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:3">
       <c r="A228" s="1" t="s">
         <v>219</v>
       </c>
@@ -6221,7 +6199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="229" spans="1:3">
       <c r="A229" s="1" t="s">
         <v>220</v>
       </c>
@@ -6232,7 +6210,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="230" spans="1:3">
       <c r="A230" s="1" t="s">
         <v>221</v>
       </c>
@@ -6243,7 +6221,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="231" spans="1:3">
       <c r="A231" s="1" t="s">
         <v>992</v>
       </c>
@@ -6254,7 +6232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:3">
       <c r="A232" s="1" t="s">
         <v>953</v>
       </c>
@@ -6265,7 +6243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="233" spans="1:3">
       <c r="A233" s="1" t="s">
         <v>892</v>
       </c>
@@ -6276,7 +6254,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:3">
       <c r="A234" s="1" t="s">
         <v>885</v>
       </c>
@@ -6287,7 +6265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="235" spans="1:3">
       <c r="A235" s="1" t="s">
         <v>991</v>
       </c>
@@ -6298,7 +6276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="236" spans="1:3">
       <c r="A236" s="1" t="s">
         <v>804</v>
       </c>
@@ -6309,7 +6287,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="237" spans="1:3">
       <c r="A237" s="1" t="s">
         <v>222</v>
       </c>
@@ -6320,7 +6298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:3">
       <c r="A238" s="1" t="s">
         <v>223</v>
       </c>
@@ -6331,7 +6309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="239" spans="1:3">
       <c r="A239" s="1" t="s">
         <v>224</v>
       </c>
@@ -6342,7 +6320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:3">
       <c r="A240" s="1" t="s">
         <v>225</v>
       </c>
@@ -6353,7 +6331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:3">
       <c r="A241" s="1" t="s">
         <v>226</v>
       </c>
@@ -6364,7 +6342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:3">
       <c r="A242" s="1" t="s">
         <v>227</v>
       </c>
@@ -6375,7 +6353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="243" spans="1:3">
       <c r="A243" s="1" t="s">
         <v>228</v>
       </c>
@@ -6386,7 +6364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="244" spans="1:3">
       <c r="A244" s="1" t="s">
         <v>229</v>
       </c>
@@ -6397,7 +6375,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="245" spans="1:3">
       <c r="A245" s="1" t="s">
         <v>230</v>
       </c>
@@ -6408,7 +6386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="246" spans="1:3">
       <c r="A246" s="1" t="s">
         <v>231</v>
       </c>
@@ -6419,7 +6397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="247" spans="1:3">
       <c r="A247" s="1" t="s">
         <v>232</v>
       </c>
@@ -6430,7 +6408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="248" spans="1:3">
       <c r="A248" s="1" t="s">
         <v>696</v>
       </c>
@@ -6441,7 +6419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="249" spans="1:3">
       <c r="A249" s="1" t="s">
         <v>917</v>
       </c>
@@ -6452,7 +6430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="250" spans="1:3">
       <c r="A250" s="1" t="s">
         <v>844</v>
       </c>
@@ -6463,7 +6441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="251" spans="1:3">
       <c r="A251" s="1" t="s">
         <v>704</v>
       </c>
@@ -6474,7 +6452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:3">
       <c r="A252" s="1" t="s">
         <v>233</v>
       </c>
@@ -6485,7 +6463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="253" spans="1:3">
       <c r="A253" s="1" t="s">
         <v>235</v>
       </c>
@@ -6496,7 +6474,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="254" spans="1:3">
       <c r="A254" s="1" t="s">
         <v>234</v>
       </c>
@@ -6507,7 +6485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="255" spans="1:3">
       <c r="A255" s="1" t="s">
         <v>754</v>
       </c>
@@ -6518,7 +6496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="256" spans="1:3">
       <c r="A256" s="1" t="s">
         <v>859</v>
       </c>
@@ -6529,7 +6507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="257" spans="1:3">
       <c r="A257" s="1" t="s">
         <v>236</v>
       </c>
@@ -6540,7 +6518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="258" spans="1:3">
       <c r="A258" s="1" t="s">
         <v>237</v>
       </c>
@@ -6551,7 +6529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="259" spans="1:3">
       <c r="A259" s="1" t="s">
         <v>890</v>
       </c>
@@ -6562,7 +6540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="260" spans="1:3">
       <c r="A260" s="1" t="s">
         <v>238</v>
       </c>
@@ -6573,7 +6551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="261" spans="1:3">
       <c r="A261" s="1" t="s">
         <v>808</v>
       </c>
@@ -6584,7 +6562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="262" spans="1:3">
       <c r="A262" s="1" t="s">
         <v>911</v>
       </c>
@@ -6595,7 +6573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="263" spans="1:3">
       <c r="A263" s="1" t="s">
         <v>239</v>
       </c>
@@ -6606,7 +6584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="264" spans="1:3">
       <c r="A264" s="1" t="s">
         <v>670</v>
       </c>
@@ -6617,7 +6595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="265" spans="1:3">
       <c r="A265" s="1" t="s">
         <v>752</v>
       </c>
@@ -6628,7 +6606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="266" spans="1:3">
       <c r="A266" s="1" t="s">
         <v>637</v>
       </c>
@@ -6639,7 +6617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="267" spans="1:3">
       <c r="A267" s="1" t="s">
         <v>240</v>
       </c>
@@ -6650,7 +6628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="268" spans="1:3">
       <c r="A268" s="1" t="s">
         <v>241</v>
       </c>
@@ -6661,7 +6639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="269" spans="1:3">
       <c r="A269" s="1" t="s">
         <v>242</v>
       </c>
@@ -6672,7 +6650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="270" spans="1:3">
       <c r="A270" s="1" t="s">
         <v>243</v>
       </c>
@@ -6680,7 +6658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="271" spans="1:3">
       <c r="A271" s="1" t="s">
         <v>244</v>
       </c>
@@ -6691,7 +6669,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="272" spans="1:3">
       <c r="A272" s="1" t="s">
         <v>245</v>
       </c>
@@ -6702,7 +6680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:3">
       <c r="A273" s="1" t="s">
         <v>706</v>
       </c>
@@ -6713,7 +6691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="274" spans="1:3">
       <c r="A274" s="1" t="s">
         <v>246</v>
       </c>
@@ -6724,7 +6702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="275" spans="1:3">
       <c r="A275" s="1" t="s">
         <v>667</v>
       </c>
@@ -6735,7 +6713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="276" spans="1:3">
       <c r="A276" s="1" t="s">
         <v>247</v>
       </c>
@@ -6746,7 +6724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="277" spans="1:3">
       <c r="A277" s="1" t="s">
         <v>766</v>
       </c>
@@ -6757,7 +6735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="278" spans="1:3">
       <c r="A278" s="1" t="s">
         <v>248</v>
       </c>
@@ -6768,7 +6746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="279" spans="1:3">
       <c r="A279" s="1" t="s">
         <v>830</v>
       </c>
@@ -6779,7 +6757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="280" spans="1:3">
       <c r="A280" s="1" t="s">
         <v>788</v>
       </c>
@@ -6790,7 +6768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="281" spans="1:3">
       <c r="A281" s="1" t="s">
         <v>249</v>
       </c>
@@ -6801,7 +6779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:3">
       <c r="A282" s="1" t="s">
         <v>250</v>
       </c>
@@ -6812,7 +6790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="283" spans="1:3">
       <c r="A283" s="1" t="s">
         <v>899</v>
       </c>
@@ -6823,7 +6801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="284" spans="1:3">
       <c r="A284" s="1" t="s">
         <v>251</v>
       </c>
@@ -6834,7 +6812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="285" spans="1:3">
       <c r="A285" s="1" t="s">
         <v>708</v>
       </c>
@@ -6845,7 +6823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="286" spans="1:3">
       <c r="A286" s="1" t="s">
         <v>252</v>
       </c>
@@ -6856,7 +6834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="287" spans="1:3">
       <c r="A287" s="1" t="s">
         <v>975</v>
       </c>
@@ -6867,7 +6845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="288" spans="1:3">
       <c r="A288" s="1" t="s">
         <v>253</v>
       </c>
@@ -6878,7 +6856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="289" spans="1:3">
       <c r="A289" s="1" t="s">
         <v>834</v>
       </c>
@@ -6889,7 +6867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="290" spans="1:3">
       <c r="A290" s="1" t="s">
         <v>254</v>
       </c>
@@ -6900,7 +6878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="291" spans="1:3">
       <c r="A291" s="1" t="s">
         <v>255</v>
       </c>
@@ -6911,7 +6889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="292" spans="1:3">
       <c r="A292" s="1" t="s">
         <v>256</v>
       </c>
@@ -6922,7 +6900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="293" spans="1:3">
       <c r="A293" s="1" t="s">
         <v>608</v>
       </c>
@@ -6933,7 +6911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="294" spans="1:3">
       <c r="A294" s="1" t="s">
         <v>907</v>
       </c>
@@ -6944,7 +6922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="295" spans="1:3">
       <c r="A295" s="1" t="s">
         <v>258</v>
       </c>
@@ -6955,7 +6933,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="296" spans="1:3">
       <c r="A296" s="1" t="s">
         <v>257</v>
       </c>
@@ -6966,7 +6944,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="297" spans="1:3">
       <c r="A297" s="1" t="s">
         <v>786</v>
       </c>
@@ -6977,7 +6955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="298" spans="1:3">
       <c r="A298" s="1" t="s">
         <v>710</v>
       </c>
@@ -6988,7 +6966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="299" spans="1:3">
       <c r="A299" s="1" t="s">
         <v>259</v>
       </c>
@@ -6999,7 +6977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="300" spans="1:3">
       <c r="A300" s="1" t="s">
         <v>260</v>
       </c>
@@ -7010,7 +6988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="301" spans="1:3">
       <c r="A301" s="1" t="s">
         <v>262</v>
       </c>
@@ -7021,7 +6999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="302" spans="1:3">
       <c r="A302" s="1" t="s">
         <v>740</v>
       </c>
@@ -7032,7 +7010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="303" spans="1:3">
       <c r="A303" s="1" t="s">
         <v>263</v>
       </c>
@@ -7043,7 +7021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="304" spans="1:3">
       <c r="A304" s="1" t="s">
         <v>1000</v>
       </c>
@@ -7054,7 +7032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="305" spans="1:3">
       <c r="A305" s="1" t="s">
         <v>264</v>
       </c>
@@ -7065,7 +7043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="306" spans="1:3">
       <c r="A306" s="1" t="s">
         <v>261</v>
       </c>
@@ -7076,7 +7054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="307" spans="1:3">
       <c r="A307" s="1" t="s">
         <v>265</v>
       </c>
@@ -7087,7 +7065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="308" spans="1:3">
       <c r="A308" s="1" t="s">
         <v>266</v>
       </c>
@@ -7098,7 +7076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="309" spans="1:3">
       <c r="A309" s="1" t="s">
         <v>267</v>
       </c>
@@ -7109,7 +7087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="310" spans="1:3">
       <c r="A310" s="1" t="s">
         <v>712</v>
       </c>
@@ -7120,7 +7098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="311" spans="1:3">
       <c r="A311" s="1" t="s">
         <v>905</v>
       </c>
@@ -7131,7 +7109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="312" spans="1:3">
       <c r="A312" s="1" t="s">
         <v>268</v>
       </c>
@@ -7142,7 +7120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="313" spans="1:3">
       <c r="A313" s="1" t="s">
         <v>269</v>
       </c>
@@ -7153,7 +7131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="314" spans="1:3">
       <c r="A314" s="1" t="s">
         <v>270</v>
       </c>
@@ -7164,7 +7142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="315" spans="1:3">
       <c r="A315" s="1" t="s">
         <v>271</v>
       </c>
@@ -7175,7 +7153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="316" spans="1:3">
       <c r="A316" s="1" t="s">
         <v>272</v>
       </c>
@@ -7186,7 +7164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="317" spans="1:3">
       <c r="A317" s="1" t="s">
         <v>973</v>
       </c>
@@ -7197,7 +7175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="318" spans="1:3">
       <c r="A318" s="1" t="s">
         <v>989</v>
       </c>
@@ -7208,7 +7186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="319" spans="1:3">
       <c r="A319" s="1" t="s">
         <v>656</v>
       </c>
@@ -7219,7 +7197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="320" spans="1:3">
       <c r="A320" s="1" t="s">
         <v>273</v>
       </c>
@@ -7230,7 +7208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="321" spans="1:3">
       <c r="A321" s="1" t="s">
         <v>274</v>
       </c>
@@ -7241,7 +7219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="322" spans="1:3">
       <c r="A322" s="1" t="s">
         <v>275</v>
       </c>
@@ -7252,7 +7230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="323" spans="1:3">
       <c r="A323" s="1" t="s">
         <v>746</v>
       </c>
@@ -7263,7 +7241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="324" spans="1:3">
       <c r="A324" s="1" t="s">
         <v>276</v>
       </c>
@@ -7274,7 +7252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="325" spans="1:3">
       <c r="A325" s="1" t="s">
         <v>277</v>
       </c>
@@ -7285,7 +7263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="326" spans="1:3">
       <c r="A326" s="1" t="s">
         <v>601</v>
       </c>
@@ -7296,7 +7274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="327" spans="1:3">
       <c r="A327" s="1" t="s">
         <v>803</v>
       </c>
@@ -7307,7 +7285,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="328" spans="1:3">
       <c r="A328" s="1" t="s">
         <v>278</v>
       </c>
@@ -7318,7 +7296,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="329" spans="1:3">
       <c r="A329" s="1" t="s">
         <v>279</v>
       </c>
@@ -7329,7 +7307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="330" spans="1:3">
       <c r="A330" s="1" t="s">
         <v>280</v>
       </c>
@@ -7340,7 +7318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="331" spans="1:3">
       <c r="A331" s="1" t="s">
         <v>744</v>
       </c>
@@ -7351,7 +7329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="332" spans="1:3">
       <c r="A332" s="1" t="s">
         <v>698</v>
       </c>
@@ -7362,7 +7340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="333" spans="1:3">
       <c r="A333" s="1" t="s">
         <v>727</v>
       </c>
@@ -7373,7 +7351,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="334" spans="1:3">
       <c r="A334" s="1" t="s">
         <v>281</v>
       </c>
@@ -7384,7 +7362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="335" spans="1:3">
       <c r="A335" s="1" t="s">
         <v>282</v>
       </c>
@@ -7395,7 +7373,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="336" spans="1:3">
       <c r="A336" s="1" t="s">
         <v>283</v>
       </c>
@@ -7406,7 +7384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="337" spans="1:3">
       <c r="A337" s="1" t="s">
         <v>987</v>
       </c>
@@ -7417,7 +7395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="338" spans="1:3">
       <c r="A338" s="1" t="s">
         <v>284</v>
       </c>
@@ -7428,7 +7406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="339" spans="1:3">
       <c r="A339" s="1" t="s">
         <v>285</v>
       </c>
@@ -7439,7 +7417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="340" spans="1:3">
       <c r="A340" s="1" t="s">
         <v>286</v>
       </c>
@@ -7450,7 +7428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="341" spans="1:3">
       <c r="A341" s="1" t="s">
         <v>967</v>
       </c>
@@ -7461,7 +7439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="342" spans="1:3">
       <c r="A342" s="1" t="s">
         <v>287</v>
       </c>
@@ -7472,7 +7450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="343" spans="1:3">
       <c r="A343" s="1" t="s">
         <v>288</v>
       </c>
@@ -7483,7 +7461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="344" spans="1:3">
       <c r="A344" s="1" t="s">
         <v>289</v>
       </c>
@@ -7494,7 +7472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="345" spans="1:3">
       <c r="A345" s="1" t="s">
         <v>290</v>
       </c>
@@ -7505,7 +7483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="346" spans="1:3">
       <c r="A346" s="1" t="s">
         <v>774</v>
       </c>
@@ -7516,7 +7494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="347" spans="1:3">
       <c r="A347" s="1" t="s">
         <v>291</v>
       </c>
@@ -7527,7 +7505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="348" spans="1:3">
       <c r="A348" s="1" t="s">
         <v>738</v>
       </c>
@@ -7538,7 +7516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="349" spans="1:3">
       <c r="A349" s="1" t="s">
         <v>881</v>
       </c>
@@ -7549,7 +7527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="350" spans="1:3">
       <c r="A350" s="1" t="s">
         <v>736</v>
       </c>
@@ -7560,7 +7538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="351" spans="1:3">
       <c r="A351" s="1" t="s">
         <v>292</v>
       </c>
@@ -7571,7 +7549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="352" spans="1:3">
       <c r="A352" s="1" t="s">
         <v>653</v>
       </c>
@@ -7582,7 +7560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="353" spans="1:3">
       <c r="A353" s="1" t="s">
         <v>952</v>
       </c>
@@ -7593,7 +7571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="354" spans="1:3">
       <c r="A354" s="1" t="s">
         <v>293</v>
       </c>
@@ -7604,7 +7582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="355" spans="1:3">
       <c r="A355" s="1" t="s">
         <v>294</v>
       </c>
@@ -7615,7 +7593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="356" spans="1:3">
       <c r="A356" s="1" t="s">
         <v>971</v>
       </c>
@@ -7626,7 +7604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="357" spans="1:3">
       <c r="A357" s="1" t="s">
         <v>295</v>
       </c>
@@ -7637,7 +7615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="358" spans="1:3">
       <c r="A358" s="1" t="s">
         <v>714</v>
       </c>
@@ -7648,7 +7626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="359" spans="1:3">
       <c r="A359" s="1" t="s">
         <v>296</v>
       </c>
@@ -7659,7 +7637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="360" spans="1:3">
       <c r="A360" s="1" t="s">
         <v>919</v>
       </c>
@@ -7670,7 +7648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="361" spans="1:3">
       <c r="A361" s="1" t="s">
         <v>297</v>
       </c>
@@ -7681,7 +7659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="362" spans="1:3">
       <c r="A362" s="1" t="s">
         <v>877</v>
       </c>
@@ -7692,7 +7670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="363" spans="1:3">
       <c r="A363" s="1" t="s">
         <v>680</v>
       </c>
@@ -7703,7 +7681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="364" spans="1:3">
       <c r="A364" s="1" t="s">
         <v>965</v>
       </c>
@@ -7714,7 +7692,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="365" spans="1:3">
       <c r="A365" s="1" t="s">
         <v>298</v>
       </c>
@@ -7725,7 +7703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="366" spans="1:3">
       <c r="A366" s="1" t="s">
         <v>913</v>
       </c>
@@ -7736,7 +7714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="367" spans="1:3">
       <c r="A367" s="1" t="s">
         <v>299</v>
       </c>
@@ -7747,7 +7725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="368" spans="1:3">
       <c r="A368" s="1" t="s">
         <v>300</v>
       </c>
@@ -7758,7 +7736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="369" spans="1:3">
       <c r="A369" s="1" t="s">
         <v>903</v>
       </c>
@@ -7769,7 +7747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="370" spans="1:3">
       <c r="A370" s="1" t="s">
         <v>836</v>
       </c>
@@ -7780,7 +7758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="371" spans="1:3">
       <c r="A371" s="1" t="s">
         <v>869</v>
       </c>
@@ -7791,7 +7769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="372" spans="1:3">
       <c r="A372" s="1" t="s">
         <v>301</v>
       </c>
@@ -7799,7 +7777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="373" spans="1:3">
       <c r="A373" s="1" t="s">
         <v>302</v>
       </c>
@@ -7810,7 +7788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="374" spans="1:3">
       <c r="A374" s="1" t="s">
         <v>303</v>
       </c>
@@ -7821,7 +7799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="375" spans="1:3">
       <c r="A375" s="1" t="s">
         <v>304</v>
       </c>
@@ -7832,7 +7810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="376" spans="1:3">
       <c r="A376" s="1" t="s">
         <v>846</v>
       </c>
@@ -7843,7 +7821,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="377" spans="1:3">
       <c r="A377" s="1" t="s">
         <v>305</v>
       </c>
@@ -7854,7 +7832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="378" spans="1:3">
       <c r="A378" s="1" t="s">
         <v>625</v>
       </c>
@@ -7865,7 +7843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="379" spans="1:3">
       <c r="A379" s="1" t="s">
         <v>639</v>
       </c>
@@ -7876,7 +7854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="380" spans="1:3">
       <c r="A380" s="1" t="s">
         <v>678</v>
       </c>
@@ -7887,7 +7865,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="381" spans="1:3">
       <c r="A381" s="1" t="s">
         <v>672</v>
       </c>
@@ -7898,7 +7876,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="382" spans="1:3">
       <c r="A382" s="1" t="s">
         <v>306</v>
       </c>
@@ -7909,7 +7887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="383" spans="1:3">
       <c r="A383" s="1" t="s">
         <v>307</v>
       </c>
@@ -7920,7 +7898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="384" spans="1:3">
       <c r="A384" s="1" t="s">
         <v>818</v>
       </c>
@@ -7931,7 +7909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="385" spans="1:3">
       <c r="A385" s="1" t="s">
         <v>308</v>
       </c>
@@ -7942,7 +7920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="386" spans="1:3">
       <c r="A386" s="1" t="s">
         <v>688</v>
       </c>
@@ -7953,7 +7931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="387" spans="1:3">
       <c r="A387" s="1" t="s">
         <v>309</v>
       </c>
@@ -7964,7 +7942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="388" spans="1:3">
       <c r="A388" s="1" t="s">
         <v>897</v>
       </c>
@@ -7975,7 +7953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="389" spans="1:3">
       <c r="A389" s="1" t="s">
         <v>310</v>
       </c>
@@ -7986,7 +7964,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="390" spans="1:3">
       <c r="A390" s="1" t="s">
         <v>716</v>
       </c>
@@ -7997,7 +7975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="391" spans="1:3">
       <c r="A391" s="1" t="s">
         <v>311</v>
       </c>
@@ -8008,7 +7986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="392" spans="1:3">
       <c r="A392" s="1" t="s">
         <v>312</v>
       </c>
@@ -8019,7 +7997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="393" spans="1:3">
       <c r="A393" s="1" t="s">
         <v>796</v>
       </c>
@@ -8030,7 +8008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="394" spans="1:3">
       <c r="A394" s="1" t="s">
         <v>313</v>
       </c>
@@ -8041,7 +8019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="395" spans="1:3">
       <c r="A395" s="1" t="s">
         <v>618</v>
       </c>
@@ -8052,7 +8030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="396" spans="1:3">
       <c r="A396" s="1" t="s">
         <v>613</v>
       </c>
@@ -8063,7 +8041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="397" spans="1:3">
       <c r="A397" s="1" t="s">
         <v>616</v>
       </c>
@@ -8074,7 +8052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="398" spans="1:3">
       <c r="A398" s="1" t="s">
         <v>314</v>
       </c>
@@ -8085,7 +8063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="399" spans="1:3">
       <c r="A399" s="1" t="s">
         <v>315</v>
       </c>
@@ -8096,7 +8074,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="400" spans="1:3">
       <c r="A400" s="1" t="s">
         <v>316</v>
       </c>
@@ -8107,7 +8085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="401" spans="1:3">
       <c r="A401" s="1" t="s">
         <v>840</v>
       </c>
@@ -8118,7 +8096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="402" spans="1:3">
       <c r="A402" s="1" t="s">
         <v>924</v>
       </c>
@@ -8129,7 +8107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="403" spans="1:3">
       <c r="A403" s="1" t="s">
         <v>731</v>
       </c>
@@ -8140,7 +8118,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="404" spans="1:3">
       <c r="A404" s="1" t="s">
         <v>770</v>
       </c>
@@ -8151,7 +8129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="405" spans="1:3">
       <c r="A405" s="1" t="s">
         <v>317</v>
       </c>
@@ -8162,7 +8140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="406" spans="1:3">
       <c r="A406" s="1" t="s">
         <v>732</v>
       </c>
@@ -8173,7 +8151,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="407" spans="1:3">
       <c r="A407" s="1" t="s">
         <v>735</v>
       </c>
@@ -8184,7 +8162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="408" spans="1:3">
       <c r="A408" s="1" t="s">
         <v>318</v>
       </c>
@@ -8195,7 +8173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="409" spans="1:3">
       <c r="A409" s="1" t="s">
         <v>319</v>
       </c>
@@ -8206,7 +8184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="410" spans="1:3">
       <c r="A410" s="1" t="s">
         <v>320</v>
       </c>
@@ -8217,7 +8195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="411" spans="1:3">
       <c r="A411" s="1" t="s">
         <v>321</v>
       </c>
@@ -8228,7 +8206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="412" spans="1:3">
       <c r="A412" s="1" t="s">
         <v>322</v>
       </c>
@@ -8239,7 +8217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="413" spans="1:3">
       <c r="A413" s="1" t="s">
         <v>323</v>
       </c>
@@ -8250,7 +8228,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="414" spans="1:3">
       <c r="A414" s="1" t="s">
         <v>324</v>
       </c>
@@ -8261,7 +8239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="415" spans="1:3">
       <c r="A415" s="1" t="s">
         <v>814</v>
       </c>
@@ -8272,7 +8250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="416" spans="1:3">
       <c r="A416" s="1" t="s">
         <v>641</v>
       </c>
@@ -8283,7 +8261,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="417" spans="1:3">
       <c r="A417" s="1" t="s">
         <v>325</v>
       </c>
@@ -8294,7 +8272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="418" spans="1:3">
       <c r="A418" s="1" t="s">
         <v>929</v>
       </c>
@@ -8305,7 +8283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="419" spans="1:3">
       <c r="A419" s="1" t="s">
         <v>326</v>
       </c>
@@ -8316,7 +8294,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="420" spans="1:3">
       <c r="A420" s="1" t="s">
         <v>327</v>
       </c>
@@ -8327,7 +8305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="421" spans="1:3">
       <c r="A421" s="1" t="s">
         <v>328</v>
       </c>
@@ -8338,7 +8316,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="422" spans="1:3">
       <c r="A422" s="1" t="s">
         <v>329</v>
       </c>
@@ -8349,7 +8327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="423" spans="1:3">
       <c r="A423" s="1" t="s">
         <v>330</v>
       </c>
@@ -8360,7 +8338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="424" spans="1:3">
       <c r="A424" s="1" t="s">
         <v>331</v>
       </c>
@@ -8371,7 +8349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="425" spans="1:3">
       <c r="A425" s="1" t="s">
         <v>332</v>
       </c>
@@ -8382,7 +8360,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="426" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="426" spans="1:3">
       <c r="A426" s="1" t="s">
         <v>333</v>
       </c>
@@ -8393,7 +8371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="427" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="427" spans="1:3">
       <c r="A427" s="1" t="s">
         <v>334</v>
       </c>
@@ -8404,7 +8382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="428" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="428" spans="1:3">
       <c r="A428" s="1" t="s">
         <v>810</v>
       </c>
@@ -8415,7 +8393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="429" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="429" spans="1:3">
       <c r="A429" s="1" t="s">
         <v>335</v>
       </c>
@@ -8426,7 +8404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="430" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="430" spans="1:3">
       <c r="A430" s="1" t="s">
         <v>828</v>
       </c>
@@ -8437,7 +8415,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="431" spans="1:3">
       <c r="A431" s="1" t="s">
         <v>718</v>
       </c>
@@ -8448,7 +8426,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="432" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="432" spans="1:3">
       <c r="A432" s="1" t="s">
         <v>629</v>
       </c>
@@ -8459,7 +8437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="433" spans="1:3">
       <c r="A433" s="1" t="s">
         <v>336</v>
       </c>
@@ -8470,7 +8448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="434" spans="1:3">
       <c r="A434" s="1" t="s">
         <v>853</v>
       </c>
@@ -8481,7 +8459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="435" spans="1:3">
       <c r="A435" s="1" t="s">
         <v>599</v>
       </c>
@@ -8492,7 +8470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="436" spans="1:3">
       <c r="A436" s="1" t="s">
         <v>337</v>
       </c>
@@ -8503,7 +8481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="437" spans="1:3">
       <c r="A437" s="1" t="s">
         <v>338</v>
       </c>
@@ -8514,7 +8492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="438" spans="1:3">
       <c r="A438" s="1" t="s">
         <v>722</v>
       </c>
@@ -8525,7 +8503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="439" spans="1:3">
       <c r="A439" s="1" t="s">
         <v>915</v>
       </c>
@@ -8536,7 +8514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="440" spans="1:3">
       <c r="A440" s="1" t="s">
         <v>723</v>
       </c>
@@ -8547,7 +8525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="441" spans="1:3">
       <c r="A441" s="1" t="s">
         <v>801</v>
       </c>
@@ -8558,7 +8536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="442" spans="1:3">
       <c r="A442" s="1" t="s">
         <v>784</v>
       </c>
@@ -8569,7 +8547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="443" spans="1:3">
       <c r="A443" s="1" t="s">
         <v>339</v>
       </c>
@@ -8580,7 +8558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="444" spans="1:3">
       <c r="A444" s="1" t="s">
         <v>842</v>
       </c>
@@ -8591,7 +8569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="445" spans="1:3">
       <c r="A445" s="1" t="s">
         <v>340</v>
       </c>
@@ -8602,7 +8580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="446" spans="1:3">
       <c r="A446" s="1" t="s">
         <v>341</v>
       </c>
@@ -8613,7 +8591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="447" spans="1:3">
       <c r="A447" s="1" t="s">
         <v>342</v>
       </c>
@@ -8624,7 +8602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="448" spans="1:3">
       <c r="A448" s="1" t="s">
         <v>645</v>
       </c>
@@ -8635,7 +8613,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="449" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="449" spans="1:3">
       <c r="A449" s="1" t="s">
         <v>343</v>
       </c>
@@ -8646,7 +8624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="450" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="450" spans="1:3">
       <c r="A450" s="1" t="s">
         <v>963</v>
       </c>
@@ -8657,7 +8635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="451" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="451" spans="1:3">
       <c r="A451" s="1" t="s">
         <v>344</v>
       </c>
@@ -8668,7 +8646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="452" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="452" spans="1:3">
       <c r="A452" s="1" t="s">
         <v>345</v>
       </c>
@@ -8679,7 +8657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="453" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="453" spans="1:3">
       <c r="A453" s="1" t="s">
         <v>346</v>
       </c>
@@ -8690,7 +8668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="454" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="454" spans="1:3">
       <c r="A454" s="1" t="s">
         <v>347</v>
       </c>
@@ -8701,7 +8679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="455" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="455" spans="1:3">
       <c r="A455" s="1" t="s">
         <v>348</v>
       </c>
@@ -8712,7 +8690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="456" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="456" spans="1:3">
       <c r="A456" s="1" t="s">
         <v>349</v>
       </c>
@@ -8723,7 +8701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="457" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="457" spans="1:3">
       <c r="A457" s="1" t="s">
         <v>350</v>
       </c>
@@ -8734,7 +8712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="458" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="458" spans="1:3">
       <c r="A458" s="1" t="s">
         <v>857</v>
       </c>
@@ -8745,7 +8723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="459" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="459" spans="1:3">
       <c r="A459" s="1" t="s">
         <v>684</v>
       </c>
@@ -8756,7 +8734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="460" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="460" spans="1:3">
       <c r="A460" s="1" t="s">
         <v>687</v>
       </c>
@@ -8767,7 +8745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="461" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="461" spans="1:3">
       <c r="A461" s="1" t="s">
         <v>351</v>
       </c>
@@ -8778,7 +8756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="462" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="462" spans="1:3">
       <c r="A462" s="1" t="s">
         <v>352</v>
       </c>
@@ -8789,7 +8767,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="463" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="463" spans="1:3">
       <c r="A463" s="1" t="s">
         <v>950</v>
       </c>
@@ -8800,7 +8778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="464" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="464" spans="1:3">
       <c r="A464" s="1" t="s">
         <v>353</v>
       </c>
@@ -8811,7 +8789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="465" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="465" spans="1:3">
       <c r="A465" s="1" t="s">
         <v>676</v>
       </c>
@@ -8822,7 +8800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="466" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="466" spans="1:3">
       <c r="A466" s="1" t="s">
         <v>821</v>
       </c>
@@ -8833,7 +8811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="467" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="467" spans="1:3">
       <c r="A467" s="1" t="s">
         <v>354</v>
       </c>
@@ -8844,7 +8822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="468" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="468" spans="1:3">
       <c r="A468" s="1" t="s">
         <v>674</v>
       </c>
@@ -8855,7 +8833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="469" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="469" spans="1:3">
       <c r="A469" s="1" t="s">
         <v>778</v>
       </c>
@@ -8866,7 +8844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="470" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="470" spans="1:3">
       <c r="A470" s="1" t="s">
         <v>355</v>
       </c>
@@ -8877,7 +8855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="471" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="471" spans="1:3">
       <c r="A471" s="1" t="s">
         <v>356</v>
       </c>
@@ -8888,7 +8866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="472" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="472" spans="1:3">
       <c r="A472" s="1" t="s">
         <v>720</v>
       </c>
@@ -8899,7 +8877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="473" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="473" spans="1:3">
       <c r="A473" s="1" t="s">
         <v>358</v>
       </c>
@@ -8910,7 +8888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="474" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="474" spans="1:3">
       <c r="A474" s="1" t="s">
         <v>357</v>
       </c>
@@ -8921,7 +8899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="475" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="475" spans="1:3">
       <c r="A475" s="1" t="s">
         <v>961</v>
       </c>
@@ -8932,7 +8910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="476" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="476" spans="1:3">
       <c r="A476" s="1" t="s">
         <v>359</v>
       </c>
@@ -8943,7 +8921,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="477" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="477" spans="1:3">
       <c r="A477" s="1" t="s">
         <v>690</v>
       </c>
@@ -8954,7 +8932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="478" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="478" spans="1:3">
       <c r="A478" s="1" t="s">
         <v>360</v>
       </c>
@@ -8965,7 +8943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="479" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="479" spans="1:3">
       <c r="A479" s="1" t="s">
         <v>361</v>
       </c>
@@ -8976,7 +8954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="480" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="480" spans="1:3">
       <c r="A480" s="1" t="s">
         <v>143</v>
       </c>
@@ -8987,7 +8965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="481" spans="1:3">
       <c r="A481" s="1" t="s">
         <v>969</v>
       </c>
@@ -8998,7 +8976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="482" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="482" spans="1:3">
       <c r="A482" s="1" t="s">
         <v>362</v>
       </c>
@@ -9009,7 +8987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="483" spans="1:3">
       <c r="A483" s="1" t="s">
         <v>609</v>
       </c>
@@ -9020,7 +8998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="484" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="484" spans="1:3">
       <c r="A484" s="1" t="s">
         <v>363</v>
       </c>
@@ -9031,7 +9009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="485" spans="1:3">
       <c r="A485" s="1" t="s">
         <v>643</v>
       </c>
@@ -9042,7 +9020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="486" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="486" spans="1:3">
       <c r="A486" s="1" t="s">
         <v>364</v>
       </c>
@@ -9053,7 +9031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="487" spans="1:3">
       <c r="A487" s="1" t="s">
         <v>365</v>
       </c>
@@ -9064,7 +9042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="488" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="488" spans="1:3">
       <c r="A488" s="1" t="s">
         <v>366</v>
       </c>
@@ -9075,7 +9053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="489" spans="1:3">
       <c r="A489" s="1" t="s">
         <v>826</v>
       </c>
@@ -9086,7 +9064,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="490" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="490" spans="1:3">
       <c r="A490" s="1" t="s">
         <v>368</v>
       </c>
@@ -9097,7 +9075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="491" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="491" spans="1:3">
       <c r="A491" s="1" t="s">
         <v>367</v>
       </c>
@@ -9108,7 +9086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="492" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="492" spans="1:3">
       <c r="A492" s="1" t="s">
         <v>369</v>
       </c>
@@ -9119,7 +9097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="493" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="493" spans="1:3">
       <c r="A493" s="1" t="s">
         <v>370</v>
       </c>
@@ -9130,7 +9108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="494" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="494" spans="1:3">
       <c r="A494" s="1" t="s">
         <v>371</v>
       </c>
@@ -9141,7 +9119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="495" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="495" spans="1:3">
       <c r="A495" s="1" t="s">
         <v>372</v>
       </c>
@@ -9152,7 +9130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="496" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="496" spans="1:3">
       <c r="A496" s="1" t="s">
         <v>838</v>
       </c>
@@ -9163,7 +9141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="497" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="497" spans="1:3">
       <c r="A497" s="1" t="s">
         <v>373</v>
       </c>
@@ -9174,7 +9152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="498" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="498" spans="1:3">
       <c r="A498" s="1" t="s">
         <v>832</v>
       </c>
@@ -9185,7 +9163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="499" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="499" spans="1:3">
       <c r="A499" s="1" t="s">
         <v>145</v>
       </c>
@@ -9196,7 +9174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="500" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="500" spans="1:3">
       <c r="A500" s="1" t="s">
         <v>147</v>
       </c>
@@ -9207,7 +9185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="501" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="501" spans="1:3">
       <c r="A501" s="1" t="s">
         <v>792</v>
       </c>
@@ -9218,7 +9196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="502" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="502" spans="1:3">
       <c r="A502" s="1" t="s">
         <v>1007</v>
       </c>
@@ -9229,7 +9207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="503" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="503" spans="1:3">
       <c r="A503" s="1" t="s">
         <v>1009</v>
       </c>
@@ -9240,7 +9218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="504" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="504" spans="1:3">
       <c r="A504" s="1" t="s">
         <v>1010</v>
       </c>
@@ -9251,7 +9229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="505" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="505" spans="1:3">
       <c r="A505" s="1" t="s">
         <v>1013</v>
       </c>
@@ -9262,7 +9240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="506" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="506" spans="1:3">
       <c r="A506" s="1" t="s">
         <v>1015</v>
       </c>
@@ -9273,7 +9251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="507" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="507" spans="1:3">
       <c r="A507" s="1" t="s">
         <v>1017</v>
       </c>
@@ -9284,7 +9262,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="508" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="508" spans="1:3">
       <c r="A508" s="1" t="s">
         <v>1019</v>
       </c>
@@ -9295,7 +9273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="509" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="509" spans="1:3">
       <c r="A509" s="1" t="s">
         <v>1021</v>
       </c>
@@ -9306,7 +9284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="510" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="510" spans="1:3">
       <c r="A510" s="1" t="s">
         <v>1023</v>
       </c>
@@ -9317,7 +9295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="511" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="511" spans="1:3">
       <c r="A511" s="1" t="s">
         <v>1025</v>
       </c>
@@ -9328,7 +9306,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="512" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="512" spans="1:3">
       <c r="A512" s="1" t="s">
         <v>1027</v>
       </c>
@@ -9339,7 +9317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="513" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="513" spans="1:3">
       <c r="A513" s="1" t="s">
         <v>1029</v>
       </c>
@@ -9350,7 +9328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="514" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="514" spans="1:3">
       <c r="A514" s="1" t="s">
         <v>1031</v>
       </c>
@@ -9361,7 +9339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="515" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="515" spans="1:3">
       <c r="A515" s="1" t="s">
         <v>1033</v>
       </c>
@@ -9372,7 +9350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="516" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="516" spans="1:3">
       <c r="A516" s="1" t="s">
         <v>1035</v>
       </c>
@@ -9383,7 +9361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="517" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="517" spans="1:3">
       <c r="A517" s="1" t="s">
         <v>1037</v>
       </c>
@@ -9394,7 +9372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="518" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="518" spans="1:3">
       <c r="A518" s="1" t="s">
         <v>1039</v>
       </c>
@@ -9405,7 +9383,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="519" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="519" spans="1:3">
       <c r="A519" s="1" t="s">
         <v>1041</v>
       </c>
@@ -9416,7 +9394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="520" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="520" spans="1:3">
       <c r="A520" s="1" t="s">
         <v>1043</v>
       </c>
@@ -9427,7 +9405,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="521" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="521" spans="1:3">
       <c r="A521" s="1" t="s">
         <v>1045</v>
       </c>
@@ -9438,7 +9416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="522" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="522" spans="1:3">
       <c r="A522" s="1" t="s">
         <v>1047</v>
       </c>
@@ -9449,7 +9427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="523" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="523" spans="1:3">
       <c r="A523" s="1" t="s">
         <v>1049</v>
       </c>
@@ -9460,7 +9438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="524" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="524" spans="1:3">
       <c r="A524" s="1" t="s">
         <v>1051</v>
       </c>
@@ -9471,7 +9449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="525" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="525" spans="1:3">
       <c r="A525" s="1" t="s">
         <v>1053</v>
       </c>
@@ -9482,7 +9460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="526" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="526" spans="1:3">
       <c r="A526" s="1" t="s">
         <v>1069</v>
       </c>
@@ -9493,7 +9471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="527" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="527" spans="1:3">
       <c r="A527" s="1" t="s">
         <v>1056</v>
       </c>
@@ -9504,7 +9482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="528" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="528" spans="1:3">
       <c r="A528" s="1" t="s">
         <v>1058</v>
       </c>
@@ -9515,7 +9493,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="529" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="529" spans="1:3">
       <c r="A529" s="1" t="s">
         <v>1060</v>
       </c>
@@ -9526,7 +9504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="530" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="530" spans="1:3">
       <c r="A530" s="1" t="s">
         <v>1062</v>
       </c>
@@ -9537,7 +9515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="531" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="531" spans="1:3">
       <c r="A531" s="1" t="s">
         <v>1064</v>
       </c>
@@ -9548,7 +9526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="532" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="532" spans="1:3">
       <c r="A532" s="1" t="s">
         <v>1066</v>
       </c>
@@ -9559,7 +9537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="533" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="533" spans="1:3">
       <c r="A533" s="1" t="s">
         <v>1068</v>
       </c>
@@ -9570,7 +9548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="534" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="534" spans="1:3">
       <c r="A534" s="1" t="s">
         <v>1071</v>
       </c>
@@ -9578,6 +9556,28 @@
         <v>1072</v>
       </c>
       <c r="C534" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="535" spans="1:3">
+      <c r="A535" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B535" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C535" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="536" spans="1:3">
+      <c r="A536" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B536" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C536" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update navigation add media data
</commit_message>
<xml_diff>
--- a/data/media.xlsx
+++ b/data/media.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7308"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="1117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="1133">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3418,6 +3418,54 @@
   </si>
   <si>
     <t>tt3967856</t>
+  </si>
+  <si>
+    <t>Wonder Woman</t>
+  </si>
+  <si>
+    <t>tt0451279</t>
+  </si>
+  <si>
+    <t>Alien: Covenant</t>
+  </si>
+  <si>
+    <t>tt2316204</t>
+  </si>
+  <si>
+    <t>My Bromance</t>
+  </si>
+  <si>
+    <t>tt3522738</t>
+  </si>
+  <si>
+    <t>Ghost In The Shell</t>
+  </si>
+  <si>
+    <t>tt1219827</t>
+  </si>
+  <si>
+    <t>Red Wine in the Dark Night</t>
+  </si>
+  <si>
+    <t>tt4556730</t>
+  </si>
+  <si>
+    <t>The Mummy</t>
+  </si>
+  <si>
+    <t>tt2345759</t>
+  </si>
+  <si>
+    <t>How to Win at Checkers (Every Time)</t>
+  </si>
+  <si>
+    <t>tt4370256</t>
+  </si>
+  <si>
+    <t>Pink Moon</t>
+  </si>
+  <si>
+    <t>tt3775450</t>
   </si>
 </sst>
 </file>
@@ -3828,10 +3876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D557"/>
+  <dimension ref="A1:D565"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A538" workbookViewId="0">
-      <selection activeCell="C556" sqref="C556:C557"/>
+    <sheetView tabSelected="1" topLeftCell="A544" workbookViewId="0">
+      <selection activeCell="C564" sqref="C564:C565"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9795,7 +9843,7 @@
       <c r="A542" s="1" t="s">
         <v>1085</v>
       </c>
-      <c r="B542" s="4" t="s">
+      <c r="B542" s="1" t="s">
         <v>1084</v>
       </c>
       <c r="C542" s="1" t="s">
@@ -9957,13 +10005,101 @@
       </c>
     </row>
     <row r="557" spans="1:3">
-      <c r="A557" s="4" t="s">
+      <c r="A557" s="1" t="s">
         <v>1115</v>
       </c>
       <c r="B557" s="1" t="s">
         <v>1116</v>
       </c>
       <c r="C557" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="558" spans="1:3">
+      <c r="A558" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C558" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="559" spans="1:3">
+      <c r="A559" s="1" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C559" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="560" spans="1:3">
+      <c r="A560" s="1" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C560" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="561" spans="1:3">
+      <c r="A561" s="1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B561" s="1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C561" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="562" spans="1:3">
+      <c r="A562" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B562" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C562" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="563" spans="1:3">
+      <c r="A563" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C563" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="564" spans="1:3">
+      <c r="A564" s="1" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B564" s="1" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C564" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3">
+      <c r="A565" s="1" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C565" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update bible DOM structure
</commit_message>
<xml_diff>
--- a/data/media.xlsx
+++ b/data/media.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7308"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="1157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="1161">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3538,6 +3538,18 @@
   </si>
   <si>
     <t>tt4613254</t>
+  </si>
+  <si>
+    <t>Spider-Man Homecoming</t>
+  </si>
+  <si>
+    <t>tt2250912</t>
+  </si>
+  <si>
+    <t>War for the Planet of the Apes</t>
+  </si>
+  <si>
+    <t>tt3450958</t>
   </si>
 </sst>
 </file>
@@ -3948,10 +3960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D577"/>
+  <dimension ref="A1:D579"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A553" workbookViewId="0">
-      <selection activeCell="C575" sqref="C575:C577"/>
+    <sheetView tabSelected="1" topLeftCell="A568" workbookViewId="0">
+      <selection activeCell="C577" sqref="C577:C579"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10307,6 +10319,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="578" spans="1:3">
+      <c r="A578" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B578" s="1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C578" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="579" spans="1:3">
+      <c r="A579" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B579" s="1" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C579" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix bug Add media data
</commit_message>
<xml_diff>
--- a/data/media.xlsx
+++ b/data/media.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7308" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7308"/>
   </bookViews>
   <sheets>
     <sheet name="media" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="1279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="1283">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3898,6 +3898,18 @@
   </si>
   <si>
     <t>The Silence of the Lambs</t>
+  </si>
+  <si>
+    <t>Paddington 2</t>
+  </si>
+  <si>
+    <t>tt4468740</t>
+  </si>
+  <si>
+    <t>Jumanji Welcome to the Jungle</t>
+  </si>
+  <si>
+    <t>tt2283362</t>
   </si>
 </sst>
 </file>
@@ -4321,10 +4333,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C522"/>
+  <dimension ref="A1:C524"/>
   <sheetViews>
-    <sheetView topLeftCell="A499" workbookViewId="0">
-      <selection activeCell="C511" sqref="C511:C522"/>
+    <sheetView tabSelected="1" topLeftCell="A505" workbookViewId="0">
+      <selection activeCell="C521" sqref="C521:C523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10072,6 +10084,28 @@
         <v>4</v>
       </c>
     </row>
+    <row r="523" spans="1:3">
+      <c r="A523" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C523" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="524" spans="1:3">
+      <c r="A524" s="4" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B524" s="1" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C524" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -10085,8 +10119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C597"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119:C120"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121:XFD121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Fix loading media issue.
</commit_message>
<xml_diff>
--- a/data/media.xlsx
+++ b/data/media.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F58D6632-B7DF-415E-9037-8713859AEAEB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1E1128CC-6B6F-488D-810B-BEB7C9632FCC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2041" uniqueCount="1359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="1359">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4214,9 +4214,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table22" displayName="Table22" ref="A1:C1048475" totalsRowShown="0">
-  <sortState ref="A2:C418">
-    <sortCondition ref="A1:A1048475"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table22" displayName="Table22" ref="A1:C1048473" totalsRowShown="0">
+  <sortState ref="A2:C417">
+    <sortCondition ref="A1:A1048473"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Title"/>
@@ -4562,10 +4562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C544"/>
+  <dimension ref="A1:C542"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A519" workbookViewId="0">
-      <selection activeCell="C538" sqref="C538:C544"/>
+    <sheetView tabSelected="1" topLeftCell="A432" workbookViewId="0">
+      <selection activeCell="A448" sqref="A448:XFD448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6471,10 +6471,10 @@
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>4</v>
@@ -6482,10 +6482,10 @@
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>4</v>
@@ -6493,10 +6493,10 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>4</v>
@@ -6504,10 +6504,10 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>4</v>
@@ -6515,10 +6515,10 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>4</v>
@@ -6526,10 +6526,10 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>4</v>
@@ -6537,10 +6537,10 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>4</v>
@@ -6548,10 +6548,10 @@
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="1" t="s">
-        <v>212</v>
+        <v>845</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>436</v>
+        <v>843</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>4</v>
@@ -6559,10 +6559,10 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="1" t="s">
-        <v>845</v>
+        <v>646</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>843</v>
+        <v>647</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>4</v>
@@ -6570,10 +6570,10 @@
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="1" t="s">
-        <v>646</v>
+        <v>767</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>647</v>
+        <v>768</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>4</v>
@@ -6581,10 +6581,10 @@
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="1" t="s">
-        <v>767</v>
+        <v>894</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>768</v>
+        <v>895</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>4</v>
@@ -6592,10 +6592,10 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="1" t="s">
-        <v>894</v>
+        <v>678</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>895</v>
+        <v>679</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>4</v>
@@ -6603,10 +6603,10 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="1" t="s">
-        <v>678</v>
+        <v>930</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>679</v>
+        <v>929</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>4</v>
@@ -6614,10 +6614,10 @@
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="1" t="s">
-        <v>930</v>
+        <v>997</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>929</v>
+        <v>998</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>4</v>
@@ -6625,10 +6625,10 @@
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="1" t="s">
-        <v>997</v>
+        <v>688</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>998</v>
+        <v>689</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>4</v>
@@ -6636,10 +6636,10 @@
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="1" t="s">
-        <v>688</v>
+        <v>620</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>689</v>
+        <v>621</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>4</v>
@@ -6647,10 +6647,10 @@
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="1" t="s">
-        <v>620</v>
+        <v>217</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>621</v>
+        <v>441</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>4</v>
@@ -6658,10 +6658,10 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>4</v>
@@ -6669,10 +6669,10 @@
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="1" t="s">
-        <v>218</v>
+        <v>945</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>442</v>
+        <v>946</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>4</v>
@@ -6680,10 +6680,10 @@
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="1" t="s">
-        <v>945</v>
+        <v>878</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>946</v>
+        <v>879</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>4</v>
@@ -6691,10 +6691,10 @@
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="1" t="s">
-        <v>878</v>
+        <v>219</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>879</v>
+        <v>443</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>4</v>
@@ -6702,10 +6702,10 @@
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>4</v>
@@ -6713,10 +6713,10 @@
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>4</v>
@@ -6724,10 +6724,10 @@
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>4</v>
@@ -6735,10 +6735,10 @@
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>4</v>
@@ -6746,10 +6746,10 @@
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>4</v>
@@ -6757,10 +6757,10 @@
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>4</v>
@@ -6768,10 +6768,10 @@
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>451</v>
+        <v>228</v>
+      </c>
+      <c r="B200" s="4" t="s">
+        <v>452</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>4</v>
@@ -6779,10 +6779,10 @@
     </row>
     <row r="201" spans="1:3">
       <c r="A201" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B201" s="4" t="s">
-        <v>452</v>
+        <v>229</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>453</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>4</v>
@@ -6790,10 +6790,10 @@
     </row>
     <row r="202" spans="1:3">
       <c r="A202" s="1" t="s">
-        <v>229</v>
+        <v>692</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>453</v>
+        <v>693</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>4</v>
@@ -6801,10 +6801,10 @@
     </row>
     <row r="203" spans="1:3">
       <c r="A203" s="1" t="s">
-        <v>692</v>
+        <v>910</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>693</v>
+        <v>911</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>4</v>
@@ -6812,10 +6812,10 @@
     </row>
     <row r="204" spans="1:3">
       <c r="A204" s="1" t="s">
-        <v>910</v>
+        <v>837</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>911</v>
+        <v>838</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>4</v>
@@ -6823,10 +6823,10 @@
     </row>
     <row r="205" spans="1:3">
       <c r="A205" s="1" t="s">
-        <v>837</v>
+        <v>700</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>838</v>
+        <v>701</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>4</v>
@@ -6834,10 +6834,10 @@
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="1" t="s">
-        <v>700</v>
+        <v>230</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>701</v>
+        <v>454</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>4</v>
@@ -6845,10 +6845,10 @@
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>4</v>
@@ -6856,10 +6856,10 @@
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>4</v>
@@ -6867,10 +6867,10 @@
     </row>
     <row r="209" spans="1:3">
       <c r="A209" s="1" t="s">
-        <v>231</v>
+        <v>749</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>455</v>
+        <v>750</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>4</v>
@@ -6878,10 +6878,10 @@
     </row>
     <row r="210" spans="1:3">
       <c r="A210" s="1" t="s">
-        <v>749</v>
+        <v>852</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>750</v>
+        <v>853</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>4</v>
@@ -6889,10 +6889,10 @@
     </row>
     <row r="211" spans="1:3">
       <c r="A211" s="1" t="s">
-        <v>852</v>
+        <v>234</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>853</v>
+        <v>458</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>4</v>
@@ -6900,10 +6900,10 @@
     </row>
     <row r="212" spans="1:3">
       <c r="A212" s="1" t="s">
-        <v>234</v>
+        <v>883</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>458</v>
+        <v>884</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>4</v>
@@ -6911,10 +6911,10 @@
     </row>
     <row r="213" spans="1:3">
       <c r="A213" s="1" t="s">
-        <v>883</v>
+        <v>235</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>884</v>
+        <v>459</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>4</v>
@@ -6922,10 +6922,10 @@
     </row>
     <row r="214" spans="1:3">
       <c r="A214" s="1" t="s">
-        <v>235</v>
+        <v>801</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>459</v>
+        <v>802</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>4</v>
@@ -6933,10 +6933,10 @@
     </row>
     <row r="215" spans="1:3">
       <c r="A215" s="1" t="s">
-        <v>801</v>
+        <v>904</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>802</v>
+        <v>905</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>4</v>
@@ -6944,10 +6944,10 @@
     </row>
     <row r="216" spans="1:3">
       <c r="A216" s="1" t="s">
-        <v>904</v>
+        <v>236</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>905</v>
+        <v>460</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>4</v>
@@ -6955,10 +6955,10 @@
     </row>
     <row r="217" spans="1:3">
       <c r="A217" s="1" t="s">
-        <v>236</v>
+        <v>666</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>460</v>
+        <v>667</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>4</v>
@@ -6966,10 +6966,10 @@
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="1" t="s">
-        <v>666</v>
+        <v>634</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>667</v>
+        <v>635</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>4</v>
@@ -6977,10 +6977,10 @@
     </row>
     <row r="219" spans="1:3">
       <c r="A219" s="1" t="s">
-        <v>634</v>
+        <v>237</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>635</v>
+        <v>461</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>4</v>
@@ -6988,10 +6988,10 @@
     </row>
     <row r="220" spans="1:3">
       <c r="A220" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>4</v>
@@ -6999,10 +6999,10 @@
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>4</v>
@@ -7010,10 +7010,7 @@
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>463</v>
+        <v>240</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>4</v>
@@ -7021,7 +7018,10 @@
     </row>
     <row r="223" spans="1:3">
       <c r="A223" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>465</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>4</v>
@@ -7029,10 +7029,10 @@
     </row>
     <row r="224" spans="1:3">
       <c r="A224" s="1" t="s">
-        <v>242</v>
+        <v>702</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>465</v>
+        <v>703</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>4</v>
@@ -7040,10 +7040,10 @@
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="1" t="s">
-        <v>702</v>
+        <v>663</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>703</v>
+        <v>662</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>4</v>
@@ -7051,10 +7051,10 @@
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="1" t="s">
-        <v>663</v>
+        <v>244</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>662</v>
+        <v>467</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>4</v>
@@ -7062,10 +7062,10 @@
     </row>
     <row r="227" spans="1:3">
       <c r="A227" s="1" t="s">
-        <v>244</v>
+        <v>761</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>467</v>
+        <v>762</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>4</v>
@@ -7073,10 +7073,10 @@
     </row>
     <row r="228" spans="1:3">
       <c r="A228" s="1" t="s">
-        <v>761</v>
+        <v>823</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>762</v>
+        <v>824</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>4</v>
@@ -7084,10 +7084,10 @@
     </row>
     <row r="229" spans="1:3">
       <c r="A229" s="1" t="s">
-        <v>823</v>
+        <v>783</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>824</v>
+        <v>784</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>4</v>
@@ -7095,10 +7095,10 @@
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="1" t="s">
-        <v>783</v>
+        <v>246</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>784</v>
+        <v>469</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>4</v>
@@ -7106,10 +7106,10 @@
     </row>
     <row r="231" spans="1:3">
       <c r="A231" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>4</v>
@@ -7117,10 +7117,10 @@
     </row>
     <row r="232" spans="1:3">
       <c r="A232" s="1" t="s">
-        <v>247</v>
+        <v>892</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>470</v>
+        <v>893</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>4</v>
@@ -7128,10 +7128,10 @@
     </row>
     <row r="233" spans="1:3">
       <c r="A233" s="1" t="s">
-        <v>892</v>
+        <v>248</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>893</v>
+        <v>471</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>4</v>
@@ -7139,10 +7139,10 @@
     </row>
     <row r="234" spans="1:3">
       <c r="A234" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>4</v>
@@ -7150,10 +7150,10 @@
     </row>
     <row r="235" spans="1:3">
       <c r="A235" s="1" t="s">
-        <v>250</v>
+        <v>827</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>473</v>
+        <v>828</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>4</v>
@@ -7161,10 +7161,10 @@
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="1" t="s">
-        <v>827</v>
+        <v>251</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>828</v>
+        <v>474</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>4</v>
@@ -7172,10 +7172,10 @@
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>4</v>
@@ -7183,10 +7183,10 @@
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>4</v>
@@ -7194,10 +7194,10 @@
     </row>
     <row r="239" spans="1:3">
       <c r="A239" s="1" t="s">
-        <v>253</v>
+        <v>605</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>476</v>
+        <v>604</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>4</v>
@@ -7205,10 +7205,10 @@
     </row>
     <row r="240" spans="1:3">
       <c r="A240" s="1" t="s">
-        <v>605</v>
+        <v>900</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>604</v>
+        <v>901</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>4</v>
@@ -7216,10 +7216,10 @@
     </row>
     <row r="241" spans="1:3">
       <c r="A241" s="1" t="s">
-        <v>900</v>
+        <v>255</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>901</v>
+        <v>478</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>4</v>
@@ -7227,32 +7227,32 @@
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>4</v>
+        <v>139</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" s="1" t="s">
-        <v>254</v>
+        <v>781</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>477</v>
+        <v>782</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>139</v>
+        <v>4</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" s="1" t="s">
-        <v>781</v>
+        <v>706</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>782</v>
+        <v>707</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>4</v>
@@ -7260,10 +7260,10 @@
     </row>
     <row r="245" spans="1:3">
       <c r="A245" s="1" t="s">
-        <v>706</v>
+        <v>256</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>707</v>
+        <v>479</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>4</v>
@@ -7271,10 +7271,10 @@
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B246" s="1" t="s">
-        <v>479</v>
+        <v>257</v>
+      </c>
+      <c r="B246" s="4" t="s">
+        <v>480</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>4</v>
@@ -7282,10 +7282,10 @@
     </row>
     <row r="247" spans="1:3">
       <c r="A247" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B247" s="4" t="s">
-        <v>480</v>
+        <v>259</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>482</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>4</v>
@@ -7293,10 +7293,10 @@
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="1" t="s">
-        <v>259</v>
+        <v>735</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>482</v>
+        <v>736</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>4</v>
@@ -7304,10 +7304,10 @@
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="1" t="s">
-        <v>735</v>
+        <v>260</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>736</v>
+        <v>483</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>4</v>
@@ -7315,10 +7315,10 @@
     </row>
     <row r="250" spans="1:3">
       <c r="A250" s="1" t="s">
-        <v>260</v>
+        <v>992</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>483</v>
+        <v>993</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>4</v>
@@ -7326,10 +7326,10 @@
     </row>
     <row r="251" spans="1:3">
       <c r="A251" s="1" t="s">
-        <v>992</v>
+        <v>258</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>993</v>
+        <v>481</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>4</v>
@@ -7337,10 +7337,10 @@
     </row>
     <row r="252" spans="1:3">
       <c r="A252" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>4</v>
@@ -7348,10 +7348,10 @@
     </row>
     <row r="253" spans="1:3">
       <c r="A253" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>4</v>
@@ -7359,10 +7359,10 @@
     </row>
     <row r="254" spans="1:3">
       <c r="A254" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>4</v>
@@ -7370,10 +7370,10 @@
     </row>
     <row r="255" spans="1:3">
       <c r="A255" s="1" t="s">
-        <v>264</v>
+        <v>898</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>487</v>
+        <v>899</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>4</v>
@@ -7381,10 +7381,10 @@
     </row>
     <row r="256" spans="1:3">
       <c r="A256" s="1" t="s">
-        <v>898</v>
+        <v>265</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>899</v>
+        <v>488</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>4</v>
@@ -7392,10 +7392,10 @@
     </row>
     <row r="257" spans="1:3">
       <c r="A257" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>4</v>
@@ -7403,10 +7403,10 @@
     </row>
     <row r="258" spans="1:3">
       <c r="A258" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>4</v>
@@ -7414,10 +7414,10 @@
     </row>
     <row r="259" spans="1:3">
       <c r="A259" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>4</v>
@@ -7425,10 +7425,10 @@
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>4</v>
@@ -7436,10 +7436,10 @@
     </row>
     <row r="261" spans="1:3">
       <c r="A261" s="1" t="s">
-        <v>269</v>
+        <v>652</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>492</v>
+        <v>653</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>4</v>
@@ -7447,10 +7447,10 @@
     </row>
     <row r="262" spans="1:3">
       <c r="A262" s="1" t="s">
-        <v>652</v>
+        <v>270</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>653</v>
+        <v>493</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>4</v>
@@ -7458,10 +7458,10 @@
     </row>
     <row r="263" spans="1:3">
       <c r="A263" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>4</v>
@@ -7469,10 +7469,10 @@
     </row>
     <row r="264" spans="1:3">
       <c r="A264" s="1" t="s">
-        <v>272</v>
+        <v>741</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>495</v>
+        <v>742</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>4</v>
@@ -7480,10 +7480,10 @@
     </row>
     <row r="265" spans="1:3">
       <c r="A265" s="1" t="s">
-        <v>741</v>
+        <v>273</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>742</v>
+        <v>496</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>4</v>
@@ -7491,10 +7491,10 @@
     </row>
     <row r="266" spans="1:3">
       <c r="A266" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>4</v>
@@ -7502,10 +7502,10 @@
     </row>
     <row r="267" spans="1:3">
       <c r="A267" s="1" t="s">
-        <v>274</v>
+        <v>598</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>497</v>
+        <v>599</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>4</v>
@@ -7513,10 +7513,10 @@
     </row>
     <row r="268" spans="1:3">
       <c r="A268" s="1" t="s">
-        <v>598</v>
+        <v>276</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>599</v>
+        <v>499</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>4</v>
@@ -7524,10 +7524,10 @@
     </row>
     <row r="269" spans="1:3">
       <c r="A269" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>4</v>
@@ -7535,10 +7535,10 @@
     </row>
     <row r="270" spans="1:3">
       <c r="A270" s="1" t="s">
-        <v>277</v>
+        <v>694</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>500</v>
+        <v>695</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>4</v>
@@ -7546,32 +7546,32 @@
     </row>
     <row r="271" spans="1:3">
       <c r="A271" s="1" t="s">
-        <v>694</v>
+        <v>723</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>695</v>
+        <v>722</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>4</v>
+        <v>139</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" s="1" t="s">
-        <v>723</v>
+        <v>278</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>722</v>
+        <v>501</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>139</v>
+        <v>4</v>
       </c>
     </row>
     <row r="273" spans="1:3">
       <c r="A273" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>4</v>
@@ -7579,10 +7579,10 @@
     </row>
     <row r="274" spans="1:3">
       <c r="A274" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>4</v>
@@ -7590,10 +7590,10 @@
     </row>
     <row r="275" spans="1:3">
       <c r="A275" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>4</v>
@@ -7601,10 +7601,10 @@
     </row>
     <row r="276" spans="1:3">
       <c r="A276" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>4</v>
@@ -7612,10 +7612,10 @@
     </row>
     <row r="277" spans="1:3">
       <c r="A277" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>4</v>
@@ -7623,10 +7623,10 @@
     </row>
     <row r="278" spans="1:3">
       <c r="A278" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>4</v>
@@ -7634,10 +7634,10 @@
     </row>
     <row r="279" spans="1:3">
       <c r="A279" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>4</v>
@@ -7645,10 +7645,10 @@
     </row>
     <row r="280" spans="1:3">
       <c r="A280" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>4</v>
@@ -7656,10 +7656,10 @@
     </row>
     <row r="281" spans="1:3">
       <c r="A281" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>4</v>
@@ -7667,10 +7667,10 @@
     </row>
     <row r="282" spans="1:3">
       <c r="A282" s="1" t="s">
-        <v>288</v>
+        <v>733</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>511</v>
+        <v>734</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>4</v>
@@ -7678,10 +7678,10 @@
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="1" t="s">
-        <v>733</v>
+        <v>874</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>734</v>
+        <v>875</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>4</v>
@@ -7689,10 +7689,10 @@
     </row>
     <row r="284" spans="1:3">
       <c r="A284" s="1" t="s">
-        <v>874</v>
+        <v>731</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>875</v>
+        <v>732</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>4</v>
@@ -7700,10 +7700,10 @@
     </row>
     <row r="285" spans="1:3">
       <c r="A285" s="1" t="s">
-        <v>731</v>
+        <v>289</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>732</v>
+        <v>512</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>4</v>
@@ -7711,10 +7711,10 @@
     </row>
     <row r="286" spans="1:3">
       <c r="A286" s="1" t="s">
-        <v>289</v>
+        <v>649</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>512</v>
+        <v>656</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>4</v>
@@ -7722,10 +7722,10 @@
     </row>
     <row r="287" spans="1:3">
       <c r="A287" s="1" t="s">
-        <v>649</v>
+        <v>290</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>656</v>
+        <v>513</v>
       </c>
       <c r="C287" s="1" t="s">
         <v>4</v>
@@ -7733,10 +7733,10 @@
     </row>
     <row r="288" spans="1:3">
       <c r="A288" s="1" t="s">
-        <v>290</v>
+        <v>963</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>513</v>
+        <v>964</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>4</v>
@@ -7744,10 +7744,10 @@
     </row>
     <row r="289" spans="1:3">
       <c r="A289" s="1" t="s">
-        <v>963</v>
+        <v>292</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>964</v>
+        <v>515</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>4</v>
@@ -7755,10 +7755,10 @@
     </row>
     <row r="290" spans="1:3">
       <c r="A290" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>4</v>
@@ -7766,10 +7766,10 @@
     </row>
     <row r="291" spans="1:3">
       <c r="A291" s="1" t="s">
-        <v>293</v>
+        <v>912</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>516</v>
+        <v>913</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>4</v>
@@ -7777,10 +7777,10 @@
     </row>
     <row r="292" spans="1:3">
       <c r="A292" s="1" t="s">
-        <v>912</v>
+        <v>294</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>913</v>
+        <v>517</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>4</v>
@@ -7788,10 +7788,10 @@
     </row>
     <row r="293" spans="1:3">
       <c r="A293" s="1" t="s">
-        <v>294</v>
+        <v>870</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>517</v>
+        <v>871</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>4</v>
@@ -7799,10 +7799,10 @@
     </row>
     <row r="294" spans="1:3">
       <c r="A294" s="1" t="s">
-        <v>870</v>
+        <v>676</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>871</v>
+        <v>677</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>4</v>
@@ -7810,10 +7810,10 @@
     </row>
     <row r="295" spans="1:3">
       <c r="A295" s="1" t="s">
-        <v>676</v>
+        <v>957</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>677</v>
+        <v>958</v>
       </c>
       <c r="C295" s="1" t="s">
         <v>4</v>
@@ -7821,10 +7821,10 @@
     </row>
     <row r="296" spans="1:3">
       <c r="A296" s="1" t="s">
-        <v>957</v>
+        <v>295</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>958</v>
+        <v>518</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>4</v>
@@ -7832,10 +7832,10 @@
     </row>
     <row r="297" spans="1:3">
       <c r="A297" s="1" t="s">
-        <v>295</v>
+        <v>906</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>518</v>
+        <v>907</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>4</v>
@@ -7843,10 +7843,10 @@
     </row>
     <row r="298" spans="1:3">
       <c r="A298" s="1" t="s">
-        <v>906</v>
+        <v>296</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>907</v>
+        <v>519</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>4</v>
@@ -7854,10 +7854,10 @@
     </row>
     <row r="299" spans="1:3">
       <c r="A299" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>4</v>
@@ -7865,10 +7865,10 @@
     </row>
     <row r="300" spans="1:3">
       <c r="A300" s="1" t="s">
-        <v>297</v>
+        <v>896</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>520</v>
+        <v>897</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>4</v>
@@ -7876,10 +7876,10 @@
     </row>
     <row r="301" spans="1:3">
       <c r="A301" s="1" t="s">
-        <v>896</v>
+        <v>829</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>897</v>
+        <v>830</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>4</v>
@@ -7887,10 +7887,10 @@
     </row>
     <row r="302" spans="1:3">
       <c r="A302" s="1" t="s">
-        <v>829</v>
+        <v>862</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>830</v>
+        <v>863</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>4</v>
@@ -7898,10 +7898,7 @@
     </row>
     <row r="303" spans="1:3">
       <c r="A303" s="1" t="s">
-        <v>862</v>
-      </c>
-      <c r="B303" s="1" t="s">
-        <v>863</v>
+        <v>298</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>4</v>
@@ -7909,7 +7906,10 @@
     </row>
     <row r="304" spans="1:3">
       <c r="A304" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>521</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>4</v>
@@ -7917,10 +7917,10 @@
     </row>
     <row r="305" spans="1:3">
       <c r="A305" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>4</v>
@@ -7928,10 +7928,10 @@
     </row>
     <row r="306" spans="1:3">
       <c r="A306" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>4</v>
@@ -7939,10 +7939,10 @@
     </row>
     <row r="307" spans="1:3">
       <c r="A307" s="1" t="s">
-        <v>301</v>
+        <v>839</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>523</v>
+        <v>840</v>
       </c>
       <c r="C307" s="1" t="s">
         <v>4</v>
@@ -7950,10 +7950,10 @@
     </row>
     <row r="308" spans="1:3">
       <c r="A308" s="1" t="s">
-        <v>839</v>
+        <v>302</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>840</v>
+        <v>524</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>4</v>
@@ -7961,10 +7961,10 @@
     </row>
     <row r="309" spans="1:3">
       <c r="A309" s="1" t="s">
-        <v>302</v>
+        <v>622</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>524</v>
+        <v>623</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>4</v>
@@ -7972,10 +7972,10 @@
     </row>
     <row r="310" spans="1:3">
       <c r="A310" s="1" t="s">
-        <v>622</v>
+        <v>636</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>623</v>
+        <v>637</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>4</v>
@@ -7983,10 +7983,10 @@
     </row>
     <row r="311" spans="1:3">
       <c r="A311" s="1" t="s">
-        <v>636</v>
+        <v>674</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>637</v>
+        <v>675</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>4</v>
@@ -7994,10 +7994,10 @@
     </row>
     <row r="312" spans="1:3">
       <c r="A312" s="1" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>4</v>
@@ -8005,10 +8005,10 @@
     </row>
     <row r="313" spans="1:3">
       <c r="A313" s="1" t="s">
-        <v>668</v>
+        <v>303</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>669</v>
+        <v>525</v>
       </c>
       <c r="C313" s="1" t="s">
         <v>4</v>
@@ -8016,10 +8016,10 @@
     </row>
     <row r="314" spans="1:3">
       <c r="A314" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>4</v>
@@ -8027,10 +8027,10 @@
     </row>
     <row r="315" spans="1:3">
       <c r="A315" s="1" t="s">
-        <v>304</v>
+        <v>811</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>526</v>
+        <v>812</v>
       </c>
       <c r="C315" s="1" t="s">
         <v>4</v>
@@ -8038,10 +8038,10 @@
     </row>
     <row r="316" spans="1:3">
       <c r="A316" s="1" t="s">
-        <v>811</v>
+        <v>305</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>812</v>
+        <v>527</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>4</v>
@@ -8049,10 +8049,10 @@
     </row>
     <row r="317" spans="1:3">
       <c r="A317" s="1" t="s">
-        <v>305</v>
+        <v>684</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>527</v>
+        <v>685</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>4</v>
@@ -8060,10 +8060,10 @@
     </row>
     <row r="318" spans="1:3">
       <c r="A318" s="1" t="s">
-        <v>684</v>
+        <v>306</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>685</v>
+        <v>528</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>4</v>
@@ -8071,10 +8071,10 @@
     </row>
     <row r="319" spans="1:3">
       <c r="A319" s="1" t="s">
-        <v>306</v>
+        <v>890</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>528</v>
+        <v>891</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>4</v>
@@ -8082,32 +8082,32 @@
     </row>
     <row r="320" spans="1:3">
       <c r="A320" s="1" t="s">
-        <v>890</v>
+        <v>307</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>891</v>
+        <v>529</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>4</v>
+        <v>139</v>
       </c>
     </row>
     <row r="321" spans="1:3">
       <c r="A321" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>139</v>
+        <v>4</v>
       </c>
     </row>
     <row r="322" spans="1:3">
       <c r="A322" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C322" s="1" t="s">
         <v>4</v>
@@ -8115,10 +8115,10 @@
     </row>
     <row r="323" spans="1:3">
       <c r="A323" s="1" t="s">
-        <v>309</v>
+        <v>791</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>531</v>
+        <v>792</v>
       </c>
       <c r="C323" s="1" t="s">
         <v>4</v>
@@ -8126,10 +8126,10 @@
     </row>
     <row r="324" spans="1:3">
       <c r="A324" s="1" t="s">
-        <v>791</v>
+        <v>310</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>792</v>
+        <v>532</v>
       </c>
       <c r="C324" s="1" t="s">
         <v>4</v>
@@ -8137,10 +8137,10 @@
     </row>
     <row r="325" spans="1:3">
       <c r="A325" s="1" t="s">
-        <v>310</v>
+        <v>615</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>532</v>
+        <v>612</v>
       </c>
       <c r="C325" s="1" t="s">
         <v>4</v>
@@ -8148,10 +8148,10 @@
     </row>
     <row r="326" spans="1:3">
       <c r="A326" s="1" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C326" s="1" t="s">
         <v>4</v>
@@ -8159,10 +8159,10 @@
     </row>
     <row r="327" spans="1:3">
       <c r="A327" s="1" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="C327" s="1" t="s">
         <v>4</v>
@@ -8170,10 +8170,10 @@
     </row>
     <row r="328" spans="1:3">
       <c r="A328" s="1" t="s">
-        <v>613</v>
+        <v>311</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>614</v>
+        <v>533</v>
       </c>
       <c r="C328" s="1" t="s">
         <v>4</v>
@@ -8181,10 +8181,10 @@
     </row>
     <row r="329" spans="1:3">
       <c r="A329" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C329" s="1" t="s">
         <v>4</v>
@@ -8192,10 +8192,10 @@
     </row>
     <row r="330" spans="1:3">
       <c r="A330" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C330" s="1" t="s">
         <v>4</v>
@@ -8203,10 +8203,10 @@
     </row>
     <row r="331" spans="1:3">
       <c r="A331" s="1" t="s">
-        <v>313</v>
+        <v>833</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>535</v>
+        <v>834</v>
       </c>
       <c r="C331" s="1" t="s">
         <v>4</v>
@@ -8214,10 +8214,10 @@
     </row>
     <row r="332" spans="1:3">
       <c r="A332" s="1" t="s">
-        <v>833</v>
+        <v>917</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>834</v>
+        <v>919</v>
       </c>
       <c r="C332" s="1" t="s">
         <v>4</v>
@@ -8225,32 +8225,32 @@
     </row>
     <row r="333" spans="1:3">
       <c r="A333" s="1" t="s">
-        <v>917</v>
+        <v>726</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>919</v>
+        <v>721</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="334" spans="1:3">
       <c r="A334" s="1" t="s">
-        <v>726</v>
+        <v>765</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>721</v>
+        <v>766</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
     </row>
     <row r="335" spans="1:3">
       <c r="A335" s="1" t="s">
-        <v>765</v>
+        <v>314</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>766</v>
+        <v>536</v>
       </c>
       <c r="C335" s="1" t="s">
         <v>4</v>
@@ -8258,10 +8258,10 @@
     </row>
     <row r="336" spans="1:3">
       <c r="A336" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C336" s="1" t="s">
         <v>4</v>
@@ -8269,10 +8269,10 @@
     </row>
     <row r="337" spans="1:3">
       <c r="A337" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C337" s="1" t="s">
         <v>4</v>
@@ -8280,10 +8280,10 @@
     </row>
     <row r="338" spans="1:3">
       <c r="A338" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C338" s="1" t="s">
         <v>4</v>
@@ -8291,10 +8291,10 @@
     </row>
     <row r="339" spans="1:3">
       <c r="A339" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C339" s="1" t="s">
         <v>4</v>
@@ -8302,10 +8302,10 @@
     </row>
     <row r="340" spans="1:3">
       <c r="A340" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C340" s="1" t="s">
         <v>4</v>
@@ -8313,32 +8313,32 @@
     </row>
     <row r="341" spans="1:3">
       <c r="A341" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>4</v>
+        <v>139</v>
       </c>
     </row>
     <row r="342" spans="1:3">
       <c r="A342" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>139</v>
+        <v>4</v>
       </c>
     </row>
     <row r="343" spans="1:3">
       <c r="A343" s="1" t="s">
-        <v>321</v>
+        <v>807</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>543</v>
+        <v>808</v>
       </c>
       <c r="C343" s="1" t="s">
         <v>4</v>
@@ -8346,10 +8346,10 @@
     </row>
     <row r="344" spans="1:3">
       <c r="A344" s="1" t="s">
-        <v>807</v>
+        <v>638</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>808</v>
+        <v>639</v>
       </c>
       <c r="C344" s="1" t="s">
         <v>4</v>
@@ -8357,10 +8357,10 @@
     </row>
     <row r="345" spans="1:3">
       <c r="A345" s="1" t="s">
-        <v>638</v>
+        <v>322</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>639</v>
+        <v>544</v>
       </c>
       <c r="C345" s="1" t="s">
         <v>4</v>
@@ -8368,10 +8368,10 @@
     </row>
     <row r="346" spans="1:3">
       <c r="A346" s="1" t="s">
-        <v>322</v>
+        <v>922</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>544</v>
+        <v>923</v>
       </c>
       <c r="C346" s="1" t="s">
         <v>4</v>
@@ -8379,10 +8379,10 @@
     </row>
     <row r="347" spans="1:3">
       <c r="A347" s="1" t="s">
-        <v>922</v>
+        <v>323</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>923</v>
+        <v>545</v>
       </c>
       <c r="C347" s="1" t="s">
         <v>4</v>
@@ -8390,10 +8390,10 @@
     </row>
     <row r="348" spans="1:3">
       <c r="A348" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="C348" s="1" t="s">
         <v>4</v>
@@ -8401,10 +8401,10 @@
     </row>
     <row r="349" spans="1:3">
       <c r="A349" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C349" s="1" t="s">
         <v>4</v>
@@ -8412,10 +8412,10 @@
     </row>
     <row r="350" spans="1:3">
       <c r="A350" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C350" s="1" t="s">
         <v>4</v>
@@ -8423,10 +8423,10 @@
     </row>
     <row r="351" spans="1:3">
       <c r="A351" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C351" s="1" t="s">
         <v>4</v>
@@ -8434,10 +8434,10 @@
     </row>
     <row r="352" spans="1:3">
       <c r="A352" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C352" s="1" t="s">
         <v>4</v>
@@ -8445,10 +8445,10 @@
     </row>
     <row r="353" spans="1:3">
       <c r="A353" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C353" s="1" t="s">
         <v>4</v>
@@ -8456,10 +8456,10 @@
     </row>
     <row r="354" spans="1:3">
       <c r="A354" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C354" s="1" t="s">
         <v>4</v>
@@ -8467,10 +8467,10 @@
     </row>
     <row r="355" spans="1:3">
       <c r="A355" s="1" t="s">
-        <v>331</v>
+        <v>803</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>553</v>
+        <v>804</v>
       </c>
       <c r="C355" s="1" t="s">
         <v>4</v>
@@ -8478,10 +8478,10 @@
     </row>
     <row r="356" spans="1:3">
       <c r="A356" s="1" t="s">
-        <v>803</v>
+        <v>332</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>804</v>
+        <v>554</v>
       </c>
       <c r="C356" s="1" t="s">
         <v>4</v>
@@ -8489,10 +8489,10 @@
     </row>
     <row r="357" spans="1:3">
       <c r="A357" s="1" t="s">
-        <v>332</v>
+        <v>821</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>554</v>
+        <v>822</v>
       </c>
       <c r="C357" s="1" t="s">
         <v>4</v>
@@ -8500,10 +8500,10 @@
     </row>
     <row r="358" spans="1:3">
       <c r="A358" s="1" t="s">
-        <v>821</v>
+        <v>626</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>822</v>
+        <v>627</v>
       </c>
       <c r="C358" s="1" t="s">
         <v>4</v>
@@ -8511,10 +8511,10 @@
     </row>
     <row r="359" spans="1:3">
       <c r="A359" s="1" t="s">
-        <v>626</v>
+        <v>333</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>627</v>
+        <v>555</v>
       </c>
       <c r="C359" s="1" t="s">
         <v>4</v>
@@ -8522,10 +8522,10 @@
     </row>
     <row r="360" spans="1:3">
       <c r="A360" s="1" t="s">
-        <v>333</v>
+        <v>846</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>555</v>
+        <v>847</v>
       </c>
       <c r="C360" s="1" t="s">
         <v>4</v>
@@ -8533,10 +8533,10 @@
     </row>
     <row r="361" spans="1:3">
       <c r="A361" s="1" t="s">
-        <v>846</v>
+        <v>596</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>847</v>
+        <v>597</v>
       </c>
       <c r="C361" s="1" t="s">
         <v>4</v>
@@ -8544,10 +8544,10 @@
     </row>
     <row r="362" spans="1:3">
       <c r="A362" s="1" t="s">
-        <v>596</v>
+        <v>334</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>597</v>
+        <v>556</v>
       </c>
       <c r="C362" s="1" t="s">
         <v>4</v>
@@ -8555,10 +8555,10 @@
     </row>
     <row r="363" spans="1:3">
       <c r="A363" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C363" s="1" t="s">
         <v>4</v>
@@ -8566,10 +8566,10 @@
     </row>
     <row r="364" spans="1:3">
       <c r="A364" s="1" t="s">
-        <v>335</v>
+        <v>718</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C364" s="1" t="s">
         <v>4</v>
@@ -8577,10 +8577,10 @@
     </row>
     <row r="365" spans="1:3">
       <c r="A365" s="1" t="s">
-        <v>718</v>
+        <v>908</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>558</v>
+        <v>909</v>
       </c>
       <c r="C365" s="1" t="s">
         <v>4</v>
@@ -8588,10 +8588,10 @@
     </row>
     <row r="366" spans="1:3">
       <c r="A366" s="1" t="s">
-        <v>908</v>
+        <v>719</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>909</v>
+        <v>720</v>
       </c>
       <c r="C366" s="1" t="s">
         <v>4</v>
@@ -8599,10 +8599,10 @@
     </row>
     <row r="367" spans="1:3">
       <c r="A367" s="1" t="s">
-        <v>719</v>
+        <v>795</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>720</v>
+        <v>796</v>
       </c>
       <c r="C367" s="1" t="s">
         <v>4</v>
@@ -8610,10 +8610,10 @@
     </row>
     <row r="368" spans="1:3">
       <c r="A368" s="1" t="s">
-        <v>795</v>
+        <v>779</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>796</v>
+        <v>780</v>
       </c>
       <c r="C368" s="1" t="s">
         <v>4</v>
@@ -8621,10 +8621,10 @@
     </row>
     <row r="369" spans="1:3">
       <c r="A369" s="1" t="s">
-        <v>779</v>
+        <v>336</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>780</v>
+        <v>559</v>
       </c>
       <c r="C369" s="1" t="s">
         <v>4</v>
@@ -8632,10 +8632,10 @@
     </row>
     <row r="370" spans="1:3">
       <c r="A370" s="1" t="s">
-        <v>336</v>
+        <v>835</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>559</v>
+        <v>836</v>
       </c>
       <c r="C370" s="1" t="s">
         <v>4</v>
@@ -8643,10 +8643,10 @@
     </row>
     <row r="371" spans="1:3">
       <c r="A371" s="1" t="s">
-        <v>835</v>
+        <v>337</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>836</v>
+        <v>560</v>
       </c>
       <c r="C371" s="1" t="s">
         <v>4</v>
@@ -8654,10 +8654,10 @@
     </row>
     <row r="372" spans="1:3">
       <c r="A372" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>4</v>
@@ -8665,32 +8665,32 @@
     </row>
     <row r="373" spans="1:3">
       <c r="A373" s="1" t="s">
-        <v>338</v>
+        <v>642</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>561</v>
+        <v>643</v>
       </c>
       <c r="C373" s="1" t="s">
-        <v>4</v>
+        <v>139</v>
       </c>
     </row>
     <row r="374" spans="1:3">
       <c r="A374" s="1" t="s">
-        <v>642</v>
+        <v>340</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>643</v>
+        <v>563</v>
       </c>
       <c r="C374" s="1" t="s">
-        <v>139</v>
+        <v>4</v>
       </c>
     </row>
     <row r="375" spans="1:3">
       <c r="A375" s="1" t="s">
-        <v>340</v>
+        <v>955</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>563</v>
+        <v>956</v>
       </c>
       <c r="C375" s="1" t="s">
         <v>4</v>
@@ -8698,10 +8698,10 @@
     </row>
     <row r="376" spans="1:3">
       <c r="A376" s="1" t="s">
-        <v>955</v>
+        <v>341</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>956</v>
+        <v>564</v>
       </c>
       <c r="C376" s="1" t="s">
         <v>4</v>
@@ -8709,10 +8709,10 @@
     </row>
     <row r="377" spans="1:3">
       <c r="A377" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C377" s="1" t="s">
         <v>4</v>
@@ -8720,10 +8720,10 @@
     </row>
     <row r="378" spans="1:3">
       <c r="A378" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C378" s="1" t="s">
         <v>4</v>
@@ -8731,10 +8731,10 @@
     </row>
     <row r="379" spans="1:3">
       <c r="A379" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C379" s="1" t="s">
         <v>4</v>
@@ -8742,10 +8742,10 @@
     </row>
     <row r="380" spans="1:3">
       <c r="A380" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C380" s="1" t="s">
         <v>4</v>
@@ -8753,10 +8753,10 @@
     </row>
     <row r="381" spans="1:3">
       <c r="A381" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C381" s="1" t="s">
         <v>4</v>
@@ -8764,10 +8764,10 @@
     </row>
     <row r="382" spans="1:3">
       <c r="A382" s="1" t="s">
-        <v>346</v>
+        <v>850</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>569</v>
+        <v>851</v>
       </c>
       <c r="C382" s="1" t="s">
         <v>4</v>
@@ -8775,10 +8775,10 @@
     </row>
     <row r="383" spans="1:3">
       <c r="A383" s="1" t="s">
-        <v>850</v>
+        <v>680</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>851</v>
+        <v>681</v>
       </c>
       <c r="C383" s="1" t="s">
         <v>4</v>
@@ -8786,10 +8786,10 @@
     </row>
     <row r="384" spans="1:3">
       <c r="A384" s="1" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="C384" s="1" t="s">
         <v>4</v>
@@ -8797,10 +8797,10 @@
     </row>
     <row r="385" spans="1:3">
       <c r="A385" s="1" t="s">
-        <v>683</v>
+        <v>348</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>682</v>
+        <v>571</v>
       </c>
       <c r="C385" s="1" t="s">
         <v>4</v>
@@ -8808,32 +8808,32 @@
     </row>
     <row r="386" spans="1:3">
       <c r="A386" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C386" s="1" t="s">
-        <v>4</v>
+        <v>139</v>
       </c>
     </row>
     <row r="387" spans="1:3">
       <c r="A387" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C387" s="1" t="s">
-        <v>139</v>
+        <v>4</v>
       </c>
     </row>
     <row r="388" spans="1:3">
       <c r="A388" s="1" t="s">
-        <v>350</v>
+        <v>672</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>573</v>
+        <v>673</v>
       </c>
       <c r="C388" s="1" t="s">
         <v>4</v>
@@ -8841,10 +8841,10 @@
     </row>
     <row r="389" spans="1:3">
       <c r="A389" s="1" t="s">
-        <v>672</v>
+        <v>351</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>673</v>
+        <v>574</v>
       </c>
       <c r="C389" s="1" t="s">
         <v>4</v>
@@ -8852,10 +8852,10 @@
     </row>
     <row r="390" spans="1:3">
       <c r="A390" s="1" t="s">
-        <v>351</v>
+        <v>670</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>574</v>
+        <v>671</v>
       </c>
       <c r="C390" s="1" t="s">
         <v>4</v>
@@ -8863,10 +8863,10 @@
     </row>
     <row r="391" spans="1:3">
       <c r="A391" s="1" t="s">
-        <v>670</v>
+        <v>773</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>671</v>
+        <v>774</v>
       </c>
       <c r="C391" s="1" t="s">
         <v>4</v>
@@ -8874,10 +8874,10 @@
     </row>
     <row r="392" spans="1:3">
       <c r="A392" s="1" t="s">
-        <v>773</v>
+        <v>352</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>774</v>
+        <v>575</v>
       </c>
       <c r="C392" s="1" t="s">
         <v>4</v>
@@ -8885,10 +8885,10 @@
     </row>
     <row r="393" spans="1:3">
       <c r="A393" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C393" s="1" t="s">
         <v>4</v>
@@ -8896,10 +8896,10 @@
     </row>
     <row r="394" spans="1:3">
       <c r="A394" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C394" s="1" t="s">
         <v>4</v>
@@ -8907,10 +8907,10 @@
     </row>
     <row r="395" spans="1:3">
       <c r="A395" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="C395" s="1" t="s">
         <v>4</v>
@@ -8918,10 +8918,10 @@
     </row>
     <row r="396" spans="1:3">
       <c r="A396" s="1" t="s">
-        <v>356</v>
+        <v>686</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>579</v>
+        <v>687</v>
       </c>
       <c r="C396" s="1" t="s">
         <v>4</v>
@@ -8929,10 +8929,10 @@
     </row>
     <row r="397" spans="1:3">
       <c r="A397" s="1" t="s">
-        <v>686</v>
+        <v>357</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>687</v>
+        <v>580</v>
       </c>
       <c r="C397" s="1" t="s">
         <v>4</v>
@@ -8940,10 +8940,10 @@
     </row>
     <row r="398" spans="1:3">
       <c r="A398" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C398" s="1" t="s">
         <v>4</v>
@@ -8951,10 +8951,10 @@
     </row>
     <row r="399" spans="1:3">
       <c r="A399" s="1" t="s">
-        <v>358</v>
+        <v>140</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>581</v>
+        <v>141</v>
       </c>
       <c r="C399" s="1" t="s">
         <v>4</v>
@@ -8962,10 +8962,10 @@
     </row>
     <row r="400" spans="1:3">
       <c r="A400" s="1" t="s">
-        <v>140</v>
+        <v>961</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>141</v>
+        <v>962</v>
       </c>
       <c r="C400" s="1" t="s">
         <v>4</v>
@@ -8973,10 +8973,10 @@
     </row>
     <row r="401" spans="1:3">
       <c r="A401" s="1" t="s">
-        <v>961</v>
+        <v>359</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>962</v>
+        <v>582</v>
       </c>
       <c r="C401" s="1" t="s">
         <v>4</v>
@@ -8984,10 +8984,10 @@
     </row>
     <row r="402" spans="1:3">
       <c r="A402" s="1" t="s">
-        <v>359</v>
+        <v>606</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>582</v>
+        <v>607</v>
       </c>
       <c r="C402" s="1" t="s">
         <v>4</v>
@@ -8995,10 +8995,10 @@
     </row>
     <row r="403" spans="1:3">
       <c r="A403" s="1" t="s">
-        <v>606</v>
+        <v>360</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>607</v>
+        <v>583</v>
       </c>
       <c r="C403" s="1" t="s">
         <v>4</v>
@@ -9006,10 +9006,10 @@
     </row>
     <row r="404" spans="1:3">
       <c r="A404" s="1" t="s">
-        <v>360</v>
+        <v>640</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>583</v>
+        <v>641</v>
       </c>
       <c r="C404" s="1" t="s">
         <v>4</v>
@@ -9017,10 +9017,10 @@
     </row>
     <row r="405" spans="1:3">
       <c r="A405" s="1" t="s">
-        <v>640</v>
+        <v>361</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>641</v>
+        <v>584</v>
       </c>
       <c r="C405" s="1" t="s">
         <v>4</v>
@@ -9028,10 +9028,10 @@
     </row>
     <row r="406" spans="1:3">
       <c r="A406" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C406" s="1" t="s">
         <v>4</v>
@@ -9039,10 +9039,10 @@
     </row>
     <row r="407" spans="1:3">
       <c r="A407" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C407" s="1" t="s">
         <v>4</v>
@@ -9050,10 +9050,10 @@
     </row>
     <row r="408" spans="1:3">
       <c r="A408" s="1" t="s">
-        <v>363</v>
+        <v>819</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>586</v>
+        <v>820</v>
       </c>
       <c r="C408" s="1" t="s">
         <v>4</v>
@@ -9061,10 +9061,10 @@
     </row>
     <row r="409" spans="1:3">
       <c r="A409" s="1" t="s">
-        <v>819</v>
+        <v>365</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>820</v>
+        <v>588</v>
       </c>
       <c r="C409" s="1" t="s">
         <v>4</v>
@@ -9072,10 +9072,10 @@
     </row>
     <row r="410" spans="1:3">
       <c r="A410" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C410" s="1" t="s">
         <v>4</v>
@@ -9083,10 +9083,10 @@
     </row>
     <row r="411" spans="1:3">
       <c r="A411" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="C411" s="1" t="s">
         <v>4</v>
@@ -9094,10 +9094,10 @@
     </row>
     <row r="412" spans="1:3">
       <c r="A412" s="1" t="s">
-        <v>368</v>
+        <v>831</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>591</v>
+        <v>832</v>
       </c>
       <c r="C412" s="1" t="s">
         <v>4</v>
@@ -9105,10 +9105,10 @@
     </row>
     <row r="413" spans="1:3">
       <c r="A413" s="1" t="s">
-        <v>831</v>
+        <v>370</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>832</v>
+        <v>593</v>
       </c>
       <c r="C413" s="1" t="s">
         <v>4</v>
@@ -9116,10 +9116,10 @@
     </row>
     <row r="414" spans="1:3">
       <c r="A414" s="1" t="s">
-        <v>370</v>
+        <v>825</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>593</v>
+        <v>826</v>
       </c>
       <c r="C414" s="1" t="s">
         <v>4</v>
@@ -9127,10 +9127,10 @@
     </row>
     <row r="415" spans="1:3">
       <c r="A415" s="1" t="s">
-        <v>825</v>
+        <v>142</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>826</v>
+        <v>143</v>
       </c>
       <c r="C415" s="1" t="s">
         <v>4</v>
@@ -9138,10 +9138,10 @@
     </row>
     <row r="416" spans="1:3">
       <c r="A416" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C416" s="1" t="s">
         <v>4</v>
@@ -9149,10 +9149,10 @@
     </row>
     <row r="417" spans="1:3">
       <c r="A417" s="1" t="s">
-        <v>144</v>
+        <v>787</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>145</v>
+        <v>788</v>
       </c>
       <c r="C417" s="1" t="s">
         <v>4</v>
@@ -9160,10 +9160,10 @@
     </row>
     <row r="418" spans="1:3">
       <c r="A418" s="1" t="s">
-        <v>787</v>
+        <v>1002</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>788</v>
+        <v>1004</v>
       </c>
       <c r="C418" s="1" t="s">
         <v>4</v>
@@ -9171,10 +9171,10 @@
     </row>
     <row r="419" spans="1:3">
       <c r="A419" s="1" t="s">
-        <v>1002</v>
+        <v>1005</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="C419" s="1" t="s">
         <v>4</v>
@@ -9182,10 +9182,10 @@
     </row>
     <row r="420" spans="1:3">
       <c r="A420" s="1" t="s">
-        <v>1005</v>
+        <v>1009</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="C420" s="1" t="s">
         <v>4</v>
@@ -9193,10 +9193,10 @@
     </row>
     <row r="421" spans="1:3">
       <c r="A421" s="1" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="C421" s="1" t="s">
         <v>4</v>
@@ -9204,10 +9204,10 @@
     </row>
     <row r="422" spans="1:3">
       <c r="A422" s="1" t="s">
-        <v>1011</v>
-      </c>
-      <c r="B422" s="1" t="s">
-        <v>1012</v>
+        <v>1013</v>
+      </c>
+      <c r="B422" s="4" t="s">
+        <v>1014</v>
       </c>
       <c r="C422" s="1" t="s">
         <v>4</v>
@@ -9215,10 +9215,10 @@
     </row>
     <row r="423" spans="1:3">
       <c r="A423" s="1" t="s">
-        <v>1013</v>
-      </c>
-      <c r="B423" s="4" t="s">
-        <v>1014</v>
+        <v>1015</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>1016</v>
       </c>
       <c r="C423" s="1" t="s">
         <v>4</v>
@@ -9226,32 +9226,32 @@
     </row>
     <row r="424" spans="1:3">
       <c r="A424" s="1" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="C424" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="425" spans="1:3">
       <c r="A425" s="1" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="C425" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
     </row>
     <row r="426" spans="1:3">
       <c r="A426" s="1" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="C426" s="1" t="s">
         <v>4</v>
@@ -9259,10 +9259,10 @@
     </row>
     <row r="427" spans="1:3">
       <c r="A427" s="1" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="C427" s="1" t="s">
         <v>4</v>
@@ -9270,10 +9270,10 @@
     </row>
     <row r="428" spans="1:3">
       <c r="A428" s="1" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="C428" s="1" t="s">
         <v>4</v>
@@ -9281,10 +9281,10 @@
     </row>
     <row r="429" spans="1:3">
       <c r="A429" s="1" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="C429" s="1" t="s">
         <v>4</v>
@@ -9292,10 +9292,10 @@
     </row>
     <row r="430" spans="1:3">
       <c r="A430" s="1" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="C430" s="1" t="s">
         <v>4</v>
@@ -9303,10 +9303,10 @@
     </row>
     <row r="431" spans="1:3">
       <c r="A431" s="1" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="C431" s="1" t="s">
         <v>4</v>
@@ -9314,10 +9314,10 @@
     </row>
     <row r="432" spans="1:3">
       <c r="A432" s="1" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="C432" s="1" t="s">
         <v>4</v>
@@ -9325,10 +9325,10 @@
     </row>
     <row r="433" spans="1:3">
       <c r="A433" s="1" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="C433" s="1" t="s">
         <v>4</v>
@@ -9336,10 +9336,10 @@
     </row>
     <row r="434" spans="1:3">
       <c r="A434" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="C434" s="1" t="s">
         <v>4</v>
@@ -9347,10 +9347,10 @@
     </row>
     <row r="435" spans="1:3">
       <c r="A435" s="1" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="C435" s="1" t="s">
         <v>4</v>
@@ -9358,10 +9358,10 @@
     </row>
     <row r="436" spans="1:3">
       <c r="A436" s="1" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="C436" s="1" t="s">
         <v>4</v>
@@ -9369,10 +9369,10 @@
     </row>
     <row r="437" spans="1:3">
       <c r="A437" s="1" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="C437" s="1" t="s">
         <v>4</v>
@@ -9380,10 +9380,10 @@
     </row>
     <row r="438" spans="1:3">
       <c r="A438" s="1" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="C438" s="1" t="s">
         <v>4</v>
@@ -9391,10 +9391,10 @@
     </row>
     <row r="439" spans="1:3">
       <c r="A439" s="1" t="s">
-        <v>1045</v>
+        <v>1061</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="C439" s="1" t="s">
         <v>4</v>
@@ -9402,10 +9402,10 @@
     </row>
     <row r="440" spans="1:3">
       <c r="A440" s="1" t="s">
-        <v>1061</v>
+        <v>1048</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="C440" s="1" t="s">
         <v>4</v>
@@ -9413,10 +9413,10 @@
     </row>
     <row r="441" spans="1:3">
       <c r="A441" s="1" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="C441" s="1" t="s">
         <v>4</v>
@@ -9424,10 +9424,10 @@
     </row>
     <row r="442" spans="1:3">
       <c r="A442" s="1" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="C442" s="1" t="s">
         <v>4</v>
@@ -9435,10 +9435,10 @@
     </row>
     <row r="443" spans="1:3">
       <c r="A443" s="1" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="C443" s="1" t="s">
         <v>4</v>
@@ -9446,10 +9446,10 @@
     </row>
     <row r="444" spans="1:3">
       <c r="A444" s="1" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="C444" s="1" t="s">
         <v>4</v>
@@ -9457,10 +9457,10 @@
     </row>
     <row r="445" spans="1:3">
       <c r="A445" s="1" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="C445" s="1" t="s">
         <v>4</v>
@@ -9468,10 +9468,10 @@
     </row>
     <row r="446" spans="1:3">
       <c r="A446" s="1" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>1059</v>
+        <v>1062</v>
       </c>
       <c r="C446" s="1" t="s">
         <v>4</v>
@@ -9479,10 +9479,10 @@
     </row>
     <row r="447" spans="1:3">
       <c r="A447" s="1" t="s">
-        <v>1060</v>
+        <v>1063</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="C447" s="1" t="s">
         <v>4</v>
@@ -9490,10 +9490,10 @@
     </row>
     <row r="448" spans="1:3">
       <c r="A448" s="1" t="s">
-        <v>1063</v>
+        <v>1067</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="C448" s="1" t="s">
         <v>4</v>
@@ -9501,10 +9501,10 @@
     </row>
     <row r="449" spans="1:3">
       <c r="A449" s="1" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>1066</v>
+        <v>1070</v>
       </c>
       <c r="C449" s="1" t="s">
         <v>4</v>
@@ -9512,10 +9512,10 @@
     </row>
     <row r="450" spans="1:3">
       <c r="A450" s="1" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="C450" s="1" t="s">
         <v>4</v>
@@ -9523,10 +9523,10 @@
     </row>
     <row r="451" spans="1:3">
       <c r="A451" s="1" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="C451" s="1" t="s">
         <v>4</v>
@@ -9534,10 +9534,10 @@
     </row>
     <row r="452" spans="1:3">
       <c r="A452" s="1" t="s">
-        <v>1065</v>
+        <v>1073</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>1066</v>
+        <v>1074</v>
       </c>
       <c r="C452" s="1" t="s">
         <v>4</v>
@@ -9545,10 +9545,10 @@
     </row>
     <row r="453" spans="1:3">
       <c r="A453" s="1" t="s">
-        <v>1071</v>
+        <v>1075</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>1072</v>
+        <v>1078</v>
       </c>
       <c r="C453" s="1" t="s">
         <v>4</v>
@@ -9556,10 +9556,10 @@
     </row>
     <row r="454" spans="1:3">
       <c r="A454" s="1" t="s">
-        <v>1073</v>
+        <v>1081</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>1074</v>
+        <v>1082</v>
       </c>
       <c r="C454" s="1" t="s">
         <v>4</v>
@@ -9567,10 +9567,10 @@
     </row>
     <row r="455" spans="1:3">
       <c r="A455" s="1" t="s">
-        <v>1075</v>
+        <v>1083</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>1078</v>
+        <v>1084</v>
       </c>
       <c r="C455" s="1" t="s">
         <v>4</v>
@@ -9578,10 +9578,10 @@
     </row>
     <row r="456" spans="1:3">
       <c r="A456" s="1" t="s">
-        <v>1081</v>
+        <v>1086</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>1082</v>
+        <v>1085</v>
       </c>
       <c r="C456" s="1" t="s">
         <v>4</v>
@@ -9589,10 +9589,10 @@
     </row>
     <row r="457" spans="1:3">
       <c r="A457" s="1" t="s">
-        <v>1083</v>
+        <v>1091</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>1084</v>
+        <v>1092</v>
       </c>
       <c r="C457" s="1" t="s">
         <v>4</v>
@@ -9600,10 +9600,10 @@
     </row>
     <row r="458" spans="1:3">
       <c r="A458" s="1" t="s">
-        <v>1086</v>
+        <v>1097</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>1085</v>
+        <v>1098</v>
       </c>
       <c r="C458" s="1" t="s">
         <v>4</v>
@@ -9611,10 +9611,10 @@
     </row>
     <row r="459" spans="1:3">
       <c r="A459" s="1" t="s">
-        <v>1091</v>
+        <v>1105</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>1092</v>
+        <v>1106</v>
       </c>
       <c r="C459" s="1" t="s">
         <v>4</v>
@@ -9622,10 +9622,10 @@
     </row>
     <row r="460" spans="1:3">
       <c r="A460" s="1" t="s">
-        <v>1097</v>
+        <v>1107</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>1098</v>
+        <v>1108</v>
       </c>
       <c r="C460" s="1" t="s">
         <v>4</v>
@@ -9633,10 +9633,10 @@
     </row>
     <row r="461" spans="1:3">
       <c r="A461" s="1" t="s">
-        <v>1105</v>
+        <v>1109</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>1106</v>
+        <v>1110</v>
       </c>
       <c r="C461" s="1" t="s">
         <v>4</v>
@@ -9644,10 +9644,10 @@
     </row>
     <row r="462" spans="1:3">
       <c r="A462" s="1" t="s">
-        <v>1107</v>
+        <v>1111</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C462" s="1" t="s">
         <v>4</v>
@@ -9655,21 +9655,21 @@
     </row>
     <row r="463" spans="1:3">
       <c r="A463" s="1" t="s">
-        <v>1109</v>
+        <v>1115</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>1110</v>
+        <v>1116</v>
       </c>
       <c r="C463" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="464" spans="1:3">
-      <c r="A464" s="1" t="s">
-        <v>1111</v>
+      <c r="A464" s="4" t="s">
+        <v>1119</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>1112</v>
+        <v>1120</v>
       </c>
       <c r="C464" s="1" t="s">
         <v>4</v>
@@ -9677,21 +9677,21 @@
     </row>
     <row r="465" spans="1:3">
       <c r="A465" s="1" t="s">
-        <v>1115</v>
+        <v>1125</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>1116</v>
+        <v>1126</v>
       </c>
       <c r="C465" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="466" spans="1:3">
-      <c r="A466" s="4" t="s">
-        <v>1119</v>
+      <c r="A466" s="1" t="s">
+        <v>1127</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>1120</v>
+        <v>1128</v>
       </c>
       <c r="C466" s="1" t="s">
         <v>4</v>
@@ -9699,10 +9699,10 @@
     </row>
     <row r="467" spans="1:3">
       <c r="A467" s="1" t="s">
-        <v>1125</v>
+        <v>1129</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>1126</v>
+        <v>1130</v>
       </c>
       <c r="C467" s="1" t="s">
         <v>4</v>
@@ -9710,10 +9710,10 @@
     </row>
     <row r="468" spans="1:3">
       <c r="A468" s="1" t="s">
-        <v>1127</v>
+        <v>1131</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>1128</v>
+        <v>1132</v>
       </c>
       <c r="C468" s="1" t="s">
         <v>4</v>
@@ -9721,10 +9721,10 @@
     </row>
     <row r="469" spans="1:3">
       <c r="A469" s="1" t="s">
-        <v>1129</v>
+        <v>1133</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>1130</v>
+        <v>1134</v>
       </c>
       <c r="C469" s="1" t="s">
         <v>4</v>
@@ -9732,10 +9732,10 @@
     </row>
     <row r="470" spans="1:3">
       <c r="A470" s="1" t="s">
-        <v>1131</v>
+        <v>1135</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>1132</v>
+        <v>1136</v>
       </c>
       <c r="C470" s="1" t="s">
         <v>4</v>
@@ -9743,10 +9743,10 @@
     </row>
     <row r="471" spans="1:3">
       <c r="A471" s="1" t="s">
-        <v>1133</v>
+        <v>1137</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>1134</v>
+        <v>1138</v>
       </c>
       <c r="C471" s="1" t="s">
         <v>4</v>
@@ -9754,10 +9754,10 @@
     </row>
     <row r="472" spans="1:3">
       <c r="A472" s="1" t="s">
-        <v>1135</v>
+        <v>1139</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>1136</v>
+        <v>1140</v>
       </c>
       <c r="C472" s="1" t="s">
         <v>4</v>
@@ -9765,10 +9765,10 @@
     </row>
     <row r="473" spans="1:3">
       <c r="A473" s="1" t="s">
-        <v>1137</v>
+        <v>1141</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>1138</v>
+        <v>1142</v>
       </c>
       <c r="C473" s="1" t="s">
         <v>4</v>
@@ -9776,10 +9776,10 @@
     </row>
     <row r="474" spans="1:3">
       <c r="A474" s="1" t="s">
-        <v>1139</v>
+        <v>1143</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>1140</v>
+        <v>1144</v>
       </c>
       <c r="C474" s="1" t="s">
         <v>4</v>
@@ -9787,10 +9787,10 @@
     </row>
     <row r="475" spans="1:3">
       <c r="A475" s="1" t="s">
-        <v>1141</v>
+        <v>1149</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>1142</v>
+        <v>1150</v>
       </c>
       <c r="C475" s="1" t="s">
         <v>4</v>
@@ -9798,10 +9798,10 @@
     </row>
     <row r="476" spans="1:3">
       <c r="A476" s="1" t="s">
-        <v>1143</v>
+        <v>1151</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>1144</v>
+        <v>1152</v>
       </c>
       <c r="C476" s="1" t="s">
         <v>4</v>
@@ -9809,10 +9809,10 @@
     </row>
     <row r="477" spans="1:3">
       <c r="A477" s="1" t="s">
-        <v>1149</v>
+        <v>1153</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>1150</v>
+        <v>1154</v>
       </c>
       <c r="C477" s="1" t="s">
         <v>4</v>
@@ -9820,10 +9820,10 @@
     </row>
     <row r="478" spans="1:3">
       <c r="A478" s="1" t="s">
-        <v>1151</v>
+        <v>1155</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>1152</v>
+        <v>1156</v>
       </c>
       <c r="C478" s="1" t="s">
         <v>4</v>
@@ -9831,21 +9831,21 @@
     </row>
     <row r="479" spans="1:3">
       <c r="A479" s="1" t="s">
-        <v>1153</v>
+        <v>1158</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>1154</v>
+        <v>1157</v>
       </c>
       <c r="C479" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="480" spans="1:3">
-      <c r="A480" s="1" t="s">
-        <v>1155</v>
+      <c r="A480" s="4" t="s">
+        <v>1159</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>1156</v>
+        <v>1160</v>
       </c>
       <c r="C480" s="1" t="s">
         <v>4</v>
@@ -9853,10 +9853,10 @@
     </row>
     <row r="481" spans="1:3">
       <c r="A481" s="1" t="s">
-        <v>1158</v>
+        <v>1161</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>1157</v>
+        <v>1162</v>
       </c>
       <c r="C481" s="1" t="s">
         <v>4</v>
@@ -9864,21 +9864,21 @@
     </row>
     <row r="482" spans="1:3">
       <c r="A482" s="4" t="s">
-        <v>1159</v>
+        <v>1163</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>1160</v>
+        <v>1164</v>
       </c>
       <c r="C482" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="483" spans="1:3">
-      <c r="A483" s="1" t="s">
-        <v>1161</v>
+      <c r="A483" s="4" t="s">
+        <v>1165</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>1162</v>
+        <v>1166</v>
       </c>
       <c r="C483" s="1" t="s">
         <v>4</v>
@@ -9886,21 +9886,21 @@
     </row>
     <row r="484" spans="1:3">
       <c r="A484" s="4" t="s">
-        <v>1163</v>
+        <v>1167</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>1164</v>
+        <v>1168</v>
       </c>
       <c r="C484" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="485" spans="1:3">
-      <c r="A485" s="4" t="s">
-        <v>1165</v>
+      <c r="A485" s="1" t="s">
+        <v>1169</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>1166</v>
+        <v>1170</v>
       </c>
       <c r="C485" s="1" t="s">
         <v>4</v>
@@ -9908,10 +9908,10 @@
     </row>
     <row r="486" spans="1:3">
       <c r="A486" s="4" t="s">
-        <v>1167</v>
+        <v>1171</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>1168</v>
+        <v>1172</v>
       </c>
       <c r="C486" s="1" t="s">
         <v>4</v>
@@ -9919,21 +9919,21 @@
     </row>
     <row r="487" spans="1:3">
       <c r="A487" s="1" t="s">
-        <v>1169</v>
+        <v>1173</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>1170</v>
+        <v>1174</v>
       </c>
       <c r="C487" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="488" spans="1:3">
-      <c r="A488" s="4" t="s">
-        <v>1171</v>
+      <c r="A488" s="1" t="s">
+        <v>1175</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>1172</v>
+        <v>1176</v>
       </c>
       <c r="C488" s="1" t="s">
         <v>4</v>
@@ -9941,21 +9941,21 @@
     </row>
     <row r="489" spans="1:3">
       <c r="A489" s="1" t="s">
-        <v>1173</v>
+        <v>1177</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>1174</v>
+        <v>1178</v>
       </c>
       <c r="C489" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="490" spans="1:3">
-      <c r="A490" s="1" t="s">
-        <v>1175</v>
+      <c r="A490" s="4" t="s">
+        <v>1180</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>1176</v>
+        <v>1179</v>
       </c>
       <c r="C490" s="1" t="s">
         <v>4</v>
@@ -9963,109 +9963,109 @@
     </row>
     <row r="491" spans="1:3">
       <c r="A491" s="1" t="s">
-        <v>1177</v>
+        <v>1181</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>1178</v>
+        <v>1182</v>
       </c>
       <c r="C491" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="492" spans="1:3">
-      <c r="A492" s="4" t="s">
-        <v>1180</v>
+      <c r="A492" s="1" t="s">
+        <v>1183</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>1179</v>
+        <v>1184</v>
       </c>
       <c r="C492" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="493" spans="1:3">
-      <c r="A493" s="1" t="s">
-        <v>1181</v>
+      <c r="A493" s="4" t="s">
+        <v>1185</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>1182</v>
+        <v>1186</v>
       </c>
       <c r="C493" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="494" spans="1:3">
-      <c r="A494" s="1" t="s">
-        <v>1183</v>
+      <c r="A494" s="4" t="s">
+        <v>1190</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1184</v>
+        <v>1189</v>
       </c>
       <c r="C494" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="495" spans="1:3">
-      <c r="A495" s="4" t="s">
-        <v>1185</v>
+      <c r="A495" s="1" t="s">
+        <v>1191</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1186</v>
+        <v>1192</v>
       </c>
       <c r="C495" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="496" spans="1:3">
-      <c r="A496" s="4" t="s">
-        <v>1190</v>
+      <c r="A496" s="1" t="s">
+        <v>1196</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1189</v>
+        <v>1197</v>
       </c>
       <c r="C496" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="497" spans="1:3">
-      <c r="A497" s="1" t="s">
-        <v>1191</v>
-      </c>
-      <c r="B497" s="1" t="s">
-        <v>1192</v>
-      </c>
-      <c r="C497" s="1" t="s">
+      <c r="A497" s="4" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B497" s="4" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C497" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="498" spans="1:3">
       <c r="A498" s="1" t="s">
-        <v>1196</v>
+        <v>1219</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1197</v>
+        <v>1218</v>
       </c>
       <c r="C498" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="499" spans="1:3">
-      <c r="A499" s="4" t="s">
-        <v>1215</v>
-      </c>
-      <c r="B499" s="4" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C499" s="4" t="s">
+      <c r="A499" s="1" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B499" s="1" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C499" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="500" spans="1:3">
-      <c r="A500" s="1" t="s">
-        <v>1219</v>
+      <c r="A500" s="4" t="s">
+        <v>1223</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1218</v>
+        <v>1222</v>
       </c>
       <c r="C500" s="1" t="s">
         <v>4</v>
@@ -10073,21 +10073,21 @@
     </row>
     <row r="501" spans="1:3">
       <c r="A501" s="1" t="s">
-        <v>1221</v>
-      </c>
-      <c r="B501" s="1" t="s">
-        <v>1220</v>
+        <v>1225</v>
+      </c>
+      <c r="B501" s="4" t="s">
+        <v>1224</v>
       </c>
       <c r="C501" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="502" spans="1:3">
-      <c r="A502" s="4" t="s">
-        <v>1223</v>
+      <c r="A502" s="1" t="s">
+        <v>1229</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1222</v>
+        <v>1228</v>
       </c>
       <c r="C502" s="1" t="s">
         <v>4</v>
@@ -10095,10 +10095,10 @@
     </row>
     <row r="503" spans="1:3">
       <c r="A503" s="1" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B503" s="4" t="s">
-        <v>1224</v>
+        <v>1231</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>1230</v>
       </c>
       <c r="C503" s="1" t="s">
         <v>4</v>
@@ -10106,10 +10106,10 @@
     </row>
     <row r="504" spans="1:3">
       <c r="A504" s="1" t="s">
-        <v>1229</v>
-      </c>
-      <c r="B504" s="1" t="s">
-        <v>1228</v>
+        <v>1233</v>
+      </c>
+      <c r="B504" s="4" t="s">
+        <v>1232</v>
       </c>
       <c r="C504" s="1" t="s">
         <v>4</v>
@@ -10117,10 +10117,10 @@
     </row>
     <row r="505" spans="1:3">
       <c r="A505" s="1" t="s">
-        <v>1231</v>
+        <v>1237</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1230</v>
+        <v>1236</v>
       </c>
       <c r="C505" s="1" t="s">
         <v>4</v>
@@ -10128,10 +10128,10 @@
     </row>
     <row r="506" spans="1:3">
       <c r="A506" s="1" t="s">
-        <v>1233</v>
-      </c>
-      <c r="B506" s="4" t="s">
-        <v>1232</v>
+        <v>1245</v>
+      </c>
+      <c r="B506" s="1" t="s">
+        <v>1244</v>
       </c>
       <c r="C506" s="1" t="s">
         <v>4</v>
@@ -10139,10 +10139,10 @@
     </row>
     <row r="507" spans="1:3">
       <c r="A507" s="1" t="s">
-        <v>1237</v>
+        <v>1252</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1236</v>
+        <v>1251</v>
       </c>
       <c r="C507" s="1" t="s">
         <v>4</v>
@@ -10150,10 +10150,10 @@
     </row>
     <row r="508" spans="1:3">
       <c r="A508" s="1" t="s">
-        <v>1245</v>
+        <v>1254</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1244</v>
+        <v>1253</v>
       </c>
       <c r="C508" s="1" t="s">
         <v>4</v>
@@ -10161,10 +10161,10 @@
     </row>
     <row r="509" spans="1:3">
       <c r="A509" s="1" t="s">
-        <v>1252</v>
+        <v>1276</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1251</v>
+        <v>1275</v>
       </c>
       <c r="C509" s="1" t="s">
         <v>4</v>
@@ -10172,10 +10172,10 @@
     </row>
     <row r="510" spans="1:3">
       <c r="A510" s="1" t="s">
-        <v>1254</v>
+        <v>1256</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1253</v>
+        <v>1255</v>
       </c>
       <c r="C510" s="1" t="s">
         <v>4</v>
@@ -10183,10 +10183,10 @@
     </row>
     <row r="511" spans="1:3">
       <c r="A511" s="1" t="s">
-        <v>1276</v>
+        <v>1258</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1275</v>
+        <v>1257</v>
       </c>
       <c r="C511" s="1" t="s">
         <v>4</v>
@@ -10194,10 +10194,10 @@
     </row>
     <row r="512" spans="1:3">
       <c r="A512" s="1" t="s">
-        <v>1256</v>
+        <v>1262</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>1255</v>
+        <v>1261</v>
       </c>
       <c r="C512" s="1" t="s">
         <v>4</v>
@@ -10205,10 +10205,10 @@
     </row>
     <row r="513" spans="1:3">
       <c r="A513" s="1" t="s">
-        <v>1258</v>
+        <v>1264</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>1257</v>
+        <v>1263</v>
       </c>
       <c r="C513" s="1" t="s">
         <v>4</v>
@@ -10216,65 +10216,65 @@
     </row>
     <row r="514" spans="1:3">
       <c r="A514" s="1" t="s">
-        <v>1262</v>
+        <v>1266</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>1261</v>
+        <v>1265</v>
       </c>
       <c r="C514" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="515" spans="1:3">
-      <c r="A515" s="1" t="s">
-        <v>1264</v>
-      </c>
-      <c r="B515" s="1" t="s">
-        <v>1263</v>
+      <c r="A515" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B515" s="4" t="s">
+        <v>1267</v>
       </c>
       <c r="C515" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="516" spans="1:3">
-      <c r="A516" s="1" t="s">
-        <v>1266</v>
+      <c r="A516" s="4" t="s">
+        <v>1269</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1265</v>
+        <v>1270</v>
       </c>
       <c r="C516" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="517" spans="1:3">
-      <c r="A517" t="s">
-        <v>1268</v>
-      </c>
-      <c r="B517" s="4" t="s">
-        <v>1267</v>
+      <c r="A517" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>1272</v>
       </c>
       <c r="C517" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="518" spans="1:3">
-      <c r="A518" s="4" t="s">
-        <v>1269</v>
+      <c r="A518" s="1" t="s">
+        <v>1274</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1270</v>
+        <v>1273</v>
       </c>
       <c r="C518" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="519" spans="1:3">
-      <c r="A519" s="4" t="s">
-        <v>1271</v>
+      <c r="A519" s="1" t="s">
+        <v>1278</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1272</v>
+        <v>1277</v>
       </c>
       <c r="C519" s="1" t="s">
         <v>4</v>
@@ -10282,21 +10282,21 @@
     </row>
     <row r="520" spans="1:3">
       <c r="A520" s="1" t="s">
-        <v>1274</v>
+        <v>1279</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1273</v>
+        <v>1280</v>
       </c>
       <c r="C520" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="521" spans="1:3">
-      <c r="A521" s="1" t="s">
-        <v>1278</v>
+      <c r="A521" s="4" t="s">
+        <v>1281</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1277</v>
+        <v>1282</v>
       </c>
       <c r="C521" s="1" t="s">
         <v>4</v>
@@ -10304,21 +10304,21 @@
     </row>
     <row r="522" spans="1:3">
       <c r="A522" s="1" t="s">
-        <v>1279</v>
+        <v>1283</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1280</v>
+        <v>1284</v>
       </c>
       <c r="C522" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="523" spans="1:3">
-      <c r="A523" s="4" t="s">
-        <v>1281</v>
+      <c r="A523" s="1" t="s">
+        <v>1285</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1282</v>
+        <v>1286</v>
       </c>
       <c r="C523" s="1" t="s">
         <v>4</v>
@@ -10326,21 +10326,21 @@
     </row>
     <row r="524" spans="1:3">
       <c r="A524" s="1" t="s">
-        <v>1283</v>
+        <v>1287</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1284</v>
+        <v>1288</v>
       </c>
       <c r="C524" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="525" spans="1:3">
-      <c r="A525" s="1" t="s">
-        <v>1285</v>
+      <c r="A525" s="4" t="s">
+        <v>1289</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1286</v>
+        <v>1290</v>
       </c>
       <c r="C525" s="1" t="s">
         <v>4</v>
@@ -10348,21 +10348,21 @@
     </row>
     <row r="526" spans="1:3">
       <c r="A526" s="1" t="s">
-        <v>1287</v>
+        <v>1291</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1288</v>
+        <v>1292</v>
       </c>
       <c r="C526" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="527" spans="1:3">
-      <c r="A527" s="4" t="s">
-        <v>1289</v>
+      <c r="A527" s="1" t="s">
+        <v>1293</v>
       </c>
       <c r="B527" s="1" t="s">
-        <v>1290</v>
+        <v>1294</v>
       </c>
       <c r="C527" s="1" t="s">
         <v>4</v>
@@ -10370,10 +10370,10 @@
     </row>
     <row r="528" spans="1:3">
       <c r="A528" s="1" t="s">
-        <v>1291</v>
+        <v>1296</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>1292</v>
+        <v>1295</v>
       </c>
       <c r="C528" s="1" t="s">
         <v>4</v>
@@ -10381,10 +10381,10 @@
     </row>
     <row r="529" spans="1:3">
       <c r="A529" s="1" t="s">
-        <v>1293</v>
+        <v>1303</v>
       </c>
       <c r="B529" s="1" t="s">
-        <v>1294</v>
+        <v>1304</v>
       </c>
       <c r="C529" s="1" t="s">
         <v>4</v>
@@ -10392,10 +10392,10 @@
     </row>
     <row r="530" spans="1:3">
       <c r="A530" s="1" t="s">
-        <v>1296</v>
+        <v>1305</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1295</v>
+        <v>1306</v>
       </c>
       <c r="C530" s="1" t="s">
         <v>4</v>
@@ -10403,10 +10403,10 @@
     </row>
     <row r="531" spans="1:3">
       <c r="A531" s="1" t="s">
-        <v>1303</v>
+        <v>1307</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>1304</v>
+        <v>1308</v>
       </c>
       <c r="C531" s="1" t="s">
         <v>4</v>
@@ -10414,10 +10414,10 @@
     </row>
     <row r="532" spans="1:3">
       <c r="A532" s="1" t="s">
-        <v>1305</v>
+        <v>1309</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>1306</v>
+        <v>1310</v>
       </c>
       <c r="C532" s="1" t="s">
         <v>4</v>
@@ -10425,10 +10425,10 @@
     </row>
     <row r="533" spans="1:3">
       <c r="A533" s="1" t="s">
-        <v>1307</v>
+        <v>1311</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>1308</v>
+        <v>1312</v>
       </c>
       <c r="C533" s="1" t="s">
         <v>4</v>
@@ -10436,10 +10436,10 @@
     </row>
     <row r="534" spans="1:3">
       <c r="A534" s="1" t="s">
-        <v>1309</v>
+        <v>1327</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>1310</v>
+        <v>1328</v>
       </c>
       <c r="C534" s="1" t="s">
         <v>4</v>
@@ -10447,10 +10447,10 @@
     </row>
     <row r="535" spans="1:3">
       <c r="A535" s="1" t="s">
-        <v>1311</v>
+        <v>1334</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>1312</v>
+        <v>1333</v>
       </c>
       <c r="C535" s="1" t="s">
         <v>4</v>
@@ -10458,10 +10458,10 @@
     </row>
     <row r="536" spans="1:3">
       <c r="A536" s="1" t="s">
-        <v>1327</v>
+        <v>1335</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1328</v>
+        <v>1336</v>
       </c>
       <c r="C536" s="1" t="s">
         <v>4</v>
@@ -10469,10 +10469,10 @@
     </row>
     <row r="537" spans="1:3">
       <c r="A537" s="1" t="s">
-        <v>1334</v>
+        <v>1347</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1333</v>
+        <v>1348</v>
       </c>
       <c r="C537" s="1" t="s">
         <v>4</v>
@@ -10480,10 +10480,10 @@
     </row>
     <row r="538" spans="1:3">
       <c r="A538" s="1" t="s">
-        <v>1335</v>
+        <v>1349</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>1336</v>
+        <v>1350</v>
       </c>
       <c r="C538" s="1" t="s">
         <v>4</v>
@@ -10491,10 +10491,10 @@
     </row>
     <row r="539" spans="1:3">
       <c r="A539" s="1" t="s">
-        <v>1347</v>
+        <v>1351</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="C539" s="1" t="s">
         <v>4</v>
@@ -10502,10 +10502,10 @@
     </row>
     <row r="540" spans="1:3">
       <c r="A540" s="1" t="s">
-        <v>1349</v>
+        <v>1353</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1350</v>
+        <v>1354</v>
       </c>
       <c r="C540" s="1" t="s">
         <v>4</v>
@@ -10513,10 +10513,10 @@
     </row>
     <row r="541" spans="1:3">
       <c r="A541" s="1" t="s">
-        <v>1351</v>
+        <v>1355</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1352</v>
+        <v>1356</v>
       </c>
       <c r="C541" s="1" t="s">
         <v>4</v>
@@ -10524,34 +10524,12 @@
     </row>
     <row r="542" spans="1:3">
       <c r="A542" s="1" t="s">
-        <v>1353</v>
+        <v>1357</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1354</v>
+        <v>1358</v>
       </c>
       <c r="C542" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="543" spans="1:3">
-      <c r="A543" s="1" t="s">
-        <v>1355</v>
-      </c>
-      <c r="B543" s="1" t="s">
-        <v>1356</v>
-      </c>
-      <c r="C543" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="544" spans="1:3">
-      <c r="A544" s="1" t="s">
-        <v>1357</v>
-      </c>
-      <c r="B544" s="1" t="s">
-        <v>1358</v>
-      </c>
-      <c r="C544" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -10569,7 +10547,7 @@
   <dimension ref="A1:C597"/>
   <sheetViews>
     <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136:C137"/>
+      <selection activeCell="A138" sqref="A138:XFD138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12087,6 +12065,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="330" spans="2:2">
       <c r="B330" s="3"/>
     </row>

</xml_diff>

<commit_message>
1. Fix font awesome icon issue 2. Fix google search issue
</commit_message>
<xml_diff>
--- a/data/media.xlsx
+++ b/data/media.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7500D7-355C-4266-95EC-14329928F9D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BACCD3-D21E-4074-AC10-9FE57499A990}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="media" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="1383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2116" uniqueCount="1407">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4211,6 +4211,78 @@
   </si>
   <si>
     <t>tt2737304</t>
+  </si>
+  <si>
+    <t>Maurice</t>
+  </si>
+  <si>
+    <t>tt0093512</t>
+  </si>
+  <si>
+    <t>Evolution</t>
+  </si>
+  <si>
+    <t>tt4291590</t>
+  </si>
+  <si>
+    <t>Polar</t>
+  </si>
+  <si>
+    <t>tt4139588</t>
+  </si>
+  <si>
+    <t>A Star is Born</t>
+  </si>
+  <si>
+    <t>tt1517451</t>
+  </si>
+  <si>
+    <t>Fair Haven</t>
+  </si>
+  <si>
+    <t>tt3520216</t>
+  </si>
+  <si>
+    <t>Gewoon Vrienden</t>
+  </si>
+  <si>
+    <t>tt7901640</t>
+  </si>
+  <si>
+    <t>Mortal Engines</t>
+  </si>
+  <si>
+    <t>tt1571234</t>
+  </si>
+  <si>
+    <t>tt7008872</t>
+  </si>
+  <si>
+    <t>Parting Glances</t>
+  </si>
+  <si>
+    <t>Boy Erased</t>
+  </si>
+  <si>
+    <t>tt0091725</t>
+  </si>
+  <si>
+    <t>Fantastic Beasts The Crimes of Grindelwald</t>
+  </si>
+  <si>
+    <t>tt4123430</t>
+  </si>
+  <si>
+    <t>The Boy Who Could Fly</t>
+  </si>
+  <si>
+    <t>tt0090768</t>
+  </si>
+  <si>
+    <t>The Last Mimzy</t>
+  </si>
+  <si>
+    <t>tt0768212</t>
   </si>
 </sst>
 </file>
@@ -4634,10 +4706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C556"/>
+  <dimension ref="A1:C563"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A531" workbookViewId="0">
-      <selection activeCell="C555" sqref="C555:C556"/>
+    <sheetView tabSelected="1" topLeftCell="A540" workbookViewId="0">
+      <selection activeCell="C560" sqref="C560:C563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10759,6 +10831,83 @@
         <v>4</v>
       </c>
     </row>
+    <row r="557" spans="1:3">
+      <c r="A557" s="1" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B557" s="1" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C557" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="558" spans="1:3">
+      <c r="A558" s="1" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>1388</v>
+      </c>
+      <c r="C558" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="559" spans="1:3">
+      <c r="A559" s="1" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C559" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="560" spans="1:3">
+      <c r="A560" s="1" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C560" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="561" spans="1:3">
+      <c r="A561" s="1" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B561" s="1" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C561" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="562" spans="1:3">
+      <c r="A562" s="1" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B562" s="1" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C562" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="563" spans="1:3">
+      <c r="A563" s="1" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C563" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -10773,7 +10922,7 @@
   <dimension ref="A1:C597"/>
   <sheetViews>
     <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138:XFD138"/>
+      <selection activeCell="C142" sqref="C142:C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12302,6 +12451,61 @@
         <v>4</v>
       </c>
     </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="1" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="1" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="4" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="330" spans="2:2">
       <c r="B330" s="3"/>
     </row>

</xml_diff>

<commit_message>
Fix some literal issues
</commit_message>
<xml_diff>
--- a/data/media.xlsx
+++ b/data/media.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD099A6E-1297-4469-A108-39C7F55FC84D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2582D31-C288-4C05-B26A-5C7B243F4645}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="1409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2134" uniqueCount="1419">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4289,6 +4289,36 @@
   </si>
   <si>
     <t>tt4633694</t>
+  </si>
+  <si>
+    <t>Glass</t>
+  </si>
+  <si>
+    <t>tt6823368</t>
+  </si>
+  <si>
+    <t>Eyes Wide Shut</t>
+  </si>
+  <si>
+    <t>tt0120663</t>
+  </si>
+  <si>
+    <t>How to Train Your Dragon: The Hidden World</t>
+  </si>
+  <si>
+    <t>tt2386490</t>
+  </si>
+  <si>
+    <t>Bumblebee</t>
+  </si>
+  <si>
+    <t>tt4701182</t>
+  </si>
+  <si>
+    <t>Mary Poppins Returns</t>
+  </si>
+  <si>
+    <t>tt5028340</t>
   </si>
 </sst>
 </file>
@@ -4712,10 +4742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C564"/>
+  <dimension ref="A1:C569"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A540" workbookViewId="0">
-      <selection activeCell="C563" sqref="C563:C564"/>
+      <selection activeCell="C564" sqref="C564:C569"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5003,7 +5033,7 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" t="s">
         <v>664</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -5014,7 +5044,7 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" t="s">
         <v>949</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -5322,7 +5352,7 @@
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="4" t="s">
+      <c r="A55" t="s">
         <v>69</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -5366,7 +5396,7 @@
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="4" t="s">
+      <c r="A59" t="s">
         <v>644</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -5377,7 +5407,7 @@
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="4" t="s">
+      <c r="A60" t="s">
         <v>79</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -5520,7 +5550,7 @@
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="4" t="s">
+      <c r="A73" t="s">
         <v>1193</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -6920,7 +6950,7 @@
       <c r="A200" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B200" s="4" t="s">
+      <c r="B200" t="s">
         <v>452</v>
       </c>
       <c r="C200" s="1" t="s">
@@ -7423,7 +7453,7 @@
       <c r="A246" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B246" s="4" t="s">
+      <c r="B246" t="s">
         <v>480</v>
       </c>
       <c r="C246" s="1" t="s">
@@ -9356,7 +9386,7 @@
       <c r="A422" s="1" t="s">
         <v>1013</v>
       </c>
-      <c r="B422" s="4" t="s">
+      <c r="B422" t="s">
         <v>1014</v>
       </c>
       <c r="C422" s="1" t="s">
@@ -9815,7 +9845,7 @@
       </c>
     </row>
     <row r="464" spans="1:3">
-      <c r="A464" s="4" t="s">
+      <c r="A464" t="s">
         <v>1119</v>
       </c>
       <c r="B464" s="1" t="s">
@@ -9991,7 +10021,7 @@
       </c>
     </row>
     <row r="480" spans="1:3">
-      <c r="A480" s="4" t="s">
+      <c r="A480" t="s">
         <v>1159</v>
       </c>
       <c r="B480" s="1" t="s">
@@ -10013,7 +10043,7 @@
       </c>
     </row>
     <row r="482" spans="1:3">
-      <c r="A482" s="4" t="s">
+      <c r="A482" t="s">
         <v>1163</v>
       </c>
       <c r="B482" s="1" t="s">
@@ -10024,7 +10054,7 @@
       </c>
     </row>
     <row r="483" spans="1:3">
-      <c r="A483" s="4" t="s">
+      <c r="A483" t="s">
         <v>1165</v>
       </c>
       <c r="B483" s="1" t="s">
@@ -10035,7 +10065,7 @@
       </c>
     </row>
     <row r="484" spans="1:3">
-      <c r="A484" s="4" t="s">
+      <c r="A484" t="s">
         <v>1167</v>
       </c>
       <c r="B484" s="1" t="s">
@@ -10057,7 +10087,7 @@
       </c>
     </row>
     <row r="486" spans="1:3">
-      <c r="A486" s="4" t="s">
+      <c r="A486" t="s">
         <v>1171</v>
       </c>
       <c r="B486" s="1" t="s">
@@ -10101,7 +10131,7 @@
       </c>
     </row>
     <row r="490" spans="1:3">
-      <c r="A490" s="4" t="s">
+      <c r="A490" t="s">
         <v>1180</v>
       </c>
       <c r="B490" s="1" t="s">
@@ -10134,7 +10164,7 @@
       </c>
     </row>
     <row r="493" spans="1:3">
-      <c r="A493" s="4" t="s">
+      <c r="A493" t="s">
         <v>1185</v>
       </c>
       <c r="B493" s="1" t="s">
@@ -10145,7 +10175,7 @@
       </c>
     </row>
     <row r="494" spans="1:3">
-      <c r="A494" s="4" t="s">
+      <c r="A494" t="s">
         <v>1190</v>
       </c>
       <c r="B494" s="1" t="s">
@@ -10178,13 +10208,13 @@
       </c>
     </row>
     <row r="497" spans="1:3">
-      <c r="A497" s="4" t="s">
+      <c r="A497" t="s">
         <v>1215</v>
       </c>
-      <c r="B497" s="4" t="s">
+      <c r="B497" t="s">
         <v>1212</v>
       </c>
-      <c r="C497" s="4" t="s">
+      <c r="C497" t="s">
         <v>4</v>
       </c>
     </row>
@@ -10211,7 +10241,7 @@
       </c>
     </row>
     <row r="500" spans="1:3">
-      <c r="A500" s="4" t="s">
+      <c r="A500" t="s">
         <v>1223</v>
       </c>
       <c r="B500" s="1" t="s">
@@ -10225,7 +10255,7 @@
       <c r="A501" s="1" t="s">
         <v>1225</v>
       </c>
-      <c r="B501" s="4" t="s">
+      <c r="B501" t="s">
         <v>1224</v>
       </c>
       <c r="C501" s="1" t="s">
@@ -10258,7 +10288,7 @@
       <c r="A504" s="1" t="s">
         <v>1233</v>
       </c>
-      <c r="B504" s="4" t="s">
+      <c r="B504" t="s">
         <v>1232</v>
       </c>
       <c r="C504" s="1" t="s">
@@ -10379,7 +10409,7 @@
       <c r="A515" t="s">
         <v>1268</v>
       </c>
-      <c r="B515" s="4" t="s">
+      <c r="B515" t="s">
         <v>1267</v>
       </c>
       <c r="C515" s="1" t="s">
@@ -10387,7 +10417,7 @@
       </c>
     </row>
     <row r="516" spans="1:3">
-      <c r="A516" s="4" t="s">
+      <c r="A516" t="s">
         <v>1269</v>
       </c>
       <c r="B516" s="1" t="s">
@@ -10398,7 +10428,7 @@
       </c>
     </row>
     <row r="517" spans="1:3">
-      <c r="A517" s="4" t="s">
+      <c r="A517" t="s">
         <v>1271</v>
       </c>
       <c r="B517" s="1" t="s">
@@ -10442,7 +10472,7 @@
       </c>
     </row>
     <row r="521" spans="1:3">
-      <c r="A521" s="4" t="s">
+      <c r="A521" t="s">
         <v>1281</v>
       </c>
       <c r="B521" s="1" t="s">
@@ -10486,7 +10516,7 @@
       </c>
     </row>
     <row r="525" spans="1:3">
-      <c r="A525" s="4" t="s">
+      <c r="A525" t="s">
         <v>1289</v>
       </c>
       <c r="B525" s="1" t="s">
@@ -10922,6 +10952,61 @@
         <v>1408</v>
       </c>
       <c r="C564" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3">
+      <c r="A565" s="1" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C565" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3">
+      <c r="A566" s="1" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B566" s="1" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C566" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="567" spans="1:3">
+      <c r="A567" s="4" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B567" s="1" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C567" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="568" spans="1:3">
+      <c r="A568" s="1" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B568" s="1" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C568" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="569" spans="1:3">
+      <c r="A569" s="1" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B569" s="1" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C569" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -11006,7 +11091,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>757</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -11017,7 +11102,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -11086,7 +11171,7 @@
       <c r="A13" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>126</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -11991,7 +12076,7 @@
       <c r="B95" s="1" t="s">
         <v>1122</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C95" t="s">
         <v>4</v>
       </c>
     </row>
@@ -12007,7 +12092,7 @@
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="4" t="s">
+      <c r="A97" t="s">
         <v>1145</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -12057,7 +12142,7 @@
       <c r="B101" s="1" t="s">
         <v>1203</v>
       </c>
-      <c r="C101" s="4" t="s">
+      <c r="C101" t="s">
         <v>40</v>
       </c>
     </row>
@@ -12073,7 +12158,7 @@
       </c>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="4" t="s">
+      <c r="A103" t="s">
         <v>1204</v>
       </c>
       <c r="B103" s="1" t="s">
@@ -12084,7 +12169,7 @@
       </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="4" t="s">
+      <c r="A104" t="s">
         <v>1206</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -12112,12 +12197,12 @@
       <c r="B106" s="1" t="s">
         <v>1210</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C106" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="4" t="s">
+      <c r="A107" t="s">
         <v>1214</v>
       </c>
       <c r="B107" s="1" t="s">
@@ -12128,7 +12213,7 @@
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="4" t="s">
+      <c r="A108" t="s">
         <v>1217</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -12186,7 +12271,7 @@
       <c r="A113" s="1" t="s">
         <v>1235</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B113" t="s">
         <v>1234</v>
       </c>
       <c r="C113" s="1" t="s">
@@ -12230,7 +12315,7 @@
       <c r="A117" s="1" t="s">
         <v>1247</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B117" t="s">
         <v>1246</v>
       </c>
       <c r="C117" s="1" t="s">
@@ -12271,7 +12356,7 @@
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="4" t="s">
+      <c r="A121" t="s">
         <v>1297</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -12381,7 +12466,7 @@
       </c>
     </row>
     <row r="131" spans="1:3">
-      <c r="A131" s="4" t="s">
+      <c r="A131" t="s">
         <v>1329</v>
       </c>
       <c r="B131" s="1" t="s">
@@ -12403,7 +12488,7 @@
       </c>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="4" t="s">
+      <c r="A133" t="s">
         <v>1337</v>
       </c>
       <c r="B133" s="1" t="s">
@@ -12414,7 +12499,7 @@
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="4" t="s">
+      <c r="A134" t="s">
         <v>1339</v>
       </c>
       <c r="B134" s="1" t="s">
@@ -12447,7 +12532,7 @@
       </c>
     </row>
     <row r="137" spans="1:3">
-      <c r="A137" s="4" t="s">
+      <c r="A137" t="s">
         <v>1345</v>
       </c>
       <c r="B137" s="1" t="s">
@@ -12502,7 +12587,7 @@
       </c>
     </row>
     <row r="142" spans="1:3">
-      <c r="A142" s="4" t="s">
+      <c r="A142" t="s">
         <v>1399</v>
       </c>
       <c r="B142" s="1" t="s">
@@ -12527,37 +12612,37 @@
       <c r="B330" s="3"/>
     </row>
     <row r="562" spans="1:3">
-      <c r="A562" s="4"/>
+      <c r="A562"/>
     </row>
     <row r="563" spans="1:3">
-      <c r="C563" s="4"/>
+      <c r="C563"/>
     </row>
     <row r="575" spans="1:3">
-      <c r="A575" s="4"/>
+      <c r="A575"/>
     </row>
     <row r="582" spans="1:1">
-      <c r="A582" s="4"/>
+      <c r="A582"/>
     </row>
     <row r="584" spans="1:1">
-      <c r="A584" s="4"/>
+      <c r="A584"/>
     </row>
     <row r="585" spans="1:1">
-      <c r="A585" s="4"/>
+      <c r="A585"/>
     </row>
     <row r="586" spans="1:1">
-      <c r="A586" s="4"/>
+      <c r="A586"/>
     </row>
     <row r="588" spans="1:1">
-      <c r="A588" s="4"/>
+      <c r="A588"/>
     </row>
     <row r="592" spans="1:1">
-      <c r="A592" s="4"/>
+      <c r="A592"/>
     </row>
     <row r="595" spans="1:1">
-      <c r="A595" s="4"/>
+      <c r="A595"/>
     </row>
     <row r="597" spans="1:1">
-      <c r="A597" s="4"/>
+      <c r="A597"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>